<commit_message>
Working on perfect sub.
</commit_message>
<xml_diff>
--- a/inst/extdata/PerfectSubstitutionraw/UTEI_Sankey_Simple_ECC_Perfect_Sub.xlsx
+++ b/inst/extdata/PerfectSubstitutionraw/UTEI_Sankey_Simple_ECC_Perfect_Sub.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mkh2/github/Recca/inst/extdata/PerfectSubstitutionraw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC906F64-8320-3F4C-9CB1-DA14A86BD493}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEADC63E-07D2-0D41-A45F-1B27FBC787DD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="17560" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="17560" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Meta" sheetId="10" r:id="rId1"/>
@@ -581,7 +581,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1282" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1282" uniqueCount="194">
   <si>
     <t>Buildings</t>
   </si>
@@ -3175,224 +3175,6 @@
   </si>
   <si>
     <r>
-      <t>B</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>'</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri (Body)"/>
-      </rPr>
-      <t>2</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>B</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>'</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri (Body)"/>
-      </rPr>
-      <t>1</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>y</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>'</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri (Body)"/>
-      </rPr>
-      <t>1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> = </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>B</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>'</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri (Body)"/>
-      </rPr>
-      <t>1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> *  </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>f</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>y</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>'</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri (Body)"/>
-      </rPr>
-      <t>2</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> = </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>B</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>'</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri (Body)"/>
-      </rPr>
-      <t>2</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> *  </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>f</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t>g</t>
     </r>
     <r>
@@ -4622,241 +4404,6 @@
   </si>
   <si>
     <r>
-      <t>B</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>'</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri (Body)"/>
-      </rPr>
-      <t>2</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> *  </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>f_hat</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>B</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>'</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri (Body)"/>
-      </rPr>
-      <t>1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> *  </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>f_hat</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>U</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri (Body)"/>
-      </rPr>
-      <t>'</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri (Body)"/>
-      </rPr>
-      <t>1</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> = Z</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> * </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>g</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>'</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri (Body)"/>
-      </rPr>
-      <t>1</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">_hat </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">+ </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>B</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>'</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri (Body)"/>
-      </rPr>
-      <t>1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> * </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>f_hat</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <rPr>
         <b/>
         <sz val="12"/>
@@ -4959,132 +4506,6 @@
         <scheme val="minor"/>
       </rPr>
       <t>i</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>U</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>'</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri (Body)"/>
-      </rPr>
-      <t>2</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> = Z</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> * </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>g</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>'</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri (Body)"/>
-      </rPr>
-      <t>2</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>_hat + B</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>'</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri (Body)"/>
-      </rPr>
-      <t>2</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> * </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>f_hat</t>
     </r>
   </si>
   <si>
@@ -5945,6 +5366,632 @@
   </si>
   <si>
     <t>Example</t>
+  </si>
+  <si>
+    <r>
+      <t>K</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> = </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>U</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> * </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>f_hat_inv</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>K</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>'</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>y</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>'</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> = </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>K</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>'</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> *  </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>f</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>K</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>'</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> *  </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>f_hat</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>K</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>'</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>2</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>y</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>'</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> = </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>K</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>'</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> *  </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>f</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>K</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>'</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> *  </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>f_hat</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>U</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>'</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> = Z</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> * </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>g</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>'</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>_hat + K</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>'</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> * </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>f_hat</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>U</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>'</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> = Z</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> * </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>g</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>'</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">_hat </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">+ </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>K</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>'</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> * </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>f_hat</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -6809,7 +6856,7 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -6818,28 +6865,28 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -30590,11 +30637,11 @@
     </row>
     <row r="26" spans="1:93">
       <c r="B26" s="10"/>
-      <c r="C26" s="75" t="s">
+      <c r="C26" s="69" t="s">
         <v>30</v>
       </c>
-      <c r="D26" s="75"/>
-      <c r="E26" s="75"/>
+      <c r="D26" s="69"/>
+      <c r="E26" s="69"/>
       <c r="F26" s="39"/>
       <c r="G26" s="39"/>
     </row>
@@ -30863,11 +30910,11 @@
       <c r="CO35" s="31"/>
     </row>
     <row r="36" spans="1:93" ht="18">
-      <c r="C36" s="75" t="s">
+      <c r="C36" s="69" t="s">
         <v>31</v>
       </c>
-      <c r="D36" s="75"/>
-      <c r="E36" s="75"/>
+      <c r="D36" s="69"/>
+      <c r="E36" s="69"/>
       <c r="F36" s="39"/>
       <c r="G36" s="39"/>
       <c r="BM36" s="31"/>
@@ -31085,7 +31132,7 @@
       </c>
       <c r="V41" s="28"/>
       <c r="W41" s="2" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
       <c r="X41" s="2" t="s">
         <v>58</v>
@@ -31193,7 +31240,7 @@
         <v>18</v>
       </c>
       <c r="CJ41" s="2" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
       <c r="CK41" s="2" t="s">
         <v>58</v>
@@ -33001,14 +33048,14 @@
       <c r="AA53" s="15"/>
     </row>
     <row r="54" spans="1:93" ht="20">
-      <c r="L54" s="73" t="s">
+      <c r="L54" s="72" t="s">
         <v>42</v>
       </c>
-      <c r="M54" s="73"/>
-      <c r="N54" s="73"/>
-      <c r="O54" s="73"/>
-      <c r="P54" s="73"/>
-      <c r="Q54" s="73"/>
+      <c r="M54" s="72"/>
+      <c r="N54" s="72"/>
+      <c r="O54" s="72"/>
+      <c r="P54" s="72"/>
+      <c r="Q54" s="72"/>
     </row>
     <row r="55" spans="1:93">
       <c r="L55" s="6">
@@ -33048,11 +33095,11 @@
     </row>
     <row r="60" spans="1:93">
       <c r="B60" s="1"/>
-      <c r="Z60" s="75" t="s">
+      <c r="Z60" s="69" t="s">
         <v>30</v>
       </c>
-      <c r="AA60" s="75"/>
-      <c r="AB60" s="75"/>
+      <c r="AA60" s="69"/>
+      <c r="AB60" s="69"/>
       <c r="AI60" s="68" t="s">
         <v>3</v>
       </c>
@@ -34188,11 +34235,11 @@
       <c r="J68" s="68"/>
       <c r="X68" s="15"/>
       <c r="Y68" s="15"/>
-      <c r="Z68" s="73" t="s">
+      <c r="Z68" s="72" t="s">
         <v>69</v>
       </c>
-      <c r="AA68" s="73"/>
-      <c r="AB68" s="73"/>
+      <c r="AA68" s="72"/>
+      <c r="AB68" s="72"/>
       <c r="AD68" s="34" t="s">
         <v>71</v>
       </c>
@@ -34398,17 +34445,17 @@
       <c r="W73" s="15"/>
       <c r="X73" s="15"/>
       <c r="Y73" s="15"/>
-      <c r="Z73" s="75" t="s">
+      <c r="Z73" s="69" t="s">
         <v>30</v>
       </c>
-      <c r="AA73" s="75"/>
-      <c r="AI73" s="76" t="s">
+      <c r="AA73" s="69"/>
+      <c r="AI73" s="73" t="s">
         <v>52</v>
       </c>
-      <c r="AJ73" s="76"/>
+      <c r="AJ73" s="73"/>
       <c r="AK73" s="31"/>
-      <c r="AL73" s="76"/>
-      <c r="AM73" s="76"/>
+      <c r="AL73" s="73"/>
+      <c r="AM73" s="73"/>
       <c r="AN73" s="31"/>
       <c r="AO73" s="31"/>
       <c r="AP73" s="31"/>
@@ -34732,29 +34779,29 @@
       <c r="AC77" s="41" t="s">
         <v>53</v>
       </c>
-      <c r="AI77" s="72" t="s">
+      <c r="AI77" s="75" t="s">
         <v>64</v>
       </c>
-      <c r="AJ77" s="72"/>
+      <c r="AJ77" s="75"/>
       <c r="AK77" s="29"/>
-      <c r="AL77" s="72"/>
-      <c r="AM77" s="72"/>
+      <c r="AL77" s="75"/>
+      <c r="AM77" s="75"/>
       <c r="AN77" s="29"/>
       <c r="AO77" s="31"/>
       <c r="AP77" s="31"/>
       <c r="AQ77" s="31"/>
       <c r="AR77" s="31"/>
       <c r="AS77" s="31"/>
-      <c r="AT77" s="72" t="s">
+      <c r="AT77" s="75" t="s">
         <v>65</v>
       </c>
-      <c r="AU77" s="72"/>
-      <c r="AV77" s="72"/>
-      <c r="AW77" s="72"/>
-      <c r="AX77" s="72"/>
-      <c r="AY77" s="72"/>
-      <c r="AZ77" s="72"/>
-      <c r="BA77" s="72"/>
+      <c r="AU77" s="75"/>
+      <c r="AV77" s="75"/>
+      <c r="AW77" s="75"/>
+      <c r="AX77" s="75"/>
+      <c r="AY77" s="75"/>
+      <c r="AZ77" s="75"/>
+      <c r="BA77" s="75"/>
     </row>
     <row r="78" spans="1:78">
       <c r="B78" s="1"/>
@@ -34854,16 +34901,16 @@
       </c>
     </row>
     <row r="81" spans="1:93" ht="16" customHeight="1">
-      <c r="C81" s="69" t="s">
+      <c r="C81" s="76" t="s">
         <v>85</v>
       </c>
-      <c r="D81" s="69"/>
-      <c r="E81" s="69"/>
-      <c r="F81" s="69"/>
-      <c r="G81" s="69"/>
-      <c r="H81" s="69"/>
-      <c r="I81" s="69"/>
-      <c r="J81" s="69"/>
+      <c r="D81" s="76"/>
+      <c r="E81" s="76"/>
+      <c r="F81" s="76"/>
+      <c r="G81" s="76"/>
+      <c r="H81" s="76"/>
+      <c r="I81" s="76"/>
+      <c r="J81" s="76"/>
       <c r="AI81" s="68" t="s">
         <v>4</v>
       </c>
@@ -36279,14 +36326,14 @@
       </c>
     </row>
     <row r="91" spans="1:93" ht="19">
-      <c r="L91" s="69" t="s">
+      <c r="L91" s="76" t="s">
         <v>13</v>
       </c>
-      <c r="M91" s="69"/>
-      <c r="N91" s="69"/>
-      <c r="O91" s="69"/>
-      <c r="P91" s="69"/>
-      <c r="Q91" s="69"/>
+      <c r="M91" s="76"/>
+      <c r="N91" s="76"/>
+      <c r="O91" s="76"/>
+      <c r="P91" s="76"/>
+      <c r="Q91" s="76"/>
       <c r="Z91" s="41" t="s">
         <v>11</v>
       </c>
@@ -36439,14 +36486,14 @@
       <c r="AA94" s="17"/>
     </row>
     <row r="95" spans="1:93" ht="20">
-      <c r="L95" s="69" t="s">
+      <c r="L95" s="76" t="s">
         <v>35</v>
       </c>
-      <c r="M95" s="69"/>
-      <c r="N95" s="69"/>
-      <c r="O95" s="69"/>
-      <c r="P95" s="69"/>
-      <c r="Q95" s="69"/>
+      <c r="M95" s="76"/>
+      <c r="N95" s="76"/>
+      <c r="O95" s="76"/>
+      <c r="P95" s="76"/>
+      <c r="Q95" s="76"/>
     </row>
     <row r="98" spans="1:40" ht="47">
       <c r="A98" s="27" t="s">
@@ -37067,16 +37114,16 @@
       </c>
       <c r="D120" s="68"/>
       <c r="E120" s="68"/>
-      <c r="G120" s="69" t="s">
+      <c r="G120" s="76" t="s">
         <v>39</v>
       </c>
-      <c r="H120" s="69"/>
-      <c r="I120" s="69"/>
-      <c r="K120" s="69" t="s">
+      <c r="H120" s="76"/>
+      <c r="I120" s="76"/>
+      <c r="K120" s="76" t="s">
         <v>40</v>
       </c>
-      <c r="L120" s="69"/>
-      <c r="M120" s="69"/>
+      <c r="L120" s="76"/>
+      <c r="M120" s="76"/>
       <c r="N120" s="17"/>
       <c r="O120" s="17" t="s">
         <v>41</v>
@@ -37500,6 +37547,65 @@
     </row>
   </sheetData>
   <mergeCells count="71">
+    <mergeCell ref="A112:I112"/>
+    <mergeCell ref="C143:H143"/>
+    <mergeCell ref="C120:E120"/>
+    <mergeCell ref="G120:I120"/>
+    <mergeCell ref="K120:M120"/>
+    <mergeCell ref="A125:A130"/>
+    <mergeCell ref="C135:H135"/>
+    <mergeCell ref="A137:A142"/>
+    <mergeCell ref="A114:A119"/>
+    <mergeCell ref="BE81:BL81"/>
+    <mergeCell ref="BT81:BY81"/>
+    <mergeCell ref="A83:A90"/>
+    <mergeCell ref="L91:Q91"/>
+    <mergeCell ref="AI91:AP91"/>
+    <mergeCell ref="AT91:BA91"/>
+    <mergeCell ref="BE91:BL91"/>
+    <mergeCell ref="BT91:BY91"/>
+    <mergeCell ref="C81:J81"/>
+    <mergeCell ref="AI81:AP81"/>
+    <mergeCell ref="AT81:BA81"/>
+    <mergeCell ref="J92:J94"/>
+    <mergeCell ref="L95:Q95"/>
+    <mergeCell ref="A100:I100"/>
+    <mergeCell ref="A102:A109"/>
+    <mergeCell ref="C77:J77"/>
+    <mergeCell ref="AI77:AJ77"/>
+    <mergeCell ref="AL77:AM77"/>
+    <mergeCell ref="AT77:BA77"/>
+    <mergeCell ref="C79:J79"/>
+    <mergeCell ref="A75:A76"/>
+    <mergeCell ref="C68:J68"/>
+    <mergeCell ref="Z68:AB68"/>
+    <mergeCell ref="AI68:AN68"/>
+    <mergeCell ref="AT68:BA68"/>
+    <mergeCell ref="C70:J70"/>
+    <mergeCell ref="Z73:AA73"/>
+    <mergeCell ref="AI73:AJ73"/>
+    <mergeCell ref="AL73:AM73"/>
+    <mergeCell ref="AT73:BA73"/>
+    <mergeCell ref="BE68:BL68"/>
+    <mergeCell ref="BT68:BY68"/>
+    <mergeCell ref="Z60:AB60"/>
+    <mergeCell ref="AI60:AN60"/>
+    <mergeCell ref="AT60:BA60"/>
+    <mergeCell ref="BE60:BL60"/>
+    <mergeCell ref="BT60:BY60"/>
+    <mergeCell ref="A62:A67"/>
+    <mergeCell ref="BE50:BJ50"/>
+    <mergeCell ref="BT50:BY50"/>
+    <mergeCell ref="CA50:CH50"/>
+    <mergeCell ref="J51:J53"/>
+    <mergeCell ref="L54:Q54"/>
+    <mergeCell ref="L56:Q56"/>
+    <mergeCell ref="AT50:AY50"/>
+    <mergeCell ref="A42:A49"/>
+    <mergeCell ref="U42:U49"/>
+    <mergeCell ref="L50:Q50"/>
+    <mergeCell ref="W50:X50"/>
+    <mergeCell ref="AI50:AP50"/>
     <mergeCell ref="CJ40:CK40"/>
     <mergeCell ref="C26:E26"/>
     <mergeCell ref="A28:A35"/>
@@ -37512,65 +37618,6 @@
     <mergeCell ref="BE40:BJ40"/>
     <mergeCell ref="BT40:BY40"/>
     <mergeCell ref="CA40:CH40"/>
-    <mergeCell ref="A42:A49"/>
-    <mergeCell ref="U42:U49"/>
-    <mergeCell ref="L50:Q50"/>
-    <mergeCell ref="W50:X50"/>
-    <mergeCell ref="AI50:AP50"/>
-    <mergeCell ref="A62:A67"/>
-    <mergeCell ref="BE50:BJ50"/>
-    <mergeCell ref="BT50:BY50"/>
-    <mergeCell ref="CA50:CH50"/>
-    <mergeCell ref="J51:J53"/>
-    <mergeCell ref="L54:Q54"/>
-    <mergeCell ref="L56:Q56"/>
-    <mergeCell ref="AT50:AY50"/>
-    <mergeCell ref="BT68:BY68"/>
-    <mergeCell ref="Z60:AB60"/>
-    <mergeCell ref="AI60:AN60"/>
-    <mergeCell ref="AT60:BA60"/>
-    <mergeCell ref="BE60:BL60"/>
-    <mergeCell ref="BT60:BY60"/>
-    <mergeCell ref="Z73:AA73"/>
-    <mergeCell ref="AI73:AJ73"/>
-    <mergeCell ref="AL73:AM73"/>
-    <mergeCell ref="AT73:BA73"/>
-    <mergeCell ref="BE68:BL68"/>
-    <mergeCell ref="C68:J68"/>
-    <mergeCell ref="Z68:AB68"/>
-    <mergeCell ref="AI68:AN68"/>
-    <mergeCell ref="AT68:BA68"/>
-    <mergeCell ref="C70:J70"/>
-    <mergeCell ref="AI77:AJ77"/>
-    <mergeCell ref="AL77:AM77"/>
-    <mergeCell ref="AT77:BA77"/>
-    <mergeCell ref="C79:J79"/>
-    <mergeCell ref="A75:A76"/>
-    <mergeCell ref="J92:J94"/>
-    <mergeCell ref="L95:Q95"/>
-    <mergeCell ref="A100:I100"/>
-    <mergeCell ref="A102:A109"/>
-    <mergeCell ref="C77:J77"/>
-    <mergeCell ref="BE81:BL81"/>
-    <mergeCell ref="BT81:BY81"/>
-    <mergeCell ref="A83:A90"/>
-    <mergeCell ref="L91:Q91"/>
-    <mergeCell ref="AI91:AP91"/>
-    <mergeCell ref="AT91:BA91"/>
-    <mergeCell ref="BE91:BL91"/>
-    <mergeCell ref="BT91:BY91"/>
-    <mergeCell ref="C81:J81"/>
-    <mergeCell ref="AI81:AP81"/>
-    <mergeCell ref="AT81:BA81"/>
-    <mergeCell ref="A112:I112"/>
-    <mergeCell ref="C143:H143"/>
-    <mergeCell ref="C120:E120"/>
-    <mergeCell ref="G120:I120"/>
-    <mergeCell ref="K120:M120"/>
-    <mergeCell ref="A125:A130"/>
-    <mergeCell ref="C135:H135"/>
-    <mergeCell ref="A137:A142"/>
-    <mergeCell ref="A114:A119"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -37583,8 +37630,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{842438A8-D71C-B444-A99F-665ABEA366D5}">
   <dimension ref="A1:LO126"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="CI41" sqref="CI41"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="2" topLeftCell="C42" activePane="bottomRight" state="frozen"/>
+      <selection activeCell="A40" sqref="A40"/>
+      <selection pane="topRight" activeCell="C40" sqref="C40"/>
+      <selection pane="bottomLeft" activeCell="A42" sqref="A42"/>
+      <selection pane="bottomRight" activeCell="EI55" sqref="EI55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -37603,7 +37654,7 @@
   <sheetData>
     <row r="1" spans="6:276">
       <c r="AI1" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
     </row>
     <row r="2" spans="6:276">
@@ -37611,7 +37662,7 @@
         <v>3</v>
       </c>
       <c r="AI2" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="CW2" s="33">
         <f ca="1">EE44</f>
@@ -38158,46 +38209,46 @@
         <v>106</v>
       </c>
       <c r="IU23" s="61" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="24" spans="1:278">
       <c r="W24" s="21"/>
       <c r="CQ24" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="FS24" t="s">
         <v>108</v>
       </c>
       <c r="IU24" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
     </row>
     <row r="25" spans="1:278">
       <c r="CQ25" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="FS25" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="IU25" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
     </row>
     <row r="26" spans="1:278">
       <c r="B26" s="10"/>
-      <c r="C26" s="75" t="s">
+      <c r="C26" s="69" t="s">
         <v>30</v>
       </c>
-      <c r="D26" s="75"/>
-      <c r="E26" s="75"/>
+      <c r="D26" s="69"/>
+      <c r="E26" s="69"/>
       <c r="F26" s="47"/>
       <c r="G26" s="47"/>
       <c r="CQ26" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="FS26" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
     </row>
     <row r="27" spans="1:278" ht="35" customHeight="1">
@@ -38449,11 +38500,11 @@
       <c r="CJ35" s="31"/>
     </row>
     <row r="36" spans="1:302" ht="18">
-      <c r="C36" s="75" t="s">
+      <c r="C36" s="69" t="s">
         <v>31</v>
       </c>
-      <c r="D36" s="75"/>
-      <c r="E36" s="75"/>
+      <c r="D36" s="69"/>
+      <c r="E36" s="69"/>
       <c r="F36" s="47"/>
       <c r="G36" s="47"/>
       <c r="BL36" s="31"/>
@@ -38508,31 +38559,31 @@
       <c r="CJ37" s="51"/>
     </row>
     <row r="38" spans="1:302">
-      <c r="BL38" s="72"/>
-      <c r="BM38" s="72"/>
-      <c r="BN38" s="72"/>
-      <c r="BO38" s="72"/>
-      <c r="BP38" s="72"/>
-      <c r="BQ38" s="72"/>
-      <c r="BR38" s="72"/>
-      <c r="BS38" s="72"/>
-      <c r="BT38" s="72"/>
-      <c r="BU38" s="72"/>
-      <c r="BV38" s="72"/>
-      <c r="BW38" s="72"/>
-      <c r="BX38" s="72"/>
-      <c r="BY38" s="72"/>
-      <c r="BZ38" s="72"/>
-      <c r="CA38" s="72"/>
-      <c r="CB38" s="72"/>
-      <c r="CC38" s="72"/>
-      <c r="CD38" s="72"/>
-      <c r="CE38" s="72"/>
-      <c r="CF38" s="72"/>
-      <c r="CG38" s="72"/>
-      <c r="CH38" s="72"/>
-      <c r="CI38" s="72"/>
-      <c r="CJ38" s="72"/>
+      <c r="BL38" s="75"/>
+      <c r="BM38" s="75"/>
+      <c r="BN38" s="75"/>
+      <c r="BO38" s="75"/>
+      <c r="BP38" s="75"/>
+      <c r="BQ38" s="75"/>
+      <c r="BR38" s="75"/>
+      <c r="BS38" s="75"/>
+      <c r="BT38" s="75"/>
+      <c r="BU38" s="75"/>
+      <c r="BV38" s="75"/>
+      <c r="BW38" s="75"/>
+      <c r="BX38" s="75"/>
+      <c r="BY38" s="75"/>
+      <c r="BZ38" s="75"/>
+      <c r="CA38" s="75"/>
+      <c r="CB38" s="75"/>
+      <c r="CC38" s="75"/>
+      <c r="CD38" s="75"/>
+      <c r="CE38" s="75"/>
+      <c r="CF38" s="75"/>
+      <c r="CG38" s="75"/>
+      <c r="CH38" s="75"/>
+      <c r="CI38" s="75"/>
+      <c r="CJ38" s="75"/>
     </row>
     <row r="40" spans="1:302">
       <c r="C40" s="68" t="s">
@@ -38678,8 +38729,8 @@
       <c r="JC40" s="68"/>
       <c r="JD40" s="68"/>
       <c r="JE40" s="68"/>
-      <c r="JL40" s="72"/>
-      <c r="JM40" s="72"/>
+      <c r="JL40" s="75"/>
+      <c r="JM40" s="75"/>
       <c r="KI40" s="68" t="s">
         <v>3</v>
       </c>
@@ -38734,7 +38785,7 @@
       </c>
       <c r="V41" s="28"/>
       <c r="W41" s="2" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
       <c r="X41" s="2" t="s">
         <v>58</v>
@@ -38842,7 +38893,7 @@
         <v>18</v>
       </c>
       <c r="CI41" s="2" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
       <c r="CJ41" s="2" t="s">
         <v>58</v>
@@ -38851,7 +38902,7 @@
       <c r="CL41" s="2"/>
       <c r="CR41" s="28"/>
       <c r="CS41" s="2" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
       <c r="CT41" s="2" t="s">
         <v>58</v>
@@ -38912,7 +38963,7 @@
       </c>
       <c r="FT41" s="28"/>
       <c r="FU41" s="2" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
       <c r="FV41" s="2" t="s">
         <v>58</v>
@@ -42307,7 +42358,7 @@
       <c r="BH50" s="68"/>
       <c r="BI50" s="68"/>
       <c r="BS50" s="71" t="s">
-        <v>104</v>
+        <v>185</v>
       </c>
       <c r="BT50" s="71"/>
       <c r="BU50" s="71"/>
@@ -42339,7 +42390,7 @@
       </c>
       <c r="CT50" s="68"/>
       <c r="CV50" s="71" t="s">
-        <v>121</v>
+        <v>186</v>
       </c>
       <c r="CW50" s="71"/>
       <c r="CX50" s="71"/>
@@ -42347,11 +42398,11 @@
       <c r="CZ50" s="71"/>
       <c r="DA50" s="71"/>
       <c r="DC50" s="52" t="s">
-        <v>122</v>
+        <v>187</v>
       </c>
       <c r="DF50" s="31"/>
       <c r="DH50" s="68" t="s">
-        <v>142</v>
+        <v>188</v>
       </c>
       <c r="DI50" s="68"/>
       <c r="DJ50" s="68"/>
@@ -42363,14 +42414,14 @@
       <c r="EB50" s="58"/>
       <c r="EC50" s="58"/>
       <c r="ED50" s="58"/>
-      <c r="EE50" s="79" t="s">
-        <v>143</v>
-      </c>
-      <c r="EF50" s="79"/>
-      <c r="EG50" s="79"/>
-      <c r="EH50" s="79"/>
-      <c r="EI50" s="79"/>
-      <c r="EJ50" s="79"/>
+      <c r="EE50" s="78" t="s">
+        <v>193</v>
+      </c>
+      <c r="EF50" s="78"/>
+      <c r="EG50" s="78"/>
+      <c r="EH50" s="78"/>
+      <c r="EI50" s="78"/>
+      <c r="EJ50" s="78"/>
       <c r="EK50" s="58"/>
       <c r="EL50" s="58"/>
       <c r="EM50" s="58"/>
@@ -42387,7 +42438,7 @@
       </c>
       <c r="FV50" s="68"/>
       <c r="FX50" s="71" t="s">
-        <v>120</v>
+        <v>189</v>
       </c>
       <c r="FY50" s="71"/>
       <c r="FZ50" s="71"/>
@@ -42395,12 +42446,12 @@
       <c r="GB50" s="71"/>
       <c r="GC50" s="71"/>
       <c r="GE50" s="52" t="s">
-        <v>123</v>
+        <v>190</v>
       </c>
       <c r="GH50" s="29"/>
       <c r="GI50" s="29"/>
       <c r="GJ50" s="68" t="s">
-        <v>141</v>
+        <v>191</v>
       </c>
       <c r="GK50" s="68"/>
       <c r="GL50" s="68"/>
@@ -42412,14 +42463,14 @@
       <c r="HD50" s="58"/>
       <c r="HE50" s="58"/>
       <c r="HF50" s="58"/>
-      <c r="HG50" s="79" t="s">
-        <v>146</v>
-      </c>
-      <c r="HH50" s="79"/>
-      <c r="HI50" s="79"/>
-      <c r="HJ50" s="79"/>
-      <c r="HK50" s="79"/>
-      <c r="HL50" s="79"/>
+      <c r="HG50" s="78" t="s">
+        <v>192</v>
+      </c>
+      <c r="HH50" s="78"/>
+      <c r="HI50" s="78"/>
+      <c r="HJ50" s="78"/>
+      <c r="HK50" s="78"/>
+      <c r="HL50" s="78"/>
       <c r="HM50" s="58"/>
       <c r="HN50" s="58"/>
       <c r="HO50" s="58"/>
@@ -42432,15 +42483,15 @@
       <c r="IS50" s="8"/>
       <c r="IT50" s="8"/>
       <c r="IV50" s="31"/>
-      <c r="IW50" s="72"/>
-      <c r="IX50" s="72"/>
+      <c r="IW50" s="75"/>
+      <c r="IX50" s="75"/>
       <c r="IY50" s="31"/>
-      <c r="IZ50" s="79"/>
-      <c r="JA50" s="79"/>
-      <c r="JB50" s="79"/>
-      <c r="JC50" s="79"/>
-      <c r="JD50" s="79"/>
-      <c r="JE50" s="79"/>
+      <c r="IZ50" s="78"/>
+      <c r="JA50" s="78"/>
+      <c r="JB50" s="78"/>
+      <c r="JC50" s="78"/>
+      <c r="JD50" s="78"/>
+      <c r="JE50" s="78"/>
       <c r="JF50" s="31"/>
       <c r="JG50" s="55"/>
       <c r="JH50" s="31"/>
@@ -42454,14 +42505,14 @@
       <c r="KF50" s="58"/>
       <c r="KG50" s="58"/>
       <c r="KH50" s="58"/>
-      <c r="KI50" s="79" t="s">
-        <v>137</v>
-      </c>
-      <c r="KJ50" s="79"/>
-      <c r="KK50" s="79"/>
-      <c r="KL50" s="79"/>
-      <c r="KM50" s="79"/>
-      <c r="KN50" s="79"/>
+      <c r="KI50" s="78" t="s">
+        <v>133</v>
+      </c>
+      <c r="KJ50" s="78"/>
+      <c r="KK50" s="78"/>
+      <c r="KL50" s="78"/>
+      <c r="KM50" s="78"/>
+      <c r="KN50" s="78"/>
       <c r="KO50" s="58"/>
       <c r="KP50" s="59" t="s">
         <v>12</v>
@@ -42776,14 +42827,14 @@
     </row>
     <row r="54" spans="1:319" ht="20">
       <c r="B54" s="1"/>
-      <c r="L54" s="73" t="s">
+      <c r="L54" s="72" t="s">
         <v>42</v>
       </c>
-      <c r="M54" s="73"/>
-      <c r="N54" s="73"/>
-      <c r="O54" s="73"/>
-      <c r="P54" s="73"/>
-      <c r="Q54" s="73"/>
+      <c r="M54" s="72"/>
+      <c r="N54" s="72"/>
+      <c r="O54" s="72"/>
+      <c r="P54" s="72"/>
+      <c r="Q54" s="72"/>
       <c r="R54" s="15"/>
       <c r="S54" s="15"/>
       <c r="T54" s="15"/>
@@ -42811,14 +42862,14 @@
       <c r="JJ54" s="31"/>
       <c r="JK54" s="31"/>
       <c r="JL54" s="31"/>
-      <c r="KI54" s="73" t="s">
-        <v>156</v>
-      </c>
-      <c r="KJ54" s="73"/>
-      <c r="KK54" s="73"/>
-      <c r="KL54" s="73"/>
-      <c r="KM54" s="73"/>
-      <c r="KN54" s="73"/>
+      <c r="KI54" s="72" t="s">
+        <v>148</v>
+      </c>
+      <c r="KJ54" s="72"/>
+      <c r="KK54" s="72"/>
+      <c r="KL54" s="72"/>
+      <c r="KM54" s="72"/>
+      <c r="KN54" s="72"/>
     </row>
     <row r="55" spans="1:319">
       <c r="B55" s="1"/>
@@ -42919,7 +42970,7 @@
       <c r="Z56" s="15"/>
       <c r="AA56" s="15"/>
       <c r="KI56" s="68" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="KJ56" s="68"/>
       <c r="KK56" s="68"/>
@@ -42962,18 +43013,18 @@
       <c r="W58" s="15"/>
       <c r="X58" s="15"/>
       <c r="Y58" s="15"/>
-      <c r="Z58" s="75" t="s">
+      <c r="Z58" s="69" t="s">
         <v>30</v>
       </c>
-      <c r="AA58" s="75"/>
-      <c r="AB58" s="75"/>
-      <c r="AH58" s="76" t="s">
+      <c r="AA58" s="69"/>
+      <c r="AB58" s="69"/>
+      <c r="AH58" s="73" t="s">
         <v>52</v>
       </c>
-      <c r="AI58" s="76"/>
+      <c r="AI58" s="73"/>
       <c r="AJ58" s="31"/>
-      <c r="AK58" s="76"/>
-      <c r="AL58" s="76"/>
+      <c r="AK58" s="73"/>
+      <c r="AL58" s="73"/>
       <c r="AM58" s="31"/>
       <c r="AN58" s="31"/>
       <c r="AO58" s="31"/>
@@ -43299,37 +43350,37 @@
       <c r="W62" s="15"/>
       <c r="X62" s="15"/>
       <c r="Y62" s="15"/>
-      <c r="Z62" s="72" t="s">
+      <c r="Z62" s="75" t="s">
         <v>95</v>
       </c>
-      <c r="AA62" s="72"/>
-      <c r="AB62" s="72"/>
+      <c r="AA62" s="75"/>
+      <c r="AB62" s="75"/>
       <c r="AD62" s="45" t="s">
         <v>53</v>
       </c>
-      <c r="AH62" s="72" t="s">
+      <c r="AH62" s="75" t="s">
         <v>64</v>
       </c>
-      <c r="AI62" s="72"/>
+      <c r="AI62" s="75"/>
       <c r="AJ62" s="29"/>
-      <c r="AK62" s="72"/>
-      <c r="AL62" s="72"/>
+      <c r="AK62" s="75"/>
+      <c r="AL62" s="75"/>
       <c r="AM62" s="29"/>
       <c r="AN62" s="31"/>
       <c r="AO62" s="31"/>
       <c r="AP62" s="31"/>
       <c r="AQ62" s="31"/>
       <c r="AR62" s="31"/>
-      <c r="AS62" s="72" t="s">
+      <c r="AS62" s="75" t="s">
         <v>65</v>
       </c>
-      <c r="AT62" s="72"/>
-      <c r="AU62" s="72"/>
-      <c r="AV62" s="72"/>
-      <c r="AW62" s="72"/>
-      <c r="AX62" s="72"/>
-      <c r="AY62" s="72"/>
-      <c r="AZ62" s="72"/>
+      <c r="AT62" s="75"/>
+      <c r="AU62" s="75"/>
+      <c r="AV62" s="75"/>
+      <c r="AW62" s="75"/>
+      <c r="AX62" s="75"/>
+      <c r="AY62" s="75"/>
+      <c r="AZ62" s="75"/>
       <c r="ES62" s="31"/>
       <c r="ET62" s="31"/>
       <c r="EU62" s="31"/>
@@ -43472,11 +43523,11 @@
       <c r="H64" s="68"/>
       <c r="I64" s="68"/>
       <c r="J64" s="68"/>
-      <c r="Z64" s="75" t="s">
+      <c r="Z64" s="69" t="s">
         <v>30</v>
       </c>
-      <c r="AA64" s="75"/>
-      <c r="AB64" s="75"/>
+      <c r="AA64" s="69"/>
+      <c r="AB64" s="69"/>
       <c r="AH64" s="68" t="s">
         <v>3</v>
       </c>
@@ -43535,14 +43586,14 @@
       <c r="EC64" s="45"/>
       <c r="ES64" s="31"/>
       <c r="ET64" s="31"/>
-      <c r="EU64" s="72"/>
-      <c r="EV64" s="72"/>
-      <c r="EW64" s="72"/>
-      <c r="EX64" s="72"/>
-      <c r="EY64" s="72"/>
-      <c r="EZ64" s="72"/>
-      <c r="FA64" s="72"/>
-      <c r="FB64" s="72"/>
+      <c r="EU64" s="75"/>
+      <c r="EV64" s="75"/>
+      <c r="EW64" s="75"/>
+      <c r="EX64" s="75"/>
+      <c r="EY64" s="75"/>
+      <c r="EZ64" s="75"/>
+      <c r="FA64" s="75"/>
+      <c r="FB64" s="75"/>
       <c r="FC64" s="31"/>
       <c r="GM64" s="68" t="s">
         <v>3</v>
@@ -43566,26 +43617,26 @@
       <c r="HE64" s="52"/>
       <c r="HU64" s="31"/>
       <c r="HV64" s="31"/>
-      <c r="HW64" s="72"/>
-      <c r="HX64" s="72"/>
-      <c r="HY64" s="72"/>
-      <c r="HZ64" s="72"/>
-      <c r="IA64" s="72"/>
-      <c r="IB64" s="72"/>
-      <c r="IC64" s="72"/>
-      <c r="ID64" s="72"/>
+      <c r="HW64" s="75"/>
+      <c r="HX64" s="75"/>
+      <c r="HY64" s="75"/>
+      <c r="HZ64" s="75"/>
+      <c r="IA64" s="75"/>
+      <c r="IB64" s="75"/>
+      <c r="IC64" s="75"/>
+      <c r="ID64" s="75"/>
       <c r="IE64" s="31"/>
       <c r="JJ64" s="31"/>
       <c r="JK64" s="31"/>
       <c r="JL64" s="31"/>
       <c r="JM64" s="31"/>
       <c r="JN64" s="31"/>
-      <c r="JO64" s="72"/>
-      <c r="JP64" s="72"/>
-      <c r="JQ64" s="72"/>
-      <c r="JR64" s="72"/>
-      <c r="JS64" s="72"/>
-      <c r="JT64" s="72"/>
+      <c r="JO64" s="75"/>
+      <c r="JP64" s="75"/>
+      <c r="JQ64" s="75"/>
+      <c r="JR64" s="75"/>
+      <c r="JS64" s="75"/>
+      <c r="JT64" s="75"/>
       <c r="JU64" s="31"/>
       <c r="JX64" s="68" t="s">
         <v>4</v>
@@ -43599,21 +43650,21 @@
       <c r="KE64" s="68"/>
       <c r="KF64" s="52"/>
       <c r="KG64" s="52"/>
-      <c r="KP64" s="75" t="s">
+      <c r="KP64" s="69" t="s">
         <v>30</v>
       </c>
-      <c r="KQ64" s="75"/>
-      <c r="KR64" s="75"/>
+      <c r="KQ64" s="69"/>
+      <c r="KR64" s="69"/>
       <c r="KW64" s="31"/>
       <c r="KX64" s="31"/>
-      <c r="KY64" s="72"/>
-      <c r="KZ64" s="72"/>
-      <c r="LA64" s="72"/>
-      <c r="LB64" s="72"/>
-      <c r="LC64" s="72"/>
-      <c r="LD64" s="72"/>
-      <c r="LE64" s="72"/>
-      <c r="LF64" s="72"/>
+      <c r="KY64" s="75"/>
+      <c r="KZ64" s="75"/>
+      <c r="LA64" s="75"/>
+      <c r="LB64" s="75"/>
+      <c r="LC64" s="75"/>
+      <c r="LD64" s="75"/>
+      <c r="LE64" s="75"/>
+      <c r="LF64" s="75"/>
       <c r="LG64" s="31"/>
     </row>
     <row r="65" spans="1:327" ht="51" customHeight="1">
@@ -44517,14 +44568,14 @@
       <c r="EC67" s="50"/>
       <c r="ES67" s="31"/>
       <c r="ET67" s="31"/>
-      <c r="EU67" s="73"/>
-      <c r="EV67" s="73"/>
-      <c r="EW67" s="73"/>
-      <c r="EX67" s="73"/>
-      <c r="EY67" s="73"/>
-      <c r="EZ67" s="73"/>
-      <c r="FA67" s="73"/>
-      <c r="FB67" s="73"/>
+      <c r="EU67" s="72"/>
+      <c r="EV67" s="72"/>
+      <c r="EW67" s="72"/>
+      <c r="EX67" s="72"/>
+      <c r="EY67" s="72"/>
+      <c r="EZ67" s="72"/>
+      <c r="FA67" s="72"/>
+      <c r="FB67" s="72"/>
       <c r="FC67" s="31"/>
       <c r="GH67" s="70"/>
       <c r="GI67" s="1" t="s">
@@ -44594,14 +44645,14 @@
       <c r="HE67" s="51"/>
       <c r="HU67" s="31"/>
       <c r="HV67" s="31"/>
-      <c r="HW67" s="73"/>
-      <c r="HX67" s="73"/>
-      <c r="HY67" s="73"/>
-      <c r="HZ67" s="73"/>
-      <c r="IA67" s="73"/>
-      <c r="IB67" s="73"/>
-      <c r="IC67" s="73"/>
-      <c r="ID67" s="73"/>
+      <c r="HW67" s="72"/>
+      <c r="HX67" s="72"/>
+      <c r="HY67" s="72"/>
+      <c r="HZ67" s="72"/>
+      <c r="IA67" s="72"/>
+      <c r="IB67" s="72"/>
+      <c r="IC67" s="72"/>
+      <c r="ID67" s="72"/>
       <c r="IE67" s="31"/>
       <c r="JJ67" s="77"/>
       <c r="JK67" s="63"/>
@@ -44671,14 +44722,14 @@
       </c>
       <c r="KW67" s="31"/>
       <c r="KX67" s="31"/>
-      <c r="KY67" s="73"/>
-      <c r="KZ67" s="73"/>
-      <c r="LA67" s="73"/>
-      <c r="LB67" s="73"/>
-      <c r="LC67" s="73"/>
-      <c r="LD67" s="73"/>
-      <c r="LE67" s="73"/>
-      <c r="LF67" s="73"/>
+      <c r="KY67" s="72"/>
+      <c r="KZ67" s="72"/>
+      <c r="LA67" s="72"/>
+      <c r="LB67" s="72"/>
+      <c r="LC67" s="72"/>
+      <c r="LD67" s="72"/>
+      <c r="LE67" s="72"/>
+      <c r="LF67" s="72"/>
       <c r="LG67" s="31"/>
     </row>
     <row r="68" spans="1:327">
@@ -46275,11 +46326,11 @@
       <c r="J72" s="68"/>
       <c r="X72" s="15"/>
       <c r="Y72" s="15"/>
-      <c r="Z72" s="73" t="s">
+      <c r="Z72" s="72" t="s">
         <v>96</v>
       </c>
-      <c r="AA72" s="73"/>
-      <c r="AB72" s="73"/>
+      <c r="AA72" s="72"/>
+      <c r="AB72" s="72"/>
       <c r="AD72" s="45" t="s">
         <v>34</v>
       </c>
@@ -46423,10 +46474,10 @@
       <c r="GF72" s="26"/>
       <c r="GG72" s="26"/>
       <c r="GJ72" s="52" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="GM72" s="68" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="GN72" s="68"/>
       <c r="GO72" s="68"/>
@@ -46434,7 +46485,7 @@
       <c r="GQ72" s="68"/>
       <c r="GR72" s="68"/>
       <c r="GV72" s="71" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="GW72" s="71"/>
       <c r="GX72" s="71"/>
@@ -46494,23 +46545,23 @@
       <c r="JL72" s="55"/>
       <c r="JM72" s="31"/>
       <c r="JN72" s="31"/>
-      <c r="JO72" s="72"/>
-      <c r="JP72" s="72"/>
-      <c r="JQ72" s="72"/>
-      <c r="JR72" s="72"/>
-      <c r="JS72" s="72"/>
-      <c r="JT72" s="72"/>
+      <c r="JO72" s="75"/>
+      <c r="JP72" s="75"/>
+      <c r="JQ72" s="75"/>
+      <c r="JR72" s="75"/>
+      <c r="JS72" s="75"/>
+      <c r="JT72" s="75"/>
       <c r="JU72" s="31"/>
-      <c r="JX72" s="78" t="s">
-        <v>138</v>
-      </c>
-      <c r="JY72" s="78"/>
-      <c r="JZ72" s="78"/>
-      <c r="KA72" s="78"/>
-      <c r="KB72" s="78"/>
-      <c r="KC72" s="78"/>
-      <c r="KD72" s="78"/>
-      <c r="KE72" s="78"/>
+      <c r="JX72" s="79" t="s">
+        <v>134</v>
+      </c>
+      <c r="JY72" s="79"/>
+      <c r="JZ72" s="79"/>
+      <c r="KA72" s="79"/>
+      <c r="KB72" s="79"/>
+      <c r="KC72" s="79"/>
+      <c r="KD72" s="79"/>
+      <c r="KE72" s="79"/>
       <c r="KF72" s="54"/>
       <c r="KG72" s="54"/>
       <c r="KH72" s="26"/>
@@ -46521,14 +46572,14 @@
       <c r="KM72" s="26"/>
       <c r="KN72" s="26"/>
       <c r="KO72" s="26"/>
-      <c r="KP72" s="73" t="s">
-        <v>150</v>
-      </c>
-      <c r="KQ72" s="73"/>
-      <c r="KR72" s="73"/>
+      <c r="KP72" s="72" t="s">
+        <v>142</v>
+      </c>
+      <c r="KQ72" s="72"/>
+      <c r="KR72" s="72"/>
       <c r="KS72" s="26"/>
       <c r="KT72" s="52" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="KU72" s="26"/>
       <c r="KW72" s="31"/>
@@ -48619,16 +48670,16 @@
       <c r="FA80" s="29"/>
       <c r="FB80" s="29"/>
       <c r="FC80" s="31"/>
-      <c r="FD80" s="69" t="s">
+      <c r="FD80" s="76" t="s">
         <v>119</v>
       </c>
-      <c r="FE80" s="69"/>
-      <c r="FF80" s="69"/>
-      <c r="FG80" s="69"/>
-      <c r="FH80" s="69"/>
-      <c r="FI80" s="69"/>
-      <c r="FJ80" s="69"/>
-      <c r="FK80" s="69"/>
+      <c r="FE80" s="76"/>
+      <c r="FF80" s="76"/>
+      <c r="FG80" s="76"/>
+      <c r="FH80" s="76"/>
+      <c r="FI80" s="76"/>
+      <c r="FJ80" s="76"/>
+      <c r="FK80" s="76"/>
       <c r="GH80" s="70"/>
       <c r="GI80" s="1" t="s">
         <v>27</v>
@@ -48740,16 +48791,16 @@
       <c r="IC80" s="29"/>
       <c r="ID80" s="29"/>
       <c r="IE80" s="31"/>
-      <c r="IF80" s="69" t="s">
-        <v>134</v>
-      </c>
-      <c r="IG80" s="69"/>
-      <c r="IH80" s="69"/>
-      <c r="II80" s="69"/>
-      <c r="IJ80" s="69"/>
-      <c r="IK80" s="69"/>
-      <c r="IL80" s="69"/>
-      <c r="IM80" s="69"/>
+      <c r="IF80" s="76" t="s">
+        <v>130</v>
+      </c>
+      <c r="IG80" s="76"/>
+      <c r="IH80" s="76"/>
+      <c r="II80" s="76"/>
+      <c r="IJ80" s="76"/>
+      <c r="IK80" s="76"/>
+      <c r="IL80" s="76"/>
+      <c r="IM80" s="76"/>
       <c r="JJ80" s="77"/>
       <c r="JK80" s="63"/>
       <c r="JL80" s="51"/>
@@ -48836,16 +48887,16 @@
       <c r="LE80" s="29"/>
       <c r="LF80" s="29"/>
       <c r="LG80" s="31"/>
-      <c r="LH80" s="69" t="s">
-        <v>147</v>
-      </c>
-      <c r="LI80" s="69"/>
-      <c r="LJ80" s="69"/>
-      <c r="LK80" s="69"/>
-      <c r="LL80" s="69"/>
-      <c r="LM80" s="69"/>
-      <c r="LN80" s="69"/>
-      <c r="LO80" s="69"/>
+      <c r="LH80" s="76" t="s">
+        <v>139</v>
+      </c>
+      <c r="LI80" s="76"/>
+      <c r="LJ80" s="76"/>
+      <c r="LK80" s="76"/>
+      <c r="LL80" s="76"/>
+      <c r="LM80" s="76"/>
+      <c r="LN80" s="76"/>
+      <c r="LO80" s="76"/>
     </row>
     <row r="81" spans="1:327">
       <c r="A81" s="70"/>
@@ -49814,16 +49865,16 @@
       <c r="LE82" s="31"/>
       <c r="LF82" s="31"/>
       <c r="LG82" s="31"/>
-      <c r="LH82" s="69" t="s">
-        <v>148</v>
-      </c>
-      <c r="LI82" s="69"/>
-      <c r="LJ82" s="69"/>
-      <c r="LK82" s="69"/>
-      <c r="LL82" s="69"/>
-      <c r="LM82" s="69"/>
-      <c r="LN82" s="69"/>
-      <c r="LO82" s="69"/>
+      <c r="LH82" s="76" t="s">
+        <v>140</v>
+      </c>
+      <c r="LI82" s="76"/>
+      <c r="LJ82" s="76"/>
+      <c r="LK82" s="76"/>
+      <c r="LL82" s="76"/>
+      <c r="LM82" s="76"/>
+      <c r="LN82" s="76"/>
+      <c r="LO82" s="76"/>
     </row>
     <row r="83" spans="1:327">
       <c r="A83" s="70"/>
@@ -51230,14 +51281,14 @@
       <c r="LG85" s="31"/>
     </row>
     <row r="86" spans="1:327" ht="20">
-      <c r="L86" s="69" t="s">
+      <c r="L86" s="76" t="s">
         <v>13</v>
       </c>
-      <c r="M86" s="69"/>
-      <c r="N86" s="69"/>
-      <c r="O86" s="69"/>
-      <c r="P86" s="69"/>
-      <c r="Q86" s="69"/>
+      <c r="M86" s="76"/>
+      <c r="N86" s="76"/>
+      <c r="O86" s="76"/>
+      <c r="P86" s="76"/>
+      <c r="Q86" s="76"/>
       <c r="Z86" s="45" t="s">
         <v>11</v>
       </c>
@@ -51343,30 +51394,30 @@
       <c r="EB86" s="8"/>
       <c r="EC86" s="8"/>
       <c r="ED86" s="8"/>
-      <c r="EE86" s="69" t="s">
+      <c r="EE86" s="76" t="s">
         <v>114</v>
       </c>
-      <c r="EF86" s="69"/>
-      <c r="EG86" s="69"/>
-      <c r="EH86" s="69"/>
-      <c r="EI86" s="69"/>
-      <c r="EJ86" s="69"/>
+      <c r="EF86" s="76"/>
+      <c r="EG86" s="76"/>
+      <c r="EH86" s="76"/>
+      <c r="EI86" s="76"/>
+      <c r="EJ86" s="76"/>
       <c r="EM86" s="45" t="s">
         <v>116</v>
       </c>
       <c r="EO86" s="48" t="s">
         <v>117</v>
       </c>
-      <c r="ER86" s="69" t="s">
+      <c r="ER86" s="76" t="s">
         <v>118</v>
       </c>
-      <c r="ES86" s="69"/>
-      <c r="ET86" s="69"/>
-      <c r="EU86" s="69"/>
-      <c r="EV86" s="69"/>
-      <c r="EW86" s="69"/>
-      <c r="EX86" s="69"/>
-      <c r="EY86" s="69"/>
+      <c r="ES86" s="76"/>
+      <c r="ET86" s="76"/>
+      <c r="EU86" s="76"/>
+      <c r="EV86" s="76"/>
+      <c r="EW86" s="76"/>
+      <c r="EX86" s="76"/>
+      <c r="EY86" s="76"/>
       <c r="FO86" s="57"/>
       <c r="FP86" s="8"/>
       <c r="FQ86" s="8"/>
@@ -51387,10 +51438,10 @@
       <c r="GF86" s="8"/>
       <c r="GG86" s="8"/>
       <c r="GJ86" s="52" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="GM86" s="68" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="GN86" s="68"/>
       <c r="GO86" s="68"/>
@@ -51411,30 +51462,30 @@
       <c r="HD86" s="8"/>
       <c r="HE86" s="8"/>
       <c r="HF86" s="8"/>
-      <c r="HG86" s="69" t="s">
+      <c r="HG86" s="76" t="s">
+        <v>125</v>
+      </c>
+      <c r="HH86" s="76"/>
+      <c r="HI86" s="76"/>
+      <c r="HJ86" s="76"/>
+      <c r="HK86" s="76"/>
+      <c r="HL86" s="76"/>
+      <c r="HO86" s="52" t="s">
+        <v>127</v>
+      </c>
+      <c r="HQ86" s="53" t="s">
+        <v>128</v>
+      </c>
+      <c r="HT86" s="76" t="s">
         <v>129</v>
       </c>
-      <c r="HH86" s="69"/>
-      <c r="HI86" s="69"/>
-      <c r="HJ86" s="69"/>
-      <c r="HK86" s="69"/>
-      <c r="HL86" s="69"/>
-      <c r="HO86" s="52" t="s">
-        <v>131</v>
-      </c>
-      <c r="HQ86" s="53" t="s">
-        <v>132</v>
-      </c>
-      <c r="HT86" s="69" t="s">
-        <v>133</v>
-      </c>
-      <c r="HU86" s="69"/>
-      <c r="HV86" s="69"/>
-      <c r="HW86" s="69"/>
-      <c r="HX86" s="69"/>
-      <c r="HY86" s="69"/>
-      <c r="HZ86" s="69"/>
-      <c r="IA86" s="69"/>
+      <c r="HU86" s="76"/>
+      <c r="HV86" s="76"/>
+      <c r="HW86" s="76"/>
+      <c r="HX86" s="76"/>
+      <c r="HY86" s="76"/>
+      <c r="HZ86" s="76"/>
+      <c r="IA86" s="76"/>
       <c r="IQ86" s="57"/>
       <c r="IR86" s="8"/>
       <c r="IS86" s="8"/>
@@ -51459,14 +51510,14 @@
       <c r="JL86" s="55"/>
       <c r="JM86" s="31"/>
       <c r="JN86" s="31"/>
-      <c r="JO86" s="72"/>
-      <c r="JP86" s="72"/>
-      <c r="JQ86" s="72"/>
-      <c r="JR86" s="72"/>
-      <c r="JS86" s="72"/>
-      <c r="JT86" s="72"/>
-      <c r="JU86" s="72"/>
-      <c r="JV86" s="72"/>
+      <c r="JO86" s="75"/>
+      <c r="JP86" s="75"/>
+      <c r="JQ86" s="75"/>
+      <c r="JR86" s="75"/>
+      <c r="JS86" s="75"/>
+      <c r="JT86" s="75"/>
+      <c r="JU86" s="75"/>
+      <c r="JV86" s="75"/>
       <c r="JW86" s="29"/>
       <c r="JX86" s="29"/>
       <c r="JY86" s="8"/>
@@ -51479,30 +51530,30 @@
       <c r="KF86" s="8"/>
       <c r="KG86" s="8"/>
       <c r="KH86" s="8"/>
-      <c r="KI86" s="69" t="s">
+      <c r="KI86" s="76" t="s">
         <v>97</v>
       </c>
-      <c r="KJ86" s="69"/>
-      <c r="KK86" s="69"/>
-      <c r="KL86" s="69"/>
-      <c r="KM86" s="69"/>
-      <c r="KN86" s="69"/>
+      <c r="KJ86" s="76"/>
+      <c r="KK86" s="76"/>
+      <c r="KL86" s="76"/>
+      <c r="KM86" s="76"/>
+      <c r="KN86" s="76"/>
       <c r="KQ86" s="52" t="s">
         <v>98</v>
       </c>
       <c r="KS86" s="53" t="s">
-        <v>139</v>
-      </c>
-      <c r="KV86" s="69" t="s">
-        <v>140</v>
-      </c>
-      <c r="KW86" s="69"/>
-      <c r="KX86" s="69"/>
-      <c r="KY86" s="69"/>
-      <c r="KZ86" s="69"/>
-      <c r="LA86" s="69"/>
-      <c r="LB86" s="69"/>
-      <c r="LC86" s="69"/>
+        <v>135</v>
+      </c>
+      <c r="KV86" s="76" t="s">
+        <v>136</v>
+      </c>
+      <c r="KW86" s="76"/>
+      <c r="KX86" s="76"/>
+      <c r="KY86" s="76"/>
+      <c r="KZ86" s="76"/>
+      <c r="LA86" s="76"/>
+      <c r="LB86" s="76"/>
+      <c r="LC86" s="76"/>
     </row>
     <row r="87" spans="1:327" ht="16" customHeight="1">
       <c r="J87" s="70" t="s">
@@ -51872,49 +51923,49 @@
       </c>
     </row>
     <row r="90" spans="1:327" ht="20">
-      <c r="L90" s="69" t="s">
+      <c r="L90" s="76" t="s">
         <v>35</v>
       </c>
-      <c r="M90" s="69"/>
-      <c r="N90" s="69"/>
-      <c r="O90" s="69"/>
-      <c r="P90" s="69"/>
-      <c r="Q90" s="69"/>
-      <c r="EE90" s="69" t="s">
+      <c r="M90" s="76"/>
+      <c r="N90" s="76"/>
+      <c r="O90" s="76"/>
+      <c r="P90" s="76"/>
+      <c r="Q90" s="76"/>
+      <c r="EE90" s="76" t="s">
         <v>115</v>
       </c>
-      <c r="EF90" s="69"/>
-      <c r="EG90" s="69"/>
-      <c r="EH90" s="69"/>
-      <c r="EI90" s="69"/>
-      <c r="EJ90" s="69"/>
+      <c r="EF90" s="76"/>
+      <c r="EG90" s="76"/>
+      <c r="EH90" s="76"/>
+      <c r="EI90" s="76"/>
+      <c r="EJ90" s="76"/>
       <c r="EM90" s="53" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="EN90" s="53"/>
       <c r="EO90" s="53"/>
       <c r="EP90" s="53"/>
       <c r="EQ90" s="53"/>
       <c r="ER90" s="53"/>
-      <c r="HG90" s="69" t="s">
-        <v>130</v>
-      </c>
-      <c r="HH90" s="69"/>
-      <c r="HI90" s="69"/>
-      <c r="HJ90" s="69"/>
-      <c r="HK90" s="69"/>
-      <c r="HL90" s="69"/>
+      <c r="HG90" s="76" t="s">
+        <v>126</v>
+      </c>
+      <c r="HH90" s="76"/>
+      <c r="HI90" s="76"/>
+      <c r="HJ90" s="76"/>
+      <c r="HK90" s="76"/>
+      <c r="HL90" s="76"/>
       <c r="HO90" s="53" t="s">
-        <v>145</v>
-      </c>
-      <c r="KI90" s="69" t="s">
+        <v>138</v>
+      </c>
+      <c r="KI90" s="76" t="s">
         <v>99</v>
       </c>
-      <c r="KJ90" s="69"/>
-      <c r="KK90" s="69"/>
-      <c r="KL90" s="69"/>
-      <c r="KM90" s="69"/>
-      <c r="KN90" s="69"/>
+      <c r="KJ90" s="76"/>
+      <c r="KK90" s="76"/>
+      <c r="KL90" s="76"/>
+      <c r="KM90" s="76"/>
+      <c r="KN90" s="76"/>
     </row>
     <row r="93" spans="1:327" ht="47">
       <c r="A93" s="27" t="s">
@@ -52365,7 +52416,7 @@
         <v>57</v>
       </c>
       <c r="JY105" s="53" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="KA105" s="52" t="s">
         <v>98</v>
@@ -53130,17 +53181,17 @@
       </c>
       <c r="D115" s="68"/>
       <c r="E115" s="68"/>
-      <c r="G115" s="69" t="s">
+      <c r="G115" s="76" t="s">
         <v>39</v>
       </c>
-      <c r="H115" s="69"/>
-      <c r="I115" s="69"/>
+      <c r="H115" s="76"/>
+      <c r="I115" s="76"/>
       <c r="J115" s="17"/>
-      <c r="K115" s="69" t="s">
+      <c r="K115" s="76" t="s">
         <v>40</v>
       </c>
-      <c r="L115" s="69"/>
-      <c r="M115" s="69"/>
+      <c r="L115" s="76"/>
+      <c r="M115" s="76"/>
       <c r="N115" s="17"/>
       <c r="O115" s="17" t="s">
         <v>41</v>
@@ -53151,24 +53202,24 @@
       <c r="AN115" s="18"/>
       <c r="AO115" s="18"/>
       <c r="JY115" s="68" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="JZ115" s="68"/>
       <c r="KA115" s="68"/>
-      <c r="KC115" s="69" t="s">
-        <v>152</v>
-      </c>
-      <c r="KD115" s="69"/>
-      <c r="KE115" s="69"/>
+      <c r="KC115" s="76" t="s">
+        <v>144</v>
+      </c>
+      <c r="KD115" s="76"/>
+      <c r="KE115" s="76"/>
       <c r="KF115" s="17"/>
-      <c r="KG115" s="69" t="s">
-        <v>157</v>
-      </c>
-      <c r="KH115" s="69"/>
-      <c r="KI115" s="69"/>
+      <c r="KG115" s="76" t="s">
+        <v>149</v>
+      </c>
+      <c r="KH115" s="76"/>
+      <c r="KI115" s="76"/>
       <c r="KJ115" s="17"/>
       <c r="KK115" s="17" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
       <c r="KL115" s="17"/>
     </row>
@@ -53424,67 +53475,134 @@
         <v>34</v>
       </c>
       <c r="D126" s="52" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="F126" s="32" t="s">
         <v>67</v>
       </c>
       <c r="JY126" s="52" t="s">
+        <v>145</v>
+      </c>
+      <c r="JZ126" s="52" t="s">
+        <v>151</v>
+      </c>
+      <c r="KB126" s="32" t="s">
+        <v>152</v>
+      </c>
+      <c r="KD126" s="32" t="s">
         <v>153</v>
-      </c>
-      <c r="JZ126" s="52" t="s">
-        <v>159</v>
-      </c>
-      <c r="KB126" s="32" t="s">
-        <v>160</v>
-      </c>
-      <c r="KD126" s="32" t="s">
-        <v>161</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="173">
-    <mergeCell ref="GH78:GH85"/>
-    <mergeCell ref="HE78:HE85"/>
-    <mergeCell ref="A120:A125"/>
-    <mergeCell ref="A97:A104"/>
-    <mergeCell ref="A107:I107"/>
-    <mergeCell ref="A109:A114"/>
-    <mergeCell ref="C115:E115"/>
-    <mergeCell ref="G115:I115"/>
-    <mergeCell ref="K115:M115"/>
-    <mergeCell ref="ER86:EY86"/>
-    <mergeCell ref="J87:J89"/>
-    <mergeCell ref="EC87:EC89"/>
-    <mergeCell ref="L90:Q90"/>
-    <mergeCell ref="EE90:EJ90"/>
-    <mergeCell ref="A95:I95"/>
-    <mergeCell ref="L86:Q86"/>
-    <mergeCell ref="AH86:AO86"/>
-    <mergeCell ref="AS86:AZ86"/>
-    <mergeCell ref="BD86:BK86"/>
-    <mergeCell ref="DK86:DR86"/>
-    <mergeCell ref="EE86:EJ86"/>
-    <mergeCell ref="BS86:BX86"/>
-    <mergeCell ref="BS72:BX72"/>
-    <mergeCell ref="EE76:EJ76"/>
-    <mergeCell ref="ER76:EY76"/>
-    <mergeCell ref="FD76:FK76"/>
-    <mergeCell ref="A78:A85"/>
-    <mergeCell ref="DF78:DF85"/>
-    <mergeCell ref="EC78:EC85"/>
-    <mergeCell ref="FB78:FB79"/>
-    <mergeCell ref="FD80:FK80"/>
-    <mergeCell ref="AH76:AO76"/>
-    <mergeCell ref="AS76:AZ76"/>
-    <mergeCell ref="BD76:BK76"/>
-    <mergeCell ref="DK76:DR76"/>
-    <mergeCell ref="C72:J72"/>
-    <mergeCell ref="Z72:AB72"/>
-    <mergeCell ref="AH72:AM72"/>
-    <mergeCell ref="AS72:AZ72"/>
-    <mergeCell ref="BD72:BK72"/>
-    <mergeCell ref="BS76:BX76"/>
+    <mergeCell ref="JW95:KE95"/>
+    <mergeCell ref="JW97:JW104"/>
+    <mergeCell ref="JW107:KE107"/>
+    <mergeCell ref="JW109:JW114"/>
+    <mergeCell ref="JY115:KA115"/>
+    <mergeCell ref="KC115:KE115"/>
+    <mergeCell ref="KG115:KI115"/>
+    <mergeCell ref="JW120:JW125"/>
+    <mergeCell ref="JJ78:JJ85"/>
+    <mergeCell ref="KG78:KG85"/>
+    <mergeCell ref="LF78:LF79"/>
+    <mergeCell ref="LH80:LO80"/>
+    <mergeCell ref="JO86:JV86"/>
+    <mergeCell ref="KI86:KN86"/>
+    <mergeCell ref="KV86:LC86"/>
+    <mergeCell ref="KG87:KG89"/>
+    <mergeCell ref="KI90:KN90"/>
+    <mergeCell ref="LH82:LO82"/>
+    <mergeCell ref="KY64:LF64"/>
+    <mergeCell ref="KP64:KR64"/>
+    <mergeCell ref="JJ66:JJ71"/>
+    <mergeCell ref="KY67:LF67"/>
+    <mergeCell ref="JO72:JT72"/>
+    <mergeCell ref="JX72:KE72"/>
+    <mergeCell ref="JO76:JV76"/>
+    <mergeCell ref="KI76:KN76"/>
+    <mergeCell ref="KV76:LC76"/>
+    <mergeCell ref="LH76:LO76"/>
+    <mergeCell ref="JV66:JV71"/>
+    <mergeCell ref="KP72:KR72"/>
+    <mergeCell ref="JL40:JM40"/>
+    <mergeCell ref="KI40:KN40"/>
+    <mergeCell ref="IU42:IU49"/>
+    <mergeCell ref="JJ42:JJ49"/>
+    <mergeCell ref="IW50:IX50"/>
+    <mergeCell ref="IZ50:JE50"/>
+    <mergeCell ref="KI50:KN50"/>
+    <mergeCell ref="JO64:JT64"/>
+    <mergeCell ref="JX64:KE64"/>
+    <mergeCell ref="KG42:KG49"/>
+    <mergeCell ref="KG51:KG53"/>
+    <mergeCell ref="KI54:KN54"/>
+    <mergeCell ref="KI56:KN56"/>
+    <mergeCell ref="ID78:ID79"/>
+    <mergeCell ref="IF80:IM80"/>
+    <mergeCell ref="GM86:GT86"/>
+    <mergeCell ref="HG86:HL86"/>
+    <mergeCell ref="HT86:IA86"/>
+    <mergeCell ref="HE87:HE89"/>
+    <mergeCell ref="HG90:HL90"/>
+    <mergeCell ref="IW40:IX40"/>
+    <mergeCell ref="IZ40:JE40"/>
+    <mergeCell ref="GJ40:GO40"/>
+    <mergeCell ref="GJ50:GO50"/>
+    <mergeCell ref="HW64:ID64"/>
+    <mergeCell ref="GM76:GT76"/>
+    <mergeCell ref="HG76:HL76"/>
+    <mergeCell ref="HT76:IA76"/>
+    <mergeCell ref="IF76:IM76"/>
+    <mergeCell ref="CV40:DA40"/>
+    <mergeCell ref="CV50:DA50"/>
+    <mergeCell ref="FU40:FV40"/>
+    <mergeCell ref="FX40:GC40"/>
+    <mergeCell ref="HG40:HL40"/>
+    <mergeCell ref="FS42:FS49"/>
+    <mergeCell ref="FU50:FV50"/>
+    <mergeCell ref="FX50:GC50"/>
+    <mergeCell ref="HG50:HL50"/>
+    <mergeCell ref="DH40:DM40"/>
+    <mergeCell ref="DH50:DM50"/>
+    <mergeCell ref="DK72:DP72"/>
+    <mergeCell ref="DT72:EA72"/>
+    <mergeCell ref="GM64:GR64"/>
+    <mergeCell ref="GV64:HC64"/>
+    <mergeCell ref="EE50:EJ50"/>
+    <mergeCell ref="AS58:AZ58"/>
+    <mergeCell ref="L50:Q50"/>
+    <mergeCell ref="W50:X50"/>
+    <mergeCell ref="A42:A49"/>
+    <mergeCell ref="U42:U49"/>
+    <mergeCell ref="GH66:GH71"/>
+    <mergeCell ref="HW67:ID67"/>
+    <mergeCell ref="GM72:GR72"/>
+    <mergeCell ref="GV72:HC72"/>
+    <mergeCell ref="CQ42:CQ49"/>
+    <mergeCell ref="DF42:DF49"/>
+    <mergeCell ref="A60:A61"/>
+    <mergeCell ref="C62:J62"/>
+    <mergeCell ref="Z62:AB62"/>
+    <mergeCell ref="AH62:AI62"/>
+    <mergeCell ref="AK62:AL62"/>
+    <mergeCell ref="AS62:AZ62"/>
+    <mergeCell ref="DT64:EA64"/>
+    <mergeCell ref="Z64:AB64"/>
+    <mergeCell ref="AH64:AM64"/>
+    <mergeCell ref="AS64:AZ64"/>
+    <mergeCell ref="BD64:BK64"/>
+    <mergeCell ref="AH50:AO50"/>
+    <mergeCell ref="AS50:AX50"/>
+    <mergeCell ref="BD50:BI50"/>
+    <mergeCell ref="CS50:CT50"/>
+    <mergeCell ref="BS50:BX50"/>
+    <mergeCell ref="BZ50:CG50"/>
+    <mergeCell ref="J51:J53"/>
+    <mergeCell ref="L54:Q54"/>
+    <mergeCell ref="Z58:AB58"/>
+    <mergeCell ref="AH58:AI58"/>
+    <mergeCell ref="AK58:AL58"/>
     <mergeCell ref="EU64:FB64"/>
     <mergeCell ref="A66:A71"/>
     <mergeCell ref="DF66:DF71"/>
@@ -53509,114 +53627,47 @@
     <mergeCell ref="CS40:CT40"/>
     <mergeCell ref="EE40:EJ40"/>
     <mergeCell ref="C64:J64"/>
-    <mergeCell ref="CQ42:CQ49"/>
-    <mergeCell ref="DF42:DF49"/>
-    <mergeCell ref="A60:A61"/>
-    <mergeCell ref="C62:J62"/>
-    <mergeCell ref="Z62:AB62"/>
-    <mergeCell ref="AH62:AI62"/>
-    <mergeCell ref="AK62:AL62"/>
-    <mergeCell ref="AS62:AZ62"/>
-    <mergeCell ref="DT64:EA64"/>
-    <mergeCell ref="Z64:AB64"/>
-    <mergeCell ref="AH64:AM64"/>
-    <mergeCell ref="AS64:AZ64"/>
-    <mergeCell ref="BD64:BK64"/>
-    <mergeCell ref="AH50:AO50"/>
-    <mergeCell ref="AS50:AX50"/>
-    <mergeCell ref="BD50:BI50"/>
-    <mergeCell ref="CS50:CT50"/>
-    <mergeCell ref="BS50:BX50"/>
-    <mergeCell ref="BZ50:CG50"/>
-    <mergeCell ref="J51:J53"/>
-    <mergeCell ref="L54:Q54"/>
-    <mergeCell ref="Z58:AB58"/>
-    <mergeCell ref="AH58:AI58"/>
-    <mergeCell ref="AK58:AL58"/>
-    <mergeCell ref="AS58:AZ58"/>
-    <mergeCell ref="L50:Q50"/>
-    <mergeCell ref="W50:X50"/>
-    <mergeCell ref="A42:A49"/>
-    <mergeCell ref="U42:U49"/>
-    <mergeCell ref="GH66:GH71"/>
-    <mergeCell ref="HW67:ID67"/>
-    <mergeCell ref="GM72:GR72"/>
-    <mergeCell ref="GV72:HC72"/>
-    <mergeCell ref="GM76:GT76"/>
-    <mergeCell ref="HG76:HL76"/>
-    <mergeCell ref="HT76:IA76"/>
-    <mergeCell ref="IF76:IM76"/>
-    <mergeCell ref="CV40:DA40"/>
-    <mergeCell ref="CV50:DA50"/>
-    <mergeCell ref="FU40:FV40"/>
-    <mergeCell ref="FX40:GC40"/>
-    <mergeCell ref="HG40:HL40"/>
-    <mergeCell ref="FS42:FS49"/>
-    <mergeCell ref="FU50:FV50"/>
-    <mergeCell ref="FX50:GC50"/>
-    <mergeCell ref="HG50:HL50"/>
-    <mergeCell ref="DH40:DM40"/>
-    <mergeCell ref="DH50:DM50"/>
-    <mergeCell ref="DK72:DP72"/>
-    <mergeCell ref="DT72:EA72"/>
-    <mergeCell ref="GM64:GR64"/>
-    <mergeCell ref="GV64:HC64"/>
-    <mergeCell ref="EE50:EJ50"/>
-    <mergeCell ref="ID78:ID79"/>
-    <mergeCell ref="IF80:IM80"/>
-    <mergeCell ref="GM86:GT86"/>
-    <mergeCell ref="HG86:HL86"/>
-    <mergeCell ref="HT86:IA86"/>
-    <mergeCell ref="HE87:HE89"/>
-    <mergeCell ref="HG90:HL90"/>
-    <mergeCell ref="IW40:IX40"/>
-    <mergeCell ref="IZ40:JE40"/>
-    <mergeCell ref="GJ40:GO40"/>
-    <mergeCell ref="GJ50:GO50"/>
-    <mergeCell ref="HW64:ID64"/>
-    <mergeCell ref="JL40:JM40"/>
-    <mergeCell ref="KI40:KN40"/>
-    <mergeCell ref="IU42:IU49"/>
-    <mergeCell ref="JJ42:JJ49"/>
-    <mergeCell ref="IW50:IX50"/>
-    <mergeCell ref="IZ50:JE50"/>
-    <mergeCell ref="KI50:KN50"/>
-    <mergeCell ref="JO64:JT64"/>
-    <mergeCell ref="JX64:KE64"/>
-    <mergeCell ref="KG42:KG49"/>
-    <mergeCell ref="KG51:KG53"/>
-    <mergeCell ref="KI54:KN54"/>
-    <mergeCell ref="KI56:KN56"/>
-    <mergeCell ref="JJ66:JJ71"/>
-    <mergeCell ref="KY67:LF67"/>
-    <mergeCell ref="JO72:JT72"/>
-    <mergeCell ref="JX72:KE72"/>
-    <mergeCell ref="JO76:JV76"/>
-    <mergeCell ref="KI76:KN76"/>
-    <mergeCell ref="KV76:LC76"/>
-    <mergeCell ref="LH76:LO76"/>
-    <mergeCell ref="JV66:JV71"/>
-    <mergeCell ref="KP72:KR72"/>
-    <mergeCell ref="LF78:LF79"/>
-    <mergeCell ref="LH80:LO80"/>
-    <mergeCell ref="JO86:JV86"/>
-    <mergeCell ref="KI86:KN86"/>
-    <mergeCell ref="KV86:LC86"/>
-    <mergeCell ref="KG87:KG89"/>
-    <mergeCell ref="KI90:KN90"/>
-    <mergeCell ref="LH82:LO82"/>
-    <mergeCell ref="KY64:LF64"/>
-    <mergeCell ref="KP64:KR64"/>
-    <mergeCell ref="JW95:KE95"/>
-    <mergeCell ref="JW97:JW104"/>
-    <mergeCell ref="JW107:KE107"/>
-    <mergeCell ref="JW109:JW114"/>
-    <mergeCell ref="JY115:KA115"/>
-    <mergeCell ref="KC115:KE115"/>
-    <mergeCell ref="KG115:KI115"/>
-    <mergeCell ref="JW120:JW125"/>
-    <mergeCell ref="JJ78:JJ85"/>
-    <mergeCell ref="KG78:KG85"/>
+    <mergeCell ref="BS72:BX72"/>
+    <mergeCell ref="EE76:EJ76"/>
+    <mergeCell ref="ER76:EY76"/>
+    <mergeCell ref="FD76:FK76"/>
+    <mergeCell ref="A78:A85"/>
+    <mergeCell ref="DF78:DF85"/>
+    <mergeCell ref="EC78:EC85"/>
+    <mergeCell ref="FB78:FB79"/>
+    <mergeCell ref="FD80:FK80"/>
+    <mergeCell ref="AH76:AO76"/>
+    <mergeCell ref="AS76:AZ76"/>
+    <mergeCell ref="BD76:BK76"/>
+    <mergeCell ref="DK76:DR76"/>
+    <mergeCell ref="C72:J72"/>
+    <mergeCell ref="Z72:AB72"/>
+    <mergeCell ref="AH72:AM72"/>
+    <mergeCell ref="AS72:AZ72"/>
+    <mergeCell ref="BD72:BK72"/>
+    <mergeCell ref="BS76:BX76"/>
+    <mergeCell ref="GH78:GH85"/>
+    <mergeCell ref="HE78:HE85"/>
+    <mergeCell ref="A120:A125"/>
+    <mergeCell ref="A97:A104"/>
+    <mergeCell ref="A107:I107"/>
+    <mergeCell ref="A109:A114"/>
+    <mergeCell ref="C115:E115"/>
+    <mergeCell ref="G115:I115"/>
+    <mergeCell ref="K115:M115"/>
+    <mergeCell ref="ER86:EY86"/>
+    <mergeCell ref="J87:J89"/>
+    <mergeCell ref="EC87:EC89"/>
+    <mergeCell ref="L90:Q90"/>
+    <mergeCell ref="EE90:EJ90"/>
+    <mergeCell ref="A95:I95"/>
+    <mergeCell ref="L86:Q86"/>
+    <mergeCell ref="AH86:AO86"/>
+    <mergeCell ref="AS86:AZ86"/>
+    <mergeCell ref="BD86:BK86"/>
+    <mergeCell ref="DK86:DR86"/>
+    <mergeCell ref="EE86:EJ86"/>
+    <mergeCell ref="BS86:BX86"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -53629,7 +53680,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81DB1CE6-E3EC-7B4E-8832-2A8872C682BA}">
   <dimension ref="A1:J21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:A21"/>
     </sheetView>
   </sheetViews>
@@ -53640,57 +53691,57 @@
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" t="s">
+        <v>162</v>
+      </c>
+      <c r="B1" t="s">
+        <v>163</v>
+      </c>
+      <c r="C1" t="s">
+        <v>164</v>
+      </c>
+      <c r="D1" t="s">
+        <v>165</v>
+      </c>
+      <c r="E1" t="s">
+        <v>166</v>
+      </c>
+      <c r="F1" t="s">
+        <v>167</v>
+      </c>
+      <c r="G1" t="s">
+        <v>168</v>
+      </c>
+      <c r="H1" t="s">
+        <v>169</v>
+      </c>
+      <c r="I1" t="s">
         <v>170</v>
       </c>
-      <c r="B1" t="s">
+      <c r="J1" t="s">
         <v>171</v>
-      </c>
-      <c r="C1" t="s">
-        <v>172</v>
-      </c>
-      <c r="D1" t="s">
-        <v>173</v>
-      </c>
-      <c r="E1" t="s">
-        <v>174</v>
-      </c>
-      <c r="F1" t="s">
-        <v>175</v>
-      </c>
-      <c r="G1" t="s">
-        <v>176</v>
-      </c>
-      <c r="H1" t="s">
-        <v>177</v>
-      </c>
-      <c r="I1" t="s">
-        <v>178</v>
-      </c>
-      <c r="J1" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="2" spans="1:10">
       <c r="A2" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="B2">
         <v>2000</v>
       </c>
       <c r="C2" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
       <c r="D2" t="s">
+        <v>173</v>
+      </c>
+      <c r="E2" t="s">
+        <v>174</v>
+      </c>
+      <c r="F2" t="s">
         <v>181</v>
       </c>
-      <c r="E2" t="s">
-        <v>182</v>
-      </c>
-      <c r="F2" t="s">
-        <v>189</v>
-      </c>
       <c r="G2" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
       <c r="H2" t="s">
         <v>23</v>
@@ -53700,27 +53751,27 @@
         <v>22.4</v>
       </c>
       <c r="J2" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="B3">
         <v>2000</v>
       </c>
       <c r="C3" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
       <c r="D3" t="s">
+        <v>173</v>
+      </c>
+      <c r="E3" t="s">
+        <v>174</v>
+      </c>
+      <c r="F3" t="s">
         <v>181</v>
-      </c>
-      <c r="E3" t="s">
-        <v>182</v>
-      </c>
-      <c r="F3" t="s">
-        <v>189</v>
       </c>
       <c r="G3" t="s">
         <v>21</v>
@@ -53733,27 +53784,27 @@
         <v>87</v>
       </c>
       <c r="J3" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="B4">
         <v>2000</v>
       </c>
       <c r="C4" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
       <c r="D4" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
       <c r="E4" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
       <c r="F4" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
       <c r="G4" t="s">
         <v>22</v>
@@ -53766,27 +53817,27 @@
         <v>-22.4</v>
       </c>
       <c r="J4" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="B5">
         <v>2000</v>
       </c>
       <c r="C5" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
       <c r="D5" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="E5" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
       <c r="F5" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
       <c r="G5" t="s">
         <v>22</v>
@@ -53799,27 +53850,27 @@
         <v>-3</v>
       </c>
       <c r="J5" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="B6">
         <v>2000</v>
       </c>
       <c r="C6" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
       <c r="D6" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
       <c r="E6" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
       <c r="F6" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
       <c r="G6" t="s">
         <v>22</v>
@@ -53832,27 +53883,27 @@
         <v>22.4</v>
       </c>
       <c r="J6" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="B7">
         <v>2000</v>
       </c>
       <c r="C7" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
       <c r="D7" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
       <c r="E7" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
       <c r="F7" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
       <c r="G7" t="s">
         <v>24</v>
@@ -53865,27 +53916,27 @@
         <v>-87</v>
       </c>
       <c r="J7" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="B8">
         <v>2000</v>
       </c>
       <c r="C8" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
       <c r="D8" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
       <c r="E8" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
       <c r="F8" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
       <c r="G8" t="s">
         <v>24</v>
@@ -53898,27 +53949,27 @@
         <v>78.2</v>
       </c>
       <c r="J8" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
     </row>
     <row r="9" spans="1:10">
       <c r="A9" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="B9">
         <v>2000</v>
       </c>
       <c r="C9" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
       <c r="D9" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
       <c r="E9" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
       <c r="F9" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
       <c r="G9" t="s">
         <v>25</v>
@@ -53931,27 +53982,27 @@
         <v>-17.8</v>
       </c>
       <c r="J9" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
     </row>
     <row r="10" spans="1:10">
       <c r="A10" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="B10">
         <v>2000</v>
       </c>
       <c r="C10" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
       <c r="D10" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
       <c r="E10" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
       <c r="F10" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
       <c r="G10" t="s">
         <v>25</v>
@@ -53964,27 +54015,27 @@
         <v>12.6</v>
       </c>
       <c r="J10" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="B11">
         <v>2000</v>
       </c>
       <c r="C11" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
       <c r="D11" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
       <c r="E11" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
       <c r="F11" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
       <c r="G11" t="s">
         <v>16</v>
@@ -53997,27 +54048,27 @@
         <v>-28.1</v>
       </c>
       <c r="J11" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
     </row>
     <row r="12" spans="1:10">
       <c r="A12" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="B12">
         <v>2000</v>
       </c>
       <c r="C12" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
       <c r="D12" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
       <c r="E12" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
       <c r="F12" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
       <c r="G12" t="s">
         <v>16</v>
@@ -54035,22 +54086,22 @@
     </row>
     <row r="13" spans="1:10">
       <c r="A13" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="B13">
         <v>2000</v>
       </c>
       <c r="C13" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
       <c r="D13" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
       <c r="E13" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
       <c r="F13" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
       <c r="G13" t="s">
         <v>15</v>
@@ -54063,27 +54114,27 @@
         <v>-19.399999999999999</v>
       </c>
       <c r="J13" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
     </row>
     <row r="14" spans="1:10">
       <c r="A14" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="B14">
         <v>2000</v>
       </c>
       <c r="C14" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
       <c r="D14" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
       <c r="E14" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
       <c r="F14" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
       <c r="G14" t="s">
         <v>15</v>
@@ -54096,27 +54147,27 @@
         <v>-0.5</v>
       </c>
       <c r="J14" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
     </row>
     <row r="15" spans="1:10">
       <c r="A15" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="B15">
         <v>2000</v>
       </c>
       <c r="C15" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
       <c r="D15" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
       <c r="E15" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
       <c r="F15" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
       <c r="G15" t="s">
         <v>15</v>
@@ -54134,22 +54185,22 @@
     </row>
     <row r="16" spans="1:10">
       <c r="A16" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="B16">
         <v>2000</v>
       </c>
       <c r="C16" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
       <c r="D16" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
       <c r="E16" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
       <c r="F16" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
       <c r="G16" t="s">
         <v>0</v>
@@ -54162,27 +54213,27 @@
         <v>-12.1</v>
       </c>
       <c r="J16" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
     </row>
     <row r="17" spans="1:10">
       <c r="A17" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="B17">
         <v>2000</v>
       </c>
       <c r="C17" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
       <c r="D17" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
       <c r="E17" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
       <c r="F17" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
       <c r="G17" t="s">
         <v>0</v>
@@ -54195,27 +54246,27 @@
         <v>-32.299999999999997</v>
       </c>
       <c r="J17" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
     </row>
     <row r="18" spans="1:10">
       <c r="A18" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="B18">
         <v>2000</v>
       </c>
       <c r="C18" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
       <c r="D18" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
       <c r="E18" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
       <c r="F18" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
       <c r="G18" t="s">
         <v>0</v>
@@ -54228,30 +54279,30 @@
         <v>25.2</v>
       </c>
       <c r="J18" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
     </row>
     <row r="19" spans="1:10">
       <c r="A19" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="B19">
         <v>2000</v>
       </c>
       <c r="C19" t="s">
-        <v>188</v>
+        <v>180</v>
       </c>
       <c r="D19" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
       <c r="E19" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
       <c r="F19" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
       <c r="G19" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
       <c r="H19" t="s">
         <v>18</v>
@@ -54266,25 +54317,25 @@
     </row>
     <row r="20" spans="1:10">
       <c r="A20" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="B20">
         <v>2000</v>
       </c>
       <c r="C20" t="s">
-        <v>188</v>
+        <v>180</v>
       </c>
       <c r="D20" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
       <c r="E20" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
       <c r="F20" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
       <c r="G20" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
       <c r="H20" t="s">
         <v>17</v>
@@ -54299,25 +54350,25 @@
     </row>
     <row r="21" spans="1:10">
       <c r="A21" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="B21">
         <v>2000</v>
       </c>
       <c r="C21" t="s">
-        <v>188</v>
+        <v>180</v>
       </c>
       <c r="D21" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
       <c r="E21" t="s">
+        <v>174</v>
+      </c>
+      <c r="F21" t="s">
+        <v>181</v>
+      </c>
+      <c r="G21" t="s">
         <v>182</v>
-      </c>
-      <c r="F21" t="s">
-        <v>189</v>
-      </c>
-      <c r="G21" t="s">
-        <v>190</v>
       </c>
       <c r="H21" t="s">
         <v>19</v>
@@ -54327,7 +54378,7 @@
         <v>25.2</v>
       </c>
       <c r="J21" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changes to upstread swim functions.
</commit_message>
<xml_diff>
--- a/inst/extdata/PerfectSubstitutionraw/UTEI_Sankey_Simple_ECC_Perfect_Sub.xlsx
+++ b/inst/extdata/PerfectSubstitutionraw/UTEI_Sankey_Simple_ECC_Perfect_Sub.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10910"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11014"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mkh2/github/Recca/inst/extdata/PerfectSubstitutionraw/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matt/github/Recca/inst/extdata/PerfectSubstitutionraw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEADC63E-07D2-0D41-A45F-1B27FBC787DD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{713B2AD8-BCA6-7C4D-B8F1-4D6EB19E176A}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="17560" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="25000" yWindow="440" windowWidth="26200" windowHeight="17560" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Meta" sheetId="10" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="Perfect substitution" sheetId="9" r:id="rId3"/>
     <sheet name="PerfectSubstitutionRaw" sheetId="11" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179021"/>
 </workbook>
 </file>
 
@@ -6856,7 +6856,7 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -6865,28 +6865,28 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -30637,11 +30637,11 @@
     </row>
     <row r="26" spans="1:93">
       <c r="B26" s="10"/>
-      <c r="C26" s="69" t="s">
+      <c r="C26" s="75" t="s">
         <v>30</v>
       </c>
-      <c r="D26" s="69"/>
-      <c r="E26" s="69"/>
+      <c r="D26" s="75"/>
+      <c r="E26" s="75"/>
       <c r="F26" s="39"/>
       <c r="G26" s="39"/>
     </row>
@@ -30910,11 +30910,11 @@
       <c r="CO35" s="31"/>
     </row>
     <row r="36" spans="1:93" ht="18">
-      <c r="C36" s="69" t="s">
+      <c r="C36" s="75" t="s">
         <v>31</v>
       </c>
-      <c r="D36" s="69"/>
-      <c r="E36" s="69"/>
+      <c r="D36" s="75"/>
+      <c r="E36" s="75"/>
       <c r="F36" s="39"/>
       <c r="G36" s="39"/>
       <c r="BM36" s="31"/>
@@ -33048,14 +33048,14 @@
       <c r="AA53" s="15"/>
     </row>
     <row r="54" spans="1:93" ht="20">
-      <c r="L54" s="72" t="s">
+      <c r="L54" s="73" t="s">
         <v>42</v>
       </c>
-      <c r="M54" s="72"/>
-      <c r="N54" s="72"/>
-      <c r="O54" s="72"/>
-      <c r="P54" s="72"/>
-      <c r="Q54" s="72"/>
+      <c r="M54" s="73"/>
+      <c r="N54" s="73"/>
+      <c r="O54" s="73"/>
+      <c r="P54" s="73"/>
+      <c r="Q54" s="73"/>
     </row>
     <row r="55" spans="1:93">
       <c r="L55" s="6">
@@ -33095,11 +33095,11 @@
     </row>
     <row r="60" spans="1:93">
       <c r="B60" s="1"/>
-      <c r="Z60" s="69" t="s">
+      <c r="Z60" s="75" t="s">
         <v>30</v>
       </c>
-      <c r="AA60" s="69"/>
-      <c r="AB60" s="69"/>
+      <c r="AA60" s="75"/>
+      <c r="AB60" s="75"/>
       <c r="AI60" s="68" t="s">
         <v>3</v>
       </c>
@@ -34235,11 +34235,11 @@
       <c r="J68" s="68"/>
       <c r="X68" s="15"/>
       <c r="Y68" s="15"/>
-      <c r="Z68" s="72" t="s">
+      <c r="Z68" s="73" t="s">
         <v>69</v>
       </c>
-      <c r="AA68" s="72"/>
-      <c r="AB68" s="72"/>
+      <c r="AA68" s="73"/>
+      <c r="AB68" s="73"/>
       <c r="AD68" s="34" t="s">
         <v>71</v>
       </c>
@@ -34445,17 +34445,17 @@
       <c r="W73" s="15"/>
       <c r="X73" s="15"/>
       <c r="Y73" s="15"/>
-      <c r="Z73" s="69" t="s">
+      <c r="Z73" s="75" t="s">
         <v>30</v>
       </c>
-      <c r="AA73" s="69"/>
-      <c r="AI73" s="73" t="s">
+      <c r="AA73" s="75"/>
+      <c r="AI73" s="76" t="s">
         <v>52</v>
       </c>
-      <c r="AJ73" s="73"/>
+      <c r="AJ73" s="76"/>
       <c r="AK73" s="31"/>
-      <c r="AL73" s="73"/>
-      <c r="AM73" s="73"/>
+      <c r="AL73" s="76"/>
+      <c r="AM73" s="76"/>
       <c r="AN73" s="31"/>
       <c r="AO73" s="31"/>
       <c r="AP73" s="31"/>
@@ -34779,29 +34779,29 @@
       <c r="AC77" s="41" t="s">
         <v>53</v>
       </c>
-      <c r="AI77" s="75" t="s">
+      <c r="AI77" s="72" t="s">
         <v>64</v>
       </c>
-      <c r="AJ77" s="75"/>
+      <c r="AJ77" s="72"/>
       <c r="AK77" s="29"/>
-      <c r="AL77" s="75"/>
-      <c r="AM77" s="75"/>
+      <c r="AL77" s="72"/>
+      <c r="AM77" s="72"/>
       <c r="AN77" s="29"/>
       <c r="AO77" s="31"/>
       <c r="AP77" s="31"/>
       <c r="AQ77" s="31"/>
       <c r="AR77" s="31"/>
       <c r="AS77" s="31"/>
-      <c r="AT77" s="75" t="s">
+      <c r="AT77" s="72" t="s">
         <v>65</v>
       </c>
-      <c r="AU77" s="75"/>
-      <c r="AV77" s="75"/>
-      <c r="AW77" s="75"/>
-      <c r="AX77" s="75"/>
-      <c r="AY77" s="75"/>
-      <c r="AZ77" s="75"/>
-      <c r="BA77" s="75"/>
+      <c r="AU77" s="72"/>
+      <c r="AV77" s="72"/>
+      <c r="AW77" s="72"/>
+      <c r="AX77" s="72"/>
+      <c r="AY77" s="72"/>
+      <c r="AZ77" s="72"/>
+      <c r="BA77" s="72"/>
     </row>
     <row r="78" spans="1:78">
       <c r="B78" s="1"/>
@@ -34901,16 +34901,16 @@
       </c>
     </row>
     <row r="81" spans="1:93" ht="16" customHeight="1">
-      <c r="C81" s="76" t="s">
+      <c r="C81" s="69" t="s">
         <v>85</v>
       </c>
-      <c r="D81" s="76"/>
-      <c r="E81" s="76"/>
-      <c r="F81" s="76"/>
-      <c r="G81" s="76"/>
-      <c r="H81" s="76"/>
-      <c r="I81" s="76"/>
-      <c r="J81" s="76"/>
+      <c r="D81" s="69"/>
+      <c r="E81" s="69"/>
+      <c r="F81" s="69"/>
+      <c r="G81" s="69"/>
+      <c r="H81" s="69"/>
+      <c r="I81" s="69"/>
+      <c r="J81" s="69"/>
       <c r="AI81" s="68" t="s">
         <v>4</v>
       </c>
@@ -36326,14 +36326,14 @@
       </c>
     </row>
     <row r="91" spans="1:93" ht="19">
-      <c r="L91" s="76" t="s">
+      <c r="L91" s="69" t="s">
         <v>13</v>
       </c>
-      <c r="M91" s="76"/>
-      <c r="N91" s="76"/>
-      <c r="O91" s="76"/>
-      <c r="P91" s="76"/>
-      <c r="Q91" s="76"/>
+      <c r="M91" s="69"/>
+      <c r="N91" s="69"/>
+      <c r="O91" s="69"/>
+      <c r="P91" s="69"/>
+      <c r="Q91" s="69"/>
       <c r="Z91" s="41" t="s">
         <v>11</v>
       </c>
@@ -36486,14 +36486,14 @@
       <c r="AA94" s="17"/>
     </row>
     <row r="95" spans="1:93" ht="20">
-      <c r="L95" s="76" t="s">
+      <c r="L95" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="M95" s="76"/>
-      <c r="N95" s="76"/>
-      <c r="O95" s="76"/>
-      <c r="P95" s="76"/>
-      <c r="Q95" s="76"/>
+      <c r="M95" s="69"/>
+      <c r="N95" s="69"/>
+      <c r="O95" s="69"/>
+      <c r="P95" s="69"/>
+      <c r="Q95" s="69"/>
     </row>
     <row r="98" spans="1:40" ht="47">
       <c r="A98" s="27" t="s">
@@ -37114,16 +37114,16 @@
       </c>
       <c r="D120" s="68"/>
       <c r="E120" s="68"/>
-      <c r="G120" s="76" t="s">
+      <c r="G120" s="69" t="s">
         <v>39</v>
       </c>
-      <c r="H120" s="76"/>
-      <c r="I120" s="76"/>
-      <c r="K120" s="76" t="s">
+      <c r="H120" s="69"/>
+      <c r="I120" s="69"/>
+      <c r="K120" s="69" t="s">
         <v>40</v>
       </c>
-      <c r="L120" s="76"/>
-      <c r="M120" s="76"/>
+      <c r="L120" s="69"/>
+      <c r="M120" s="69"/>
       <c r="N120" s="17"/>
       <c r="O120" s="17" t="s">
         <v>41</v>
@@ -37547,65 +37547,6 @@
     </row>
   </sheetData>
   <mergeCells count="71">
-    <mergeCell ref="A112:I112"/>
-    <mergeCell ref="C143:H143"/>
-    <mergeCell ref="C120:E120"/>
-    <mergeCell ref="G120:I120"/>
-    <mergeCell ref="K120:M120"/>
-    <mergeCell ref="A125:A130"/>
-    <mergeCell ref="C135:H135"/>
-    <mergeCell ref="A137:A142"/>
-    <mergeCell ref="A114:A119"/>
-    <mergeCell ref="BE81:BL81"/>
-    <mergeCell ref="BT81:BY81"/>
-    <mergeCell ref="A83:A90"/>
-    <mergeCell ref="L91:Q91"/>
-    <mergeCell ref="AI91:AP91"/>
-    <mergeCell ref="AT91:BA91"/>
-    <mergeCell ref="BE91:BL91"/>
-    <mergeCell ref="BT91:BY91"/>
-    <mergeCell ref="C81:J81"/>
-    <mergeCell ref="AI81:AP81"/>
-    <mergeCell ref="AT81:BA81"/>
-    <mergeCell ref="J92:J94"/>
-    <mergeCell ref="L95:Q95"/>
-    <mergeCell ref="A100:I100"/>
-    <mergeCell ref="A102:A109"/>
-    <mergeCell ref="C77:J77"/>
-    <mergeCell ref="AI77:AJ77"/>
-    <mergeCell ref="AL77:AM77"/>
-    <mergeCell ref="AT77:BA77"/>
-    <mergeCell ref="C79:J79"/>
-    <mergeCell ref="A75:A76"/>
-    <mergeCell ref="C68:J68"/>
-    <mergeCell ref="Z68:AB68"/>
-    <mergeCell ref="AI68:AN68"/>
-    <mergeCell ref="AT68:BA68"/>
-    <mergeCell ref="C70:J70"/>
-    <mergeCell ref="Z73:AA73"/>
-    <mergeCell ref="AI73:AJ73"/>
-    <mergeCell ref="AL73:AM73"/>
-    <mergeCell ref="AT73:BA73"/>
-    <mergeCell ref="BE68:BL68"/>
-    <mergeCell ref="BT68:BY68"/>
-    <mergeCell ref="Z60:AB60"/>
-    <mergeCell ref="AI60:AN60"/>
-    <mergeCell ref="AT60:BA60"/>
-    <mergeCell ref="BE60:BL60"/>
-    <mergeCell ref="BT60:BY60"/>
-    <mergeCell ref="A62:A67"/>
-    <mergeCell ref="BE50:BJ50"/>
-    <mergeCell ref="BT50:BY50"/>
-    <mergeCell ref="CA50:CH50"/>
-    <mergeCell ref="J51:J53"/>
-    <mergeCell ref="L54:Q54"/>
-    <mergeCell ref="L56:Q56"/>
-    <mergeCell ref="AT50:AY50"/>
-    <mergeCell ref="A42:A49"/>
-    <mergeCell ref="U42:U49"/>
-    <mergeCell ref="L50:Q50"/>
-    <mergeCell ref="W50:X50"/>
-    <mergeCell ref="AI50:AP50"/>
     <mergeCell ref="CJ40:CK40"/>
     <mergeCell ref="C26:E26"/>
     <mergeCell ref="A28:A35"/>
@@ -37618,6 +37559,65 @@
     <mergeCell ref="BE40:BJ40"/>
     <mergeCell ref="BT40:BY40"/>
     <mergeCell ref="CA40:CH40"/>
+    <mergeCell ref="A42:A49"/>
+    <mergeCell ref="U42:U49"/>
+    <mergeCell ref="L50:Q50"/>
+    <mergeCell ref="W50:X50"/>
+    <mergeCell ref="AI50:AP50"/>
+    <mergeCell ref="A62:A67"/>
+    <mergeCell ref="BE50:BJ50"/>
+    <mergeCell ref="BT50:BY50"/>
+    <mergeCell ref="CA50:CH50"/>
+    <mergeCell ref="J51:J53"/>
+    <mergeCell ref="L54:Q54"/>
+    <mergeCell ref="L56:Q56"/>
+    <mergeCell ref="AT50:AY50"/>
+    <mergeCell ref="BT68:BY68"/>
+    <mergeCell ref="Z60:AB60"/>
+    <mergeCell ref="AI60:AN60"/>
+    <mergeCell ref="AT60:BA60"/>
+    <mergeCell ref="BE60:BL60"/>
+    <mergeCell ref="BT60:BY60"/>
+    <mergeCell ref="Z73:AA73"/>
+    <mergeCell ref="AI73:AJ73"/>
+    <mergeCell ref="AL73:AM73"/>
+    <mergeCell ref="AT73:BA73"/>
+    <mergeCell ref="BE68:BL68"/>
+    <mergeCell ref="C68:J68"/>
+    <mergeCell ref="Z68:AB68"/>
+    <mergeCell ref="AI68:AN68"/>
+    <mergeCell ref="AT68:BA68"/>
+    <mergeCell ref="C70:J70"/>
+    <mergeCell ref="AI77:AJ77"/>
+    <mergeCell ref="AL77:AM77"/>
+    <mergeCell ref="AT77:BA77"/>
+    <mergeCell ref="C79:J79"/>
+    <mergeCell ref="A75:A76"/>
+    <mergeCell ref="J92:J94"/>
+    <mergeCell ref="L95:Q95"/>
+    <mergeCell ref="A100:I100"/>
+    <mergeCell ref="A102:A109"/>
+    <mergeCell ref="C77:J77"/>
+    <mergeCell ref="BE81:BL81"/>
+    <mergeCell ref="BT81:BY81"/>
+    <mergeCell ref="A83:A90"/>
+    <mergeCell ref="L91:Q91"/>
+    <mergeCell ref="AI91:AP91"/>
+    <mergeCell ref="AT91:BA91"/>
+    <mergeCell ref="BE91:BL91"/>
+    <mergeCell ref="BT91:BY91"/>
+    <mergeCell ref="C81:J81"/>
+    <mergeCell ref="AI81:AP81"/>
+    <mergeCell ref="AT81:BA81"/>
+    <mergeCell ref="A112:I112"/>
+    <mergeCell ref="C143:H143"/>
+    <mergeCell ref="C120:E120"/>
+    <mergeCell ref="G120:I120"/>
+    <mergeCell ref="K120:M120"/>
+    <mergeCell ref="A125:A130"/>
+    <mergeCell ref="C135:H135"/>
+    <mergeCell ref="A137:A142"/>
+    <mergeCell ref="A114:A119"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -37631,11 +37631,11 @@
   <dimension ref="A1:LO126"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C42" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="BI42" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A40" sqref="A40"/>
       <selection pane="topRight" activeCell="C40" sqref="C40"/>
       <selection pane="bottomLeft" activeCell="A42" sqref="A42"/>
-      <selection pane="bottomRight" activeCell="EI55" sqref="EI55"/>
+      <selection pane="bottomRight" activeCell="DX68" sqref="DX68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -38237,11 +38237,11 @@
     </row>
     <row r="26" spans="1:278">
       <c r="B26" s="10"/>
-      <c r="C26" s="69" t="s">
+      <c r="C26" s="75" t="s">
         <v>30</v>
       </c>
-      <c r="D26" s="69"/>
-      <c r="E26" s="69"/>
+      <c r="D26" s="75"/>
+      <c r="E26" s="75"/>
       <c r="F26" s="47"/>
       <c r="G26" s="47"/>
       <c r="CQ26" t="s">
@@ -38500,11 +38500,11 @@
       <c r="CJ35" s="31"/>
     </row>
     <row r="36" spans="1:302" ht="18">
-      <c r="C36" s="69" t="s">
+      <c r="C36" s="75" t="s">
         <v>31</v>
       </c>
-      <c r="D36" s="69"/>
-      <c r="E36" s="69"/>
+      <c r="D36" s="75"/>
+      <c r="E36" s="75"/>
       <c r="F36" s="47"/>
       <c r="G36" s="47"/>
       <c r="BL36" s="31"/>
@@ -38559,31 +38559,31 @@
       <c r="CJ37" s="51"/>
     </row>
     <row r="38" spans="1:302">
-      <c r="BL38" s="75"/>
-      <c r="BM38" s="75"/>
-      <c r="BN38" s="75"/>
-      <c r="BO38" s="75"/>
-      <c r="BP38" s="75"/>
-      <c r="BQ38" s="75"/>
-      <c r="BR38" s="75"/>
-      <c r="BS38" s="75"/>
-      <c r="BT38" s="75"/>
-      <c r="BU38" s="75"/>
-      <c r="BV38" s="75"/>
-      <c r="BW38" s="75"/>
-      <c r="BX38" s="75"/>
-      <c r="BY38" s="75"/>
-      <c r="BZ38" s="75"/>
-      <c r="CA38" s="75"/>
-      <c r="CB38" s="75"/>
-      <c r="CC38" s="75"/>
-      <c r="CD38" s="75"/>
-      <c r="CE38" s="75"/>
-      <c r="CF38" s="75"/>
-      <c r="CG38" s="75"/>
-      <c r="CH38" s="75"/>
-      <c r="CI38" s="75"/>
-      <c r="CJ38" s="75"/>
+      <c r="BL38" s="72"/>
+      <c r="BM38" s="72"/>
+      <c r="BN38" s="72"/>
+      <c r="BO38" s="72"/>
+      <c r="BP38" s="72"/>
+      <c r="BQ38" s="72"/>
+      <c r="BR38" s="72"/>
+      <c r="BS38" s="72"/>
+      <c r="BT38" s="72"/>
+      <c r="BU38" s="72"/>
+      <c r="BV38" s="72"/>
+      <c r="BW38" s="72"/>
+      <c r="BX38" s="72"/>
+      <c r="BY38" s="72"/>
+      <c r="BZ38" s="72"/>
+      <c r="CA38" s="72"/>
+      <c r="CB38" s="72"/>
+      <c r="CC38" s="72"/>
+      <c r="CD38" s="72"/>
+      <c r="CE38" s="72"/>
+      <c r="CF38" s="72"/>
+      <c r="CG38" s="72"/>
+      <c r="CH38" s="72"/>
+      <c r="CI38" s="72"/>
+      <c r="CJ38" s="72"/>
     </row>
     <row r="40" spans="1:302">
       <c r="C40" s="68" t="s">
@@ -38729,8 +38729,8 @@
       <c r="JC40" s="68"/>
       <c r="JD40" s="68"/>
       <c r="JE40" s="68"/>
-      <c r="JL40" s="75"/>
-      <c r="JM40" s="75"/>
+      <c r="JL40" s="72"/>
+      <c r="JM40" s="72"/>
       <c r="KI40" s="68" t="s">
         <v>3</v>
       </c>
@@ -42414,14 +42414,14 @@
       <c r="EB50" s="58"/>
       <c r="EC50" s="58"/>
       <c r="ED50" s="58"/>
-      <c r="EE50" s="78" t="s">
+      <c r="EE50" s="79" t="s">
         <v>193</v>
       </c>
-      <c r="EF50" s="78"/>
-      <c r="EG50" s="78"/>
-      <c r="EH50" s="78"/>
-      <c r="EI50" s="78"/>
-      <c r="EJ50" s="78"/>
+      <c r="EF50" s="79"/>
+      <c r="EG50" s="79"/>
+      <c r="EH50" s="79"/>
+      <c r="EI50" s="79"/>
+      <c r="EJ50" s="79"/>
       <c r="EK50" s="58"/>
       <c r="EL50" s="58"/>
       <c r="EM50" s="58"/>
@@ -42463,14 +42463,14 @@
       <c r="HD50" s="58"/>
       <c r="HE50" s="58"/>
       <c r="HF50" s="58"/>
-      <c r="HG50" s="78" t="s">
+      <c r="HG50" s="79" t="s">
         <v>192</v>
       </c>
-      <c r="HH50" s="78"/>
-      <c r="HI50" s="78"/>
-      <c r="HJ50" s="78"/>
-      <c r="HK50" s="78"/>
-      <c r="HL50" s="78"/>
+      <c r="HH50" s="79"/>
+      <c r="HI50" s="79"/>
+      <c r="HJ50" s="79"/>
+      <c r="HK50" s="79"/>
+      <c r="HL50" s="79"/>
       <c r="HM50" s="58"/>
       <c r="HN50" s="58"/>
       <c r="HO50" s="58"/>
@@ -42483,15 +42483,15 @@
       <c r="IS50" s="8"/>
       <c r="IT50" s="8"/>
       <c r="IV50" s="31"/>
-      <c r="IW50" s="75"/>
-      <c r="IX50" s="75"/>
+      <c r="IW50" s="72"/>
+      <c r="IX50" s="72"/>
       <c r="IY50" s="31"/>
-      <c r="IZ50" s="78"/>
-      <c r="JA50" s="78"/>
-      <c r="JB50" s="78"/>
-      <c r="JC50" s="78"/>
-      <c r="JD50" s="78"/>
-      <c r="JE50" s="78"/>
+      <c r="IZ50" s="79"/>
+      <c r="JA50" s="79"/>
+      <c r="JB50" s="79"/>
+      <c r="JC50" s="79"/>
+      <c r="JD50" s="79"/>
+      <c r="JE50" s="79"/>
       <c r="JF50" s="31"/>
       <c r="JG50" s="55"/>
       <c r="JH50" s="31"/>
@@ -42505,14 +42505,14 @@
       <c r="KF50" s="58"/>
       <c r="KG50" s="58"/>
       <c r="KH50" s="58"/>
-      <c r="KI50" s="78" t="s">
+      <c r="KI50" s="79" t="s">
         <v>133</v>
       </c>
-      <c r="KJ50" s="78"/>
-      <c r="KK50" s="78"/>
-      <c r="KL50" s="78"/>
-      <c r="KM50" s="78"/>
-      <c r="KN50" s="78"/>
+      <c r="KJ50" s="79"/>
+      <c r="KK50" s="79"/>
+      <c r="KL50" s="79"/>
+      <c r="KM50" s="79"/>
+      <c r="KN50" s="79"/>
       <c r="KO50" s="58"/>
       <c r="KP50" s="59" t="s">
         <v>12</v>
@@ -42827,14 +42827,14 @@
     </row>
     <row r="54" spans="1:319" ht="20">
       <c r="B54" s="1"/>
-      <c r="L54" s="72" t="s">
+      <c r="L54" s="73" t="s">
         <v>42</v>
       </c>
-      <c r="M54" s="72"/>
-      <c r="N54" s="72"/>
-      <c r="O54" s="72"/>
-      <c r="P54" s="72"/>
-      <c r="Q54" s="72"/>
+      <c r="M54" s="73"/>
+      <c r="N54" s="73"/>
+      <c r="O54" s="73"/>
+      <c r="P54" s="73"/>
+      <c r="Q54" s="73"/>
       <c r="R54" s="15"/>
       <c r="S54" s="15"/>
       <c r="T54" s="15"/>
@@ -42862,14 +42862,14 @@
       <c r="JJ54" s="31"/>
       <c r="JK54" s="31"/>
       <c r="JL54" s="31"/>
-      <c r="KI54" s="72" t="s">
+      <c r="KI54" s="73" t="s">
         <v>148</v>
       </c>
-      <c r="KJ54" s="72"/>
-      <c r="KK54" s="72"/>
-      <c r="KL54" s="72"/>
-      <c r="KM54" s="72"/>
-      <c r="KN54" s="72"/>
+      <c r="KJ54" s="73"/>
+      <c r="KK54" s="73"/>
+      <c r="KL54" s="73"/>
+      <c r="KM54" s="73"/>
+      <c r="KN54" s="73"/>
     </row>
     <row r="55" spans="1:319">
       <c r="B55" s="1"/>
@@ -43013,18 +43013,18 @@
       <c r="W58" s="15"/>
       <c r="X58" s="15"/>
       <c r="Y58" s="15"/>
-      <c r="Z58" s="69" t="s">
+      <c r="Z58" s="75" t="s">
         <v>30</v>
       </c>
-      <c r="AA58" s="69"/>
-      <c r="AB58" s="69"/>
-      <c r="AH58" s="73" t="s">
+      <c r="AA58" s="75"/>
+      <c r="AB58" s="75"/>
+      <c r="AH58" s="76" t="s">
         <v>52</v>
       </c>
-      <c r="AI58" s="73"/>
+      <c r="AI58" s="76"/>
       <c r="AJ58" s="31"/>
-      <c r="AK58" s="73"/>
-      <c r="AL58" s="73"/>
+      <c r="AK58" s="76"/>
+      <c r="AL58" s="76"/>
       <c r="AM58" s="31"/>
       <c r="AN58" s="31"/>
       <c r="AO58" s="31"/>
@@ -43350,37 +43350,37 @@
       <c r="W62" s="15"/>
       <c r="X62" s="15"/>
       <c r="Y62" s="15"/>
-      <c r="Z62" s="75" t="s">
+      <c r="Z62" s="72" t="s">
         <v>95</v>
       </c>
-      <c r="AA62" s="75"/>
-      <c r="AB62" s="75"/>
+      <c r="AA62" s="72"/>
+      <c r="AB62" s="72"/>
       <c r="AD62" s="45" t="s">
         <v>53</v>
       </c>
-      <c r="AH62" s="75" t="s">
+      <c r="AH62" s="72" t="s">
         <v>64</v>
       </c>
-      <c r="AI62" s="75"/>
+      <c r="AI62" s="72"/>
       <c r="AJ62" s="29"/>
-      <c r="AK62" s="75"/>
-      <c r="AL62" s="75"/>
+      <c r="AK62" s="72"/>
+      <c r="AL62" s="72"/>
       <c r="AM62" s="29"/>
       <c r="AN62" s="31"/>
       <c r="AO62" s="31"/>
       <c r="AP62" s="31"/>
       <c r="AQ62" s="31"/>
       <c r="AR62" s="31"/>
-      <c r="AS62" s="75" t="s">
+      <c r="AS62" s="72" t="s">
         <v>65</v>
       </c>
-      <c r="AT62" s="75"/>
-      <c r="AU62" s="75"/>
-      <c r="AV62" s="75"/>
-      <c r="AW62" s="75"/>
-      <c r="AX62" s="75"/>
-      <c r="AY62" s="75"/>
-      <c r="AZ62" s="75"/>
+      <c r="AT62" s="72"/>
+      <c r="AU62" s="72"/>
+      <c r="AV62" s="72"/>
+      <c r="AW62" s="72"/>
+      <c r="AX62" s="72"/>
+      <c r="AY62" s="72"/>
+      <c r="AZ62" s="72"/>
       <c r="ES62" s="31"/>
       <c r="ET62" s="31"/>
       <c r="EU62" s="31"/>
@@ -43523,11 +43523,11 @@
       <c r="H64" s="68"/>
       <c r="I64" s="68"/>
       <c r="J64" s="68"/>
-      <c r="Z64" s="69" t="s">
+      <c r="Z64" s="75" t="s">
         <v>30</v>
       </c>
-      <c r="AA64" s="69"/>
-      <c r="AB64" s="69"/>
+      <c r="AA64" s="75"/>
+      <c r="AB64" s="75"/>
       <c r="AH64" s="68" t="s">
         <v>3</v>
       </c>
@@ -43586,14 +43586,14 @@
       <c r="EC64" s="45"/>
       <c r="ES64" s="31"/>
       <c r="ET64" s="31"/>
-      <c r="EU64" s="75"/>
-      <c r="EV64" s="75"/>
-      <c r="EW64" s="75"/>
-      <c r="EX64" s="75"/>
-      <c r="EY64" s="75"/>
-      <c r="EZ64" s="75"/>
-      <c r="FA64" s="75"/>
-      <c r="FB64" s="75"/>
+      <c r="EU64" s="72"/>
+      <c r="EV64" s="72"/>
+      <c r="EW64" s="72"/>
+      <c r="EX64" s="72"/>
+      <c r="EY64" s="72"/>
+      <c r="EZ64" s="72"/>
+      <c r="FA64" s="72"/>
+      <c r="FB64" s="72"/>
       <c r="FC64" s="31"/>
       <c r="GM64" s="68" t="s">
         <v>3</v>
@@ -43617,26 +43617,26 @@
       <c r="HE64" s="52"/>
       <c r="HU64" s="31"/>
       <c r="HV64" s="31"/>
-      <c r="HW64" s="75"/>
-      <c r="HX64" s="75"/>
-      <c r="HY64" s="75"/>
-      <c r="HZ64" s="75"/>
-      <c r="IA64" s="75"/>
-      <c r="IB64" s="75"/>
-      <c r="IC64" s="75"/>
-      <c r="ID64" s="75"/>
+      <c r="HW64" s="72"/>
+      <c r="HX64" s="72"/>
+      <c r="HY64" s="72"/>
+      <c r="HZ64" s="72"/>
+      <c r="IA64" s="72"/>
+      <c r="IB64" s="72"/>
+      <c r="IC64" s="72"/>
+      <c r="ID64" s="72"/>
       <c r="IE64" s="31"/>
       <c r="JJ64" s="31"/>
       <c r="JK64" s="31"/>
       <c r="JL64" s="31"/>
       <c r="JM64" s="31"/>
       <c r="JN64" s="31"/>
-      <c r="JO64" s="75"/>
-      <c r="JP64" s="75"/>
-      <c r="JQ64" s="75"/>
-      <c r="JR64" s="75"/>
-      <c r="JS64" s="75"/>
-      <c r="JT64" s="75"/>
+      <c r="JO64" s="72"/>
+      <c r="JP64" s="72"/>
+      <c r="JQ64" s="72"/>
+      <c r="JR64" s="72"/>
+      <c r="JS64" s="72"/>
+      <c r="JT64" s="72"/>
       <c r="JU64" s="31"/>
       <c r="JX64" s="68" t="s">
         <v>4</v>
@@ -43650,21 +43650,21 @@
       <c r="KE64" s="68"/>
       <c r="KF64" s="52"/>
       <c r="KG64" s="52"/>
-      <c r="KP64" s="69" t="s">
+      <c r="KP64" s="75" t="s">
         <v>30</v>
       </c>
-      <c r="KQ64" s="69"/>
-      <c r="KR64" s="69"/>
+      <c r="KQ64" s="75"/>
+      <c r="KR64" s="75"/>
       <c r="KW64" s="31"/>
       <c r="KX64" s="31"/>
-      <c r="KY64" s="75"/>
-      <c r="KZ64" s="75"/>
-      <c r="LA64" s="75"/>
-      <c r="LB64" s="75"/>
-      <c r="LC64" s="75"/>
-      <c r="LD64" s="75"/>
-      <c r="LE64" s="75"/>
-      <c r="LF64" s="75"/>
+      <c r="KY64" s="72"/>
+      <c r="KZ64" s="72"/>
+      <c r="LA64" s="72"/>
+      <c r="LB64" s="72"/>
+      <c r="LC64" s="72"/>
+      <c r="LD64" s="72"/>
+      <c r="LE64" s="72"/>
+      <c r="LF64" s="72"/>
       <c r="LG64" s="31"/>
     </row>
     <row r="65" spans="1:327" ht="51" customHeight="1">
@@ -44568,14 +44568,14 @@
       <c r="EC67" s="50"/>
       <c r="ES67" s="31"/>
       <c r="ET67" s="31"/>
-      <c r="EU67" s="72"/>
-      <c r="EV67" s="72"/>
-      <c r="EW67" s="72"/>
-      <c r="EX67" s="72"/>
-      <c r="EY67" s="72"/>
-      <c r="EZ67" s="72"/>
-      <c r="FA67" s="72"/>
-      <c r="FB67" s="72"/>
+      <c r="EU67" s="73"/>
+      <c r="EV67" s="73"/>
+      <c r="EW67" s="73"/>
+      <c r="EX67" s="73"/>
+      <c r="EY67" s="73"/>
+      <c r="EZ67" s="73"/>
+      <c r="FA67" s="73"/>
+      <c r="FB67" s="73"/>
       <c r="FC67" s="31"/>
       <c r="GH67" s="70"/>
       <c r="GI67" s="1" t="s">
@@ -44645,14 +44645,14 @@
       <c r="HE67" s="51"/>
       <c r="HU67" s="31"/>
       <c r="HV67" s="31"/>
-      <c r="HW67" s="72"/>
-      <c r="HX67" s="72"/>
-      <c r="HY67" s="72"/>
-      <c r="HZ67" s="72"/>
-      <c r="IA67" s="72"/>
-      <c r="IB67" s="72"/>
-      <c r="IC67" s="72"/>
-      <c r="ID67" s="72"/>
+      <c r="HW67" s="73"/>
+      <c r="HX67" s="73"/>
+      <c r="HY67" s="73"/>
+      <c r="HZ67" s="73"/>
+      <c r="IA67" s="73"/>
+      <c r="IB67" s="73"/>
+      <c r="IC67" s="73"/>
+      <c r="ID67" s="73"/>
       <c r="IE67" s="31"/>
       <c r="JJ67" s="77"/>
       <c r="JK67" s="63"/>
@@ -44722,14 +44722,14 @@
       </c>
       <c r="KW67" s="31"/>
       <c r="KX67" s="31"/>
-      <c r="KY67" s="72"/>
-      <c r="KZ67" s="72"/>
-      <c r="LA67" s="72"/>
-      <c r="LB67" s="72"/>
-      <c r="LC67" s="72"/>
-      <c r="LD67" s="72"/>
-      <c r="LE67" s="72"/>
-      <c r="LF67" s="72"/>
+      <c r="KY67" s="73"/>
+      <c r="KZ67" s="73"/>
+      <c r="LA67" s="73"/>
+      <c r="LB67" s="73"/>
+      <c r="LC67" s="73"/>
+      <c r="LD67" s="73"/>
+      <c r="LE67" s="73"/>
+      <c r="LF67" s="73"/>
       <c r="LG67" s="31"/>
     </row>
     <row r="68" spans="1:327">
@@ -46326,11 +46326,11 @@
       <c r="J72" s="68"/>
       <c r="X72" s="15"/>
       <c r="Y72" s="15"/>
-      <c r="Z72" s="72" t="s">
+      <c r="Z72" s="73" t="s">
         <v>96</v>
       </c>
-      <c r="AA72" s="72"/>
-      <c r="AB72" s="72"/>
+      <c r="AA72" s="73"/>
+      <c r="AB72" s="73"/>
       <c r="AD72" s="45" t="s">
         <v>34</v>
       </c>
@@ -46545,23 +46545,23 @@
       <c r="JL72" s="55"/>
       <c r="JM72" s="31"/>
       <c r="JN72" s="31"/>
-      <c r="JO72" s="75"/>
-      <c r="JP72" s="75"/>
-      <c r="JQ72" s="75"/>
-      <c r="JR72" s="75"/>
-      <c r="JS72" s="75"/>
-      <c r="JT72" s="75"/>
+      <c r="JO72" s="72"/>
+      <c r="JP72" s="72"/>
+      <c r="JQ72" s="72"/>
+      <c r="JR72" s="72"/>
+      <c r="JS72" s="72"/>
+      <c r="JT72" s="72"/>
       <c r="JU72" s="31"/>
-      <c r="JX72" s="79" t="s">
+      <c r="JX72" s="78" t="s">
         <v>134</v>
       </c>
-      <c r="JY72" s="79"/>
-      <c r="JZ72" s="79"/>
-      <c r="KA72" s="79"/>
-      <c r="KB72" s="79"/>
-      <c r="KC72" s="79"/>
-      <c r="KD72" s="79"/>
-      <c r="KE72" s="79"/>
+      <c r="JY72" s="78"/>
+      <c r="JZ72" s="78"/>
+      <c r="KA72" s="78"/>
+      <c r="KB72" s="78"/>
+      <c r="KC72" s="78"/>
+      <c r="KD72" s="78"/>
+      <c r="KE72" s="78"/>
       <c r="KF72" s="54"/>
       <c r="KG72" s="54"/>
       <c r="KH72" s="26"/>
@@ -46572,11 +46572,11 @@
       <c r="KM72" s="26"/>
       <c r="KN72" s="26"/>
       <c r="KO72" s="26"/>
-      <c r="KP72" s="72" t="s">
+      <c r="KP72" s="73" t="s">
         <v>142</v>
       </c>
-      <c r="KQ72" s="72"/>
-      <c r="KR72" s="72"/>
+      <c r="KQ72" s="73"/>
+      <c r="KR72" s="73"/>
       <c r="KS72" s="26"/>
       <c r="KT72" s="52" t="s">
         <v>145</v>
@@ -48670,16 +48670,16 @@
       <c r="FA80" s="29"/>
       <c r="FB80" s="29"/>
       <c r="FC80" s="31"/>
-      <c r="FD80" s="76" t="s">
+      <c r="FD80" s="69" t="s">
         <v>119</v>
       </c>
-      <c r="FE80" s="76"/>
-      <c r="FF80" s="76"/>
-      <c r="FG80" s="76"/>
-      <c r="FH80" s="76"/>
-      <c r="FI80" s="76"/>
-      <c r="FJ80" s="76"/>
-      <c r="FK80" s="76"/>
+      <c r="FE80" s="69"/>
+      <c r="FF80" s="69"/>
+      <c r="FG80" s="69"/>
+      <c r="FH80" s="69"/>
+      <c r="FI80" s="69"/>
+      <c r="FJ80" s="69"/>
+      <c r="FK80" s="69"/>
       <c r="GH80" s="70"/>
       <c r="GI80" s="1" t="s">
         <v>27</v>
@@ -48791,16 +48791,16 @@
       <c r="IC80" s="29"/>
       <c r="ID80" s="29"/>
       <c r="IE80" s="31"/>
-      <c r="IF80" s="76" t="s">
+      <c r="IF80" s="69" t="s">
         <v>130</v>
       </c>
-      <c r="IG80" s="76"/>
-      <c r="IH80" s="76"/>
-      <c r="II80" s="76"/>
-      <c r="IJ80" s="76"/>
-      <c r="IK80" s="76"/>
-      <c r="IL80" s="76"/>
-      <c r="IM80" s="76"/>
+      <c r="IG80" s="69"/>
+      <c r="IH80" s="69"/>
+      <c r="II80" s="69"/>
+      <c r="IJ80" s="69"/>
+      <c r="IK80" s="69"/>
+      <c r="IL80" s="69"/>
+      <c r="IM80" s="69"/>
       <c r="JJ80" s="77"/>
       <c r="JK80" s="63"/>
       <c r="JL80" s="51"/>
@@ -48887,16 +48887,16 @@
       <c r="LE80" s="29"/>
       <c r="LF80" s="29"/>
       <c r="LG80" s="31"/>
-      <c r="LH80" s="76" t="s">
+      <c r="LH80" s="69" t="s">
         <v>139</v>
       </c>
-      <c r="LI80" s="76"/>
-      <c r="LJ80" s="76"/>
-      <c r="LK80" s="76"/>
-      <c r="LL80" s="76"/>
-      <c r="LM80" s="76"/>
-      <c r="LN80" s="76"/>
-      <c r="LO80" s="76"/>
+      <c r="LI80" s="69"/>
+      <c r="LJ80" s="69"/>
+      <c r="LK80" s="69"/>
+      <c r="LL80" s="69"/>
+      <c r="LM80" s="69"/>
+      <c r="LN80" s="69"/>
+      <c r="LO80" s="69"/>
     </row>
     <row r="81" spans="1:327">
       <c r="A81" s="70"/>
@@ -49865,16 +49865,16 @@
       <c r="LE82" s="31"/>
       <c r="LF82" s="31"/>
       <c r="LG82" s="31"/>
-      <c r="LH82" s="76" t="s">
+      <c r="LH82" s="69" t="s">
         <v>140</v>
       </c>
-      <c r="LI82" s="76"/>
-      <c r="LJ82" s="76"/>
-      <c r="LK82" s="76"/>
-      <c r="LL82" s="76"/>
-      <c r="LM82" s="76"/>
-      <c r="LN82" s="76"/>
-      <c r="LO82" s="76"/>
+      <c r="LI82" s="69"/>
+      <c r="LJ82" s="69"/>
+      <c r="LK82" s="69"/>
+      <c r="LL82" s="69"/>
+      <c r="LM82" s="69"/>
+      <c r="LN82" s="69"/>
+      <c r="LO82" s="69"/>
     </row>
     <row r="83" spans="1:327">
       <c r="A83" s="70"/>
@@ -51281,14 +51281,14 @@
       <c r="LG85" s="31"/>
     </row>
     <row r="86" spans="1:327" ht="20">
-      <c r="L86" s="76" t="s">
+      <c r="L86" s="69" t="s">
         <v>13</v>
       </c>
-      <c r="M86" s="76"/>
-      <c r="N86" s="76"/>
-      <c r="O86" s="76"/>
-      <c r="P86" s="76"/>
-      <c r="Q86" s="76"/>
+      <c r="M86" s="69"/>
+      <c r="N86" s="69"/>
+      <c r="O86" s="69"/>
+      <c r="P86" s="69"/>
+      <c r="Q86" s="69"/>
       <c r="Z86" s="45" t="s">
         <v>11</v>
       </c>
@@ -51394,30 +51394,30 @@
       <c r="EB86" s="8"/>
       <c r="EC86" s="8"/>
       <c r="ED86" s="8"/>
-      <c r="EE86" s="76" t="s">
+      <c r="EE86" s="69" t="s">
         <v>114</v>
       </c>
-      <c r="EF86" s="76"/>
-      <c r="EG86" s="76"/>
-      <c r="EH86" s="76"/>
-      <c r="EI86" s="76"/>
-      <c r="EJ86" s="76"/>
+      <c r="EF86" s="69"/>
+      <c r="EG86" s="69"/>
+      <c r="EH86" s="69"/>
+      <c r="EI86" s="69"/>
+      <c r="EJ86" s="69"/>
       <c r="EM86" s="45" t="s">
         <v>116</v>
       </c>
       <c r="EO86" s="48" t="s">
         <v>117</v>
       </c>
-      <c r="ER86" s="76" t="s">
+      <c r="ER86" s="69" t="s">
         <v>118</v>
       </c>
-      <c r="ES86" s="76"/>
-      <c r="ET86" s="76"/>
-      <c r="EU86" s="76"/>
-      <c r="EV86" s="76"/>
-      <c r="EW86" s="76"/>
-      <c r="EX86" s="76"/>
-      <c r="EY86" s="76"/>
+      <c r="ES86" s="69"/>
+      <c r="ET86" s="69"/>
+      <c r="EU86" s="69"/>
+      <c r="EV86" s="69"/>
+      <c r="EW86" s="69"/>
+      <c r="EX86" s="69"/>
+      <c r="EY86" s="69"/>
       <c r="FO86" s="57"/>
       <c r="FP86" s="8"/>
       <c r="FQ86" s="8"/>
@@ -51462,30 +51462,30 @@
       <c r="HD86" s="8"/>
       <c r="HE86" s="8"/>
       <c r="HF86" s="8"/>
-      <c r="HG86" s="76" t="s">
+      <c r="HG86" s="69" t="s">
         <v>125</v>
       </c>
-      <c r="HH86" s="76"/>
-      <c r="HI86" s="76"/>
-      <c r="HJ86" s="76"/>
-      <c r="HK86" s="76"/>
-      <c r="HL86" s="76"/>
+      <c r="HH86" s="69"/>
+      <c r="HI86" s="69"/>
+      <c r="HJ86" s="69"/>
+      <c r="HK86" s="69"/>
+      <c r="HL86" s="69"/>
       <c r="HO86" s="52" t="s">
         <v>127</v>
       </c>
       <c r="HQ86" s="53" t="s">
         <v>128</v>
       </c>
-      <c r="HT86" s="76" t="s">
+      <c r="HT86" s="69" t="s">
         <v>129</v>
       </c>
-      <c r="HU86" s="76"/>
-      <c r="HV86" s="76"/>
-      <c r="HW86" s="76"/>
-      <c r="HX86" s="76"/>
-      <c r="HY86" s="76"/>
-      <c r="HZ86" s="76"/>
-      <c r="IA86" s="76"/>
+      <c r="HU86" s="69"/>
+      <c r="HV86" s="69"/>
+      <c r="HW86" s="69"/>
+      <c r="HX86" s="69"/>
+      <c r="HY86" s="69"/>
+      <c r="HZ86" s="69"/>
+      <c r="IA86" s="69"/>
       <c r="IQ86" s="57"/>
       <c r="IR86" s="8"/>
       <c r="IS86" s="8"/>
@@ -51510,14 +51510,14 @@
       <c r="JL86" s="55"/>
       <c r="JM86" s="31"/>
       <c r="JN86" s="31"/>
-      <c r="JO86" s="75"/>
-      <c r="JP86" s="75"/>
-      <c r="JQ86" s="75"/>
-      <c r="JR86" s="75"/>
-      <c r="JS86" s="75"/>
-      <c r="JT86" s="75"/>
-      <c r="JU86" s="75"/>
-      <c r="JV86" s="75"/>
+      <c r="JO86" s="72"/>
+      <c r="JP86" s="72"/>
+      <c r="JQ86" s="72"/>
+      <c r="JR86" s="72"/>
+      <c r="JS86" s="72"/>
+      <c r="JT86" s="72"/>
+      <c r="JU86" s="72"/>
+      <c r="JV86" s="72"/>
       <c r="JW86" s="29"/>
       <c r="JX86" s="29"/>
       <c r="JY86" s="8"/>
@@ -51530,30 +51530,30 @@
       <c r="KF86" s="8"/>
       <c r="KG86" s="8"/>
       <c r="KH86" s="8"/>
-      <c r="KI86" s="76" t="s">
+      <c r="KI86" s="69" t="s">
         <v>97</v>
       </c>
-      <c r="KJ86" s="76"/>
-      <c r="KK86" s="76"/>
-      <c r="KL86" s="76"/>
-      <c r="KM86" s="76"/>
-      <c r="KN86" s="76"/>
+      <c r="KJ86" s="69"/>
+      <c r="KK86" s="69"/>
+      <c r="KL86" s="69"/>
+      <c r="KM86" s="69"/>
+      <c r="KN86" s="69"/>
       <c r="KQ86" s="52" t="s">
         <v>98</v>
       </c>
       <c r="KS86" s="53" t="s">
         <v>135</v>
       </c>
-      <c r="KV86" s="76" t="s">
+      <c r="KV86" s="69" t="s">
         <v>136</v>
       </c>
-      <c r="KW86" s="76"/>
-      <c r="KX86" s="76"/>
-      <c r="KY86" s="76"/>
-      <c r="KZ86" s="76"/>
-      <c r="LA86" s="76"/>
-      <c r="LB86" s="76"/>
-      <c r="LC86" s="76"/>
+      <c r="KW86" s="69"/>
+      <c r="KX86" s="69"/>
+      <c r="KY86" s="69"/>
+      <c r="KZ86" s="69"/>
+      <c r="LA86" s="69"/>
+      <c r="LB86" s="69"/>
+      <c r="LC86" s="69"/>
     </row>
     <row r="87" spans="1:327" ht="16" customHeight="1">
       <c r="J87" s="70" t="s">
@@ -51923,22 +51923,22 @@
       </c>
     </row>
     <row r="90" spans="1:327" ht="20">
-      <c r="L90" s="76" t="s">
+      <c r="L90" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="M90" s="76"/>
-      <c r="N90" s="76"/>
-      <c r="O90" s="76"/>
-      <c r="P90" s="76"/>
-      <c r="Q90" s="76"/>
-      <c r="EE90" s="76" t="s">
+      <c r="M90" s="69"/>
+      <c r="N90" s="69"/>
+      <c r="O90" s="69"/>
+      <c r="P90" s="69"/>
+      <c r="Q90" s="69"/>
+      <c r="EE90" s="69" t="s">
         <v>115</v>
       </c>
-      <c r="EF90" s="76"/>
-      <c r="EG90" s="76"/>
-      <c r="EH90" s="76"/>
-      <c r="EI90" s="76"/>
-      <c r="EJ90" s="76"/>
+      <c r="EF90" s="69"/>
+      <c r="EG90" s="69"/>
+      <c r="EH90" s="69"/>
+      <c r="EI90" s="69"/>
+      <c r="EJ90" s="69"/>
       <c r="EM90" s="53" t="s">
         <v>137</v>
       </c>
@@ -51947,25 +51947,25 @@
       <c r="EP90" s="53"/>
       <c r="EQ90" s="53"/>
       <c r="ER90" s="53"/>
-      <c r="HG90" s="76" t="s">
+      <c r="HG90" s="69" t="s">
         <v>126</v>
       </c>
-      <c r="HH90" s="76"/>
-      <c r="HI90" s="76"/>
-      <c r="HJ90" s="76"/>
-      <c r="HK90" s="76"/>
-      <c r="HL90" s="76"/>
+      <c r="HH90" s="69"/>
+      <c r="HI90" s="69"/>
+      <c r="HJ90" s="69"/>
+      <c r="HK90" s="69"/>
+      <c r="HL90" s="69"/>
       <c r="HO90" s="53" t="s">
         <v>138</v>
       </c>
-      <c r="KI90" s="76" t="s">
+      <c r="KI90" s="69" t="s">
         <v>99</v>
       </c>
-      <c r="KJ90" s="76"/>
-      <c r="KK90" s="76"/>
-      <c r="KL90" s="76"/>
-      <c r="KM90" s="76"/>
-      <c r="KN90" s="76"/>
+      <c r="KJ90" s="69"/>
+      <c r="KK90" s="69"/>
+      <c r="KL90" s="69"/>
+      <c r="KM90" s="69"/>
+      <c r="KN90" s="69"/>
     </row>
     <row r="93" spans="1:327" ht="47">
       <c r="A93" s="27" t="s">
@@ -53181,17 +53181,17 @@
       </c>
       <c r="D115" s="68"/>
       <c r="E115" s="68"/>
-      <c r="G115" s="76" t="s">
+      <c r="G115" s="69" t="s">
         <v>39</v>
       </c>
-      <c r="H115" s="76"/>
-      <c r="I115" s="76"/>
+      <c r="H115" s="69"/>
+      <c r="I115" s="69"/>
       <c r="J115" s="17"/>
-      <c r="K115" s="76" t="s">
+      <c r="K115" s="69" t="s">
         <v>40</v>
       </c>
-      <c r="L115" s="76"/>
-      <c r="M115" s="76"/>
+      <c r="L115" s="69"/>
+      <c r="M115" s="69"/>
       <c r="N115" s="17"/>
       <c r="O115" s="17" t="s">
         <v>41</v>
@@ -53206,17 +53206,17 @@
       </c>
       <c r="JZ115" s="68"/>
       <c r="KA115" s="68"/>
-      <c r="KC115" s="76" t="s">
+      <c r="KC115" s="69" t="s">
         <v>144</v>
       </c>
-      <c r="KD115" s="76"/>
-      <c r="KE115" s="76"/>
+      <c r="KD115" s="69"/>
+      <c r="KE115" s="69"/>
       <c r="KF115" s="17"/>
-      <c r="KG115" s="76" t="s">
+      <c r="KG115" s="69" t="s">
         <v>149</v>
       </c>
-      <c r="KH115" s="76"/>
-      <c r="KI115" s="76"/>
+      <c r="KH115" s="69"/>
+      <c r="KI115" s="69"/>
       <c r="KJ115" s="17"/>
       <c r="KK115" s="17" t="s">
         <v>150</v>
@@ -53495,114 +53495,47 @@
     </row>
   </sheetData>
   <mergeCells count="173">
-    <mergeCell ref="JW95:KE95"/>
-    <mergeCell ref="JW97:JW104"/>
-    <mergeCell ref="JW107:KE107"/>
-    <mergeCell ref="JW109:JW114"/>
-    <mergeCell ref="JY115:KA115"/>
-    <mergeCell ref="KC115:KE115"/>
-    <mergeCell ref="KG115:KI115"/>
-    <mergeCell ref="JW120:JW125"/>
-    <mergeCell ref="JJ78:JJ85"/>
-    <mergeCell ref="KG78:KG85"/>
-    <mergeCell ref="LF78:LF79"/>
-    <mergeCell ref="LH80:LO80"/>
-    <mergeCell ref="JO86:JV86"/>
-    <mergeCell ref="KI86:KN86"/>
-    <mergeCell ref="KV86:LC86"/>
-    <mergeCell ref="KG87:KG89"/>
-    <mergeCell ref="KI90:KN90"/>
-    <mergeCell ref="LH82:LO82"/>
-    <mergeCell ref="KY64:LF64"/>
-    <mergeCell ref="KP64:KR64"/>
-    <mergeCell ref="JJ66:JJ71"/>
-    <mergeCell ref="KY67:LF67"/>
-    <mergeCell ref="JO72:JT72"/>
-    <mergeCell ref="JX72:KE72"/>
-    <mergeCell ref="JO76:JV76"/>
-    <mergeCell ref="KI76:KN76"/>
-    <mergeCell ref="KV76:LC76"/>
-    <mergeCell ref="LH76:LO76"/>
-    <mergeCell ref="JV66:JV71"/>
-    <mergeCell ref="KP72:KR72"/>
-    <mergeCell ref="JL40:JM40"/>
-    <mergeCell ref="KI40:KN40"/>
-    <mergeCell ref="IU42:IU49"/>
-    <mergeCell ref="JJ42:JJ49"/>
-    <mergeCell ref="IW50:IX50"/>
-    <mergeCell ref="IZ50:JE50"/>
-    <mergeCell ref="KI50:KN50"/>
-    <mergeCell ref="JO64:JT64"/>
-    <mergeCell ref="JX64:KE64"/>
-    <mergeCell ref="KG42:KG49"/>
-    <mergeCell ref="KG51:KG53"/>
-    <mergeCell ref="KI54:KN54"/>
-    <mergeCell ref="KI56:KN56"/>
-    <mergeCell ref="ID78:ID79"/>
-    <mergeCell ref="IF80:IM80"/>
-    <mergeCell ref="GM86:GT86"/>
-    <mergeCell ref="HG86:HL86"/>
-    <mergeCell ref="HT86:IA86"/>
-    <mergeCell ref="HE87:HE89"/>
-    <mergeCell ref="HG90:HL90"/>
-    <mergeCell ref="IW40:IX40"/>
-    <mergeCell ref="IZ40:JE40"/>
-    <mergeCell ref="GJ40:GO40"/>
-    <mergeCell ref="GJ50:GO50"/>
-    <mergeCell ref="HW64:ID64"/>
-    <mergeCell ref="GM76:GT76"/>
-    <mergeCell ref="HG76:HL76"/>
-    <mergeCell ref="HT76:IA76"/>
-    <mergeCell ref="IF76:IM76"/>
-    <mergeCell ref="CV40:DA40"/>
-    <mergeCell ref="CV50:DA50"/>
-    <mergeCell ref="FU40:FV40"/>
-    <mergeCell ref="FX40:GC40"/>
-    <mergeCell ref="HG40:HL40"/>
-    <mergeCell ref="FS42:FS49"/>
-    <mergeCell ref="FU50:FV50"/>
-    <mergeCell ref="FX50:GC50"/>
-    <mergeCell ref="HG50:HL50"/>
-    <mergeCell ref="DH40:DM40"/>
-    <mergeCell ref="DH50:DM50"/>
-    <mergeCell ref="DK72:DP72"/>
-    <mergeCell ref="DT72:EA72"/>
-    <mergeCell ref="GM64:GR64"/>
-    <mergeCell ref="GV64:HC64"/>
-    <mergeCell ref="EE50:EJ50"/>
-    <mergeCell ref="AS58:AZ58"/>
-    <mergeCell ref="L50:Q50"/>
-    <mergeCell ref="W50:X50"/>
-    <mergeCell ref="A42:A49"/>
-    <mergeCell ref="U42:U49"/>
-    <mergeCell ref="GH66:GH71"/>
-    <mergeCell ref="HW67:ID67"/>
-    <mergeCell ref="GM72:GR72"/>
-    <mergeCell ref="GV72:HC72"/>
-    <mergeCell ref="CQ42:CQ49"/>
-    <mergeCell ref="DF42:DF49"/>
-    <mergeCell ref="A60:A61"/>
-    <mergeCell ref="C62:J62"/>
-    <mergeCell ref="Z62:AB62"/>
-    <mergeCell ref="AH62:AI62"/>
-    <mergeCell ref="AK62:AL62"/>
-    <mergeCell ref="AS62:AZ62"/>
-    <mergeCell ref="DT64:EA64"/>
-    <mergeCell ref="Z64:AB64"/>
-    <mergeCell ref="AH64:AM64"/>
-    <mergeCell ref="AS64:AZ64"/>
-    <mergeCell ref="BD64:BK64"/>
-    <mergeCell ref="AH50:AO50"/>
-    <mergeCell ref="AS50:AX50"/>
-    <mergeCell ref="BD50:BI50"/>
-    <mergeCell ref="CS50:CT50"/>
-    <mergeCell ref="BS50:BX50"/>
-    <mergeCell ref="BZ50:CG50"/>
-    <mergeCell ref="J51:J53"/>
-    <mergeCell ref="L54:Q54"/>
-    <mergeCell ref="Z58:AB58"/>
-    <mergeCell ref="AH58:AI58"/>
-    <mergeCell ref="AK58:AL58"/>
+    <mergeCell ref="GH78:GH85"/>
+    <mergeCell ref="HE78:HE85"/>
+    <mergeCell ref="A120:A125"/>
+    <mergeCell ref="A97:A104"/>
+    <mergeCell ref="A107:I107"/>
+    <mergeCell ref="A109:A114"/>
+    <mergeCell ref="C115:E115"/>
+    <mergeCell ref="G115:I115"/>
+    <mergeCell ref="K115:M115"/>
+    <mergeCell ref="ER86:EY86"/>
+    <mergeCell ref="J87:J89"/>
+    <mergeCell ref="EC87:EC89"/>
+    <mergeCell ref="L90:Q90"/>
+    <mergeCell ref="EE90:EJ90"/>
+    <mergeCell ref="A95:I95"/>
+    <mergeCell ref="L86:Q86"/>
+    <mergeCell ref="AH86:AO86"/>
+    <mergeCell ref="AS86:AZ86"/>
+    <mergeCell ref="BD86:BK86"/>
+    <mergeCell ref="DK86:DR86"/>
+    <mergeCell ref="EE86:EJ86"/>
+    <mergeCell ref="BS86:BX86"/>
+    <mergeCell ref="BS72:BX72"/>
+    <mergeCell ref="EE76:EJ76"/>
+    <mergeCell ref="ER76:EY76"/>
+    <mergeCell ref="FD76:FK76"/>
+    <mergeCell ref="A78:A85"/>
+    <mergeCell ref="DF78:DF85"/>
+    <mergeCell ref="EC78:EC85"/>
+    <mergeCell ref="FB78:FB79"/>
+    <mergeCell ref="FD80:FK80"/>
+    <mergeCell ref="AH76:AO76"/>
+    <mergeCell ref="AS76:AZ76"/>
+    <mergeCell ref="BD76:BK76"/>
+    <mergeCell ref="DK76:DR76"/>
+    <mergeCell ref="C72:J72"/>
+    <mergeCell ref="Z72:AB72"/>
+    <mergeCell ref="AH72:AM72"/>
+    <mergeCell ref="AS72:AZ72"/>
+    <mergeCell ref="BD72:BK72"/>
+    <mergeCell ref="BS76:BX76"/>
     <mergeCell ref="EU64:FB64"/>
     <mergeCell ref="A66:A71"/>
     <mergeCell ref="DF66:DF71"/>
@@ -53627,47 +53560,114 @@
     <mergeCell ref="CS40:CT40"/>
     <mergeCell ref="EE40:EJ40"/>
     <mergeCell ref="C64:J64"/>
-    <mergeCell ref="BS72:BX72"/>
-    <mergeCell ref="EE76:EJ76"/>
-    <mergeCell ref="ER76:EY76"/>
-    <mergeCell ref="FD76:FK76"/>
-    <mergeCell ref="A78:A85"/>
-    <mergeCell ref="DF78:DF85"/>
-    <mergeCell ref="EC78:EC85"/>
-    <mergeCell ref="FB78:FB79"/>
-    <mergeCell ref="FD80:FK80"/>
-    <mergeCell ref="AH76:AO76"/>
-    <mergeCell ref="AS76:AZ76"/>
-    <mergeCell ref="BD76:BK76"/>
-    <mergeCell ref="DK76:DR76"/>
-    <mergeCell ref="C72:J72"/>
-    <mergeCell ref="Z72:AB72"/>
-    <mergeCell ref="AH72:AM72"/>
-    <mergeCell ref="AS72:AZ72"/>
-    <mergeCell ref="BD72:BK72"/>
-    <mergeCell ref="BS76:BX76"/>
-    <mergeCell ref="GH78:GH85"/>
-    <mergeCell ref="HE78:HE85"/>
-    <mergeCell ref="A120:A125"/>
-    <mergeCell ref="A97:A104"/>
-    <mergeCell ref="A107:I107"/>
-    <mergeCell ref="A109:A114"/>
-    <mergeCell ref="C115:E115"/>
-    <mergeCell ref="G115:I115"/>
-    <mergeCell ref="K115:M115"/>
-    <mergeCell ref="ER86:EY86"/>
-    <mergeCell ref="J87:J89"/>
-    <mergeCell ref="EC87:EC89"/>
-    <mergeCell ref="L90:Q90"/>
-    <mergeCell ref="EE90:EJ90"/>
-    <mergeCell ref="A95:I95"/>
-    <mergeCell ref="L86:Q86"/>
-    <mergeCell ref="AH86:AO86"/>
-    <mergeCell ref="AS86:AZ86"/>
-    <mergeCell ref="BD86:BK86"/>
-    <mergeCell ref="DK86:DR86"/>
-    <mergeCell ref="EE86:EJ86"/>
-    <mergeCell ref="BS86:BX86"/>
+    <mergeCell ref="AS64:AZ64"/>
+    <mergeCell ref="BD64:BK64"/>
+    <mergeCell ref="AH50:AO50"/>
+    <mergeCell ref="AS50:AX50"/>
+    <mergeCell ref="BD50:BI50"/>
+    <mergeCell ref="CS50:CT50"/>
+    <mergeCell ref="BS50:BX50"/>
+    <mergeCell ref="BZ50:CG50"/>
+    <mergeCell ref="J51:J53"/>
+    <mergeCell ref="L54:Q54"/>
+    <mergeCell ref="Z58:AB58"/>
+    <mergeCell ref="AH58:AI58"/>
+    <mergeCell ref="AK58:AL58"/>
+    <mergeCell ref="DK72:DP72"/>
+    <mergeCell ref="DT72:EA72"/>
+    <mergeCell ref="GM64:GR64"/>
+    <mergeCell ref="GV64:HC64"/>
+    <mergeCell ref="EE50:EJ50"/>
+    <mergeCell ref="AS58:AZ58"/>
+    <mergeCell ref="L50:Q50"/>
+    <mergeCell ref="W50:X50"/>
+    <mergeCell ref="A42:A49"/>
+    <mergeCell ref="U42:U49"/>
+    <mergeCell ref="GH66:GH71"/>
+    <mergeCell ref="GM72:GR72"/>
+    <mergeCell ref="GV72:HC72"/>
+    <mergeCell ref="CQ42:CQ49"/>
+    <mergeCell ref="DF42:DF49"/>
+    <mergeCell ref="A60:A61"/>
+    <mergeCell ref="C62:J62"/>
+    <mergeCell ref="Z62:AB62"/>
+    <mergeCell ref="AH62:AI62"/>
+    <mergeCell ref="AK62:AL62"/>
+    <mergeCell ref="AS62:AZ62"/>
+    <mergeCell ref="DT64:EA64"/>
+    <mergeCell ref="Z64:AB64"/>
+    <mergeCell ref="AH64:AM64"/>
+    <mergeCell ref="CV40:DA40"/>
+    <mergeCell ref="CV50:DA50"/>
+    <mergeCell ref="FU40:FV40"/>
+    <mergeCell ref="FX40:GC40"/>
+    <mergeCell ref="HG40:HL40"/>
+    <mergeCell ref="FS42:FS49"/>
+    <mergeCell ref="FU50:FV50"/>
+    <mergeCell ref="FX50:GC50"/>
+    <mergeCell ref="HG50:HL50"/>
+    <mergeCell ref="DH40:DM40"/>
+    <mergeCell ref="DH50:DM50"/>
+    <mergeCell ref="ID78:ID79"/>
+    <mergeCell ref="IF80:IM80"/>
+    <mergeCell ref="GM86:GT86"/>
+    <mergeCell ref="HG86:HL86"/>
+    <mergeCell ref="HT86:IA86"/>
+    <mergeCell ref="HE87:HE89"/>
+    <mergeCell ref="HG90:HL90"/>
+    <mergeCell ref="IW40:IX40"/>
+    <mergeCell ref="IZ40:JE40"/>
+    <mergeCell ref="GJ40:GO40"/>
+    <mergeCell ref="GJ50:GO50"/>
+    <mergeCell ref="HW64:ID64"/>
+    <mergeCell ref="GM76:GT76"/>
+    <mergeCell ref="HG76:HL76"/>
+    <mergeCell ref="HT76:IA76"/>
+    <mergeCell ref="IF76:IM76"/>
+    <mergeCell ref="HW67:ID67"/>
+    <mergeCell ref="JL40:JM40"/>
+    <mergeCell ref="KI40:KN40"/>
+    <mergeCell ref="IU42:IU49"/>
+    <mergeCell ref="JJ42:JJ49"/>
+    <mergeCell ref="IW50:IX50"/>
+    <mergeCell ref="IZ50:JE50"/>
+    <mergeCell ref="KI50:KN50"/>
+    <mergeCell ref="JO64:JT64"/>
+    <mergeCell ref="JX64:KE64"/>
+    <mergeCell ref="KG42:KG49"/>
+    <mergeCell ref="KG51:KG53"/>
+    <mergeCell ref="KI54:KN54"/>
+    <mergeCell ref="KI56:KN56"/>
+    <mergeCell ref="JJ66:JJ71"/>
+    <mergeCell ref="KY67:LF67"/>
+    <mergeCell ref="JO72:JT72"/>
+    <mergeCell ref="JX72:KE72"/>
+    <mergeCell ref="JO76:JV76"/>
+    <mergeCell ref="KI76:KN76"/>
+    <mergeCell ref="KV76:LC76"/>
+    <mergeCell ref="LH76:LO76"/>
+    <mergeCell ref="JV66:JV71"/>
+    <mergeCell ref="KP72:KR72"/>
+    <mergeCell ref="LF78:LF79"/>
+    <mergeCell ref="LH80:LO80"/>
+    <mergeCell ref="JO86:JV86"/>
+    <mergeCell ref="KI86:KN86"/>
+    <mergeCell ref="KV86:LC86"/>
+    <mergeCell ref="KG87:KG89"/>
+    <mergeCell ref="KI90:KN90"/>
+    <mergeCell ref="LH82:LO82"/>
+    <mergeCell ref="KY64:LF64"/>
+    <mergeCell ref="KP64:KR64"/>
+    <mergeCell ref="JW95:KE95"/>
+    <mergeCell ref="JW97:JW104"/>
+    <mergeCell ref="JW107:KE107"/>
+    <mergeCell ref="JW109:JW114"/>
+    <mergeCell ref="JY115:KA115"/>
+    <mergeCell ref="KC115:KE115"/>
+    <mergeCell ref="KG115:KI115"/>
+    <mergeCell ref="JW120:JW125"/>
+    <mergeCell ref="JJ78:JJ85"/>
+    <mergeCell ref="KG78:KG85"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
Now includes perfect sub data in package.
</commit_message>
<xml_diff>
--- a/inst/extdata/PerfectSubstitutionraw/UTEI_Sankey_Simple_ECC_Perfect_Sub.xlsx
+++ b/inst/extdata/PerfectSubstitutionraw/UTEI_Sankey_Simple_ECC_Perfect_Sub.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mkh2/github/Recca/inst/extdata/PerfectSubstitutionraw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{386DAC91-4A8A-C349-A07F-63D9231C127A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89B8A3E8-598D-834E-BAC9-A087FDB82C51}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2600" yWindow="440" windowWidth="26200" windowHeight="17560" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30459,7 +30459,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{338BDA73-949D-6141-997A-6445BD9150B1}">
   <dimension ref="A1:CO144"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A23" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A74" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="W41" sqref="W41"/>
     </sheetView>
   </sheetViews>
@@ -37633,12 +37633,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{842438A8-D71C-B444-A99F-665ABEA366D5}">
   <dimension ref="A1:LO129"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C42" activePane="bottomRight" state="frozen"/>
-      <selection activeCell="A40" sqref="A40"/>
-      <selection pane="topRight" activeCell="C40" sqref="C40"/>
-      <selection pane="bottomLeft" activeCell="A42" sqref="A42"/>
-      <selection pane="bottomRight" activeCell="L55" sqref="L55"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A53" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L55" sqref="L55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>

</xml_diff>

<commit_message>
Working on downstream swim.
</commit_message>
<xml_diff>
--- a/inst/extdata/PerfectSubstitutionraw/UTEI_Sankey_Simple_ECC_Perfect_Sub.xlsx
+++ b/inst/extdata/PerfectSubstitutionraw/UTEI_Sankey_Simple_ECC_Perfect_Sub.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11014"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11109"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matt/github/Recca/inst/extdata/PerfectSubstitutionraw/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mkh2/github/Recca/inst/extdata/PerfectSubstitutionraw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D233B7BC-7BFF-9344-B83F-C45E11F3D6BB}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A39AC02-0FAA-C344-A179-FC0EFD04C3AB}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12800" yWindow="6640" windowWidth="26200" windowHeight="17560" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20680" yWindow="440" windowWidth="26200" windowHeight="17560" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Meta" sheetId="10" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="Perfect substitution" sheetId="9" r:id="rId3"/>
     <sheet name="PerfectSubstitutionRaw" sheetId="11" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
@@ -189,7 +189,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Gives fraction of total production of products (in rows) consumed by each industry (in rows). Rows should sum to 1 or zero.</t>
+          <t>Gives fraction of total production of products (in rows) consumed by each industry (in rows). Rows should sum to zero when all of the Product is consumed by final demand. Rows should sum to 1 when all of the Product is consumed in the intermediate industries. Rows should sum to something between 0 and 1 when some product is used by final demand and some product is used by intermediate industries.</t>
         </r>
       </text>
     </comment>
@@ -6859,7 +6859,7 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -6868,28 +6868,28 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -30459,8 +30459,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{338BDA73-949D-6141-997A-6445BD9150B1}">
   <dimension ref="A1:CO144"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A36" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="W41" sqref="W41"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="AW56" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="BT50" sqref="BT50:BY50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -30640,11 +30640,11 @@
     </row>
     <row r="26" spans="1:93">
       <c r="B26" s="10"/>
-      <c r="C26" s="76" t="s">
+      <c r="C26" s="70" t="s">
         <v>30</v>
       </c>
-      <c r="D26" s="76"/>
-      <c r="E26" s="76"/>
+      <c r="D26" s="70"/>
+      <c r="E26" s="70"/>
       <c r="F26" s="39"/>
       <c r="G26" s="39"/>
     </row>
@@ -30913,11 +30913,11 @@
       <c r="CO35" s="31"/>
     </row>
     <row r="36" spans="1:93" ht="18">
-      <c r="C36" s="76" t="s">
+      <c r="C36" s="70" t="s">
         <v>31</v>
       </c>
-      <c r="D36" s="76"/>
-      <c r="E36" s="76"/>
+      <c r="D36" s="70"/>
+      <c r="E36" s="70"/>
       <c r="F36" s="39"/>
       <c r="G36" s="39"/>
       <c r="BM36" s="31"/>
@@ -33051,14 +33051,14 @@
       <c r="AA53" s="15"/>
     </row>
     <row r="54" spans="1:93" ht="20">
-      <c r="L54" s="74" t="s">
+      <c r="L54" s="73" t="s">
         <v>42</v>
       </c>
-      <c r="M54" s="74"/>
-      <c r="N54" s="74"/>
-      <c r="O54" s="74"/>
-      <c r="P54" s="74"/>
-      <c r="Q54" s="74"/>
+      <c r="M54" s="73"/>
+      <c r="N54" s="73"/>
+      <c r="O54" s="73"/>
+      <c r="P54" s="73"/>
+      <c r="Q54" s="73"/>
     </row>
     <row r="55" spans="1:93">
       <c r="L55" s="6">
@@ -33098,11 +33098,11 @@
     </row>
     <row r="60" spans="1:93">
       <c r="B60" s="1"/>
-      <c r="Z60" s="76" t="s">
+      <c r="Z60" s="70" t="s">
         <v>30</v>
       </c>
-      <c r="AA60" s="76"/>
-      <c r="AB60" s="76"/>
+      <c r="AA60" s="70"/>
+      <c r="AB60" s="70"/>
       <c r="AI60" s="69" t="s">
         <v>3</v>
       </c>
@@ -34238,11 +34238,11 @@
       <c r="J68" s="69"/>
       <c r="X68" s="15"/>
       <c r="Y68" s="15"/>
-      <c r="Z68" s="74" t="s">
+      <c r="Z68" s="73" t="s">
         <v>69</v>
       </c>
-      <c r="AA68" s="74"/>
-      <c r="AB68" s="74"/>
+      <c r="AA68" s="73"/>
+      <c r="AB68" s="73"/>
       <c r="AD68" s="34" t="s">
         <v>71</v>
       </c>
@@ -34448,17 +34448,17 @@
       <c r="W73" s="15"/>
       <c r="X73" s="15"/>
       <c r="Y73" s="15"/>
-      <c r="Z73" s="76" t="s">
+      <c r="Z73" s="70" t="s">
         <v>30</v>
       </c>
-      <c r="AA73" s="76"/>
-      <c r="AI73" s="77" t="s">
+      <c r="AA73" s="70"/>
+      <c r="AI73" s="74" t="s">
         <v>52</v>
       </c>
-      <c r="AJ73" s="77"/>
+      <c r="AJ73" s="74"/>
       <c r="AK73" s="31"/>
-      <c r="AL73" s="77"/>
-      <c r="AM73" s="77"/>
+      <c r="AL73" s="74"/>
+      <c r="AM73" s="74"/>
       <c r="AN73" s="31"/>
       <c r="AO73" s="31"/>
       <c r="AP73" s="31"/>
@@ -34782,29 +34782,29 @@
       <c r="AC77" s="41" t="s">
         <v>53</v>
       </c>
-      <c r="AI77" s="73" t="s">
+      <c r="AI77" s="76" t="s">
         <v>64</v>
       </c>
-      <c r="AJ77" s="73"/>
+      <c r="AJ77" s="76"/>
       <c r="AK77" s="29"/>
-      <c r="AL77" s="73"/>
-      <c r="AM77" s="73"/>
+      <c r="AL77" s="76"/>
+      <c r="AM77" s="76"/>
       <c r="AN77" s="29"/>
       <c r="AO77" s="31"/>
       <c r="AP77" s="31"/>
       <c r="AQ77" s="31"/>
       <c r="AR77" s="31"/>
       <c r="AS77" s="31"/>
-      <c r="AT77" s="73" t="s">
+      <c r="AT77" s="76" t="s">
         <v>65</v>
       </c>
-      <c r="AU77" s="73"/>
-      <c r="AV77" s="73"/>
-      <c r="AW77" s="73"/>
-      <c r="AX77" s="73"/>
-      <c r="AY77" s="73"/>
-      <c r="AZ77" s="73"/>
-      <c r="BA77" s="73"/>
+      <c r="AU77" s="76"/>
+      <c r="AV77" s="76"/>
+      <c r="AW77" s="76"/>
+      <c r="AX77" s="76"/>
+      <c r="AY77" s="76"/>
+      <c r="AZ77" s="76"/>
+      <c r="BA77" s="76"/>
     </row>
     <row r="78" spans="1:78">
       <c r="B78" s="1"/>
@@ -34904,16 +34904,16 @@
       </c>
     </row>
     <row r="81" spans="1:93" ht="16" customHeight="1">
-      <c r="C81" s="70" t="s">
+      <c r="C81" s="77" t="s">
         <v>85</v>
       </c>
-      <c r="D81" s="70"/>
-      <c r="E81" s="70"/>
-      <c r="F81" s="70"/>
-      <c r="G81" s="70"/>
-      <c r="H81" s="70"/>
-      <c r="I81" s="70"/>
-      <c r="J81" s="70"/>
+      <c r="D81" s="77"/>
+      <c r="E81" s="77"/>
+      <c r="F81" s="77"/>
+      <c r="G81" s="77"/>
+      <c r="H81" s="77"/>
+      <c r="I81" s="77"/>
+      <c r="J81" s="77"/>
       <c r="AI81" s="69" t="s">
         <v>4</v>
       </c>
@@ -36329,14 +36329,14 @@
       </c>
     </row>
     <row r="91" spans="1:93" ht="19">
-      <c r="L91" s="70" t="s">
+      <c r="L91" s="77" t="s">
         <v>13</v>
       </c>
-      <c r="M91" s="70"/>
-      <c r="N91" s="70"/>
-      <c r="O91" s="70"/>
-      <c r="P91" s="70"/>
-      <c r="Q91" s="70"/>
+      <c r="M91" s="77"/>
+      <c r="N91" s="77"/>
+      <c r="O91" s="77"/>
+      <c r="P91" s="77"/>
+      <c r="Q91" s="77"/>
       <c r="Z91" s="41" t="s">
         <v>11</v>
       </c>
@@ -36489,14 +36489,14 @@
       <c r="AA94" s="17"/>
     </row>
     <row r="95" spans="1:93" ht="20">
-      <c r="L95" s="70" t="s">
+      <c r="L95" s="77" t="s">
         <v>35</v>
       </c>
-      <c r="M95" s="70"/>
-      <c r="N95" s="70"/>
-      <c r="O95" s="70"/>
-      <c r="P95" s="70"/>
-      <c r="Q95" s="70"/>
+      <c r="M95" s="77"/>
+      <c r="N95" s="77"/>
+      <c r="O95" s="77"/>
+      <c r="P95" s="77"/>
+      <c r="Q95" s="77"/>
     </row>
     <row r="98" spans="1:40" ht="47">
       <c r="A98" s="27" t="s">
@@ -37117,16 +37117,16 @@
       </c>
       <c r="D120" s="69"/>
       <c r="E120" s="69"/>
-      <c r="G120" s="70" t="s">
+      <c r="G120" s="77" t="s">
         <v>39</v>
       </c>
-      <c r="H120" s="70"/>
-      <c r="I120" s="70"/>
-      <c r="K120" s="70" t="s">
+      <c r="H120" s="77"/>
+      <c r="I120" s="77"/>
+      <c r="K120" s="77" t="s">
         <v>40</v>
       </c>
-      <c r="L120" s="70"/>
-      <c r="M120" s="70"/>
+      <c r="L120" s="77"/>
+      <c r="M120" s="77"/>
       <c r="N120" s="17"/>
       <c r="O120" s="17" t="s">
         <v>41</v>
@@ -37550,6 +37550,65 @@
     </row>
   </sheetData>
   <mergeCells count="71">
+    <mergeCell ref="A112:I112"/>
+    <mergeCell ref="C143:H143"/>
+    <mergeCell ref="C120:E120"/>
+    <mergeCell ref="G120:I120"/>
+    <mergeCell ref="K120:M120"/>
+    <mergeCell ref="A125:A130"/>
+    <mergeCell ref="C135:H135"/>
+    <mergeCell ref="A137:A142"/>
+    <mergeCell ref="A114:A119"/>
+    <mergeCell ref="BE81:BL81"/>
+    <mergeCell ref="BT81:BY81"/>
+    <mergeCell ref="A83:A90"/>
+    <mergeCell ref="L91:Q91"/>
+    <mergeCell ref="AI91:AP91"/>
+    <mergeCell ref="AT91:BA91"/>
+    <mergeCell ref="BE91:BL91"/>
+    <mergeCell ref="BT91:BY91"/>
+    <mergeCell ref="C81:J81"/>
+    <mergeCell ref="AI81:AP81"/>
+    <mergeCell ref="AT81:BA81"/>
+    <mergeCell ref="J92:J94"/>
+    <mergeCell ref="L95:Q95"/>
+    <mergeCell ref="A100:I100"/>
+    <mergeCell ref="A102:A109"/>
+    <mergeCell ref="C77:J77"/>
+    <mergeCell ref="AI77:AJ77"/>
+    <mergeCell ref="AL77:AM77"/>
+    <mergeCell ref="AT77:BA77"/>
+    <mergeCell ref="C79:J79"/>
+    <mergeCell ref="A75:A76"/>
+    <mergeCell ref="C68:J68"/>
+    <mergeCell ref="Z68:AB68"/>
+    <mergeCell ref="AI68:AN68"/>
+    <mergeCell ref="AT68:BA68"/>
+    <mergeCell ref="C70:J70"/>
+    <mergeCell ref="Z73:AA73"/>
+    <mergeCell ref="AI73:AJ73"/>
+    <mergeCell ref="AL73:AM73"/>
+    <mergeCell ref="AT73:BA73"/>
+    <mergeCell ref="BE68:BL68"/>
+    <mergeCell ref="BT68:BY68"/>
+    <mergeCell ref="Z60:AB60"/>
+    <mergeCell ref="AI60:AN60"/>
+    <mergeCell ref="AT60:BA60"/>
+    <mergeCell ref="BE60:BL60"/>
+    <mergeCell ref="BT60:BY60"/>
+    <mergeCell ref="A62:A67"/>
+    <mergeCell ref="BE50:BJ50"/>
+    <mergeCell ref="BT50:BY50"/>
+    <mergeCell ref="CA50:CH50"/>
+    <mergeCell ref="J51:J53"/>
+    <mergeCell ref="L54:Q54"/>
+    <mergeCell ref="L56:Q56"/>
+    <mergeCell ref="AT50:AY50"/>
+    <mergeCell ref="A42:A49"/>
+    <mergeCell ref="U42:U49"/>
+    <mergeCell ref="L50:Q50"/>
+    <mergeCell ref="W50:X50"/>
+    <mergeCell ref="AI50:AP50"/>
     <mergeCell ref="CJ40:CK40"/>
     <mergeCell ref="C26:E26"/>
     <mergeCell ref="A28:A35"/>
@@ -37562,65 +37621,6 @@
     <mergeCell ref="BE40:BJ40"/>
     <mergeCell ref="BT40:BY40"/>
     <mergeCell ref="CA40:CH40"/>
-    <mergeCell ref="A42:A49"/>
-    <mergeCell ref="U42:U49"/>
-    <mergeCell ref="L50:Q50"/>
-    <mergeCell ref="W50:X50"/>
-    <mergeCell ref="AI50:AP50"/>
-    <mergeCell ref="A62:A67"/>
-    <mergeCell ref="BE50:BJ50"/>
-    <mergeCell ref="BT50:BY50"/>
-    <mergeCell ref="CA50:CH50"/>
-    <mergeCell ref="J51:J53"/>
-    <mergeCell ref="L54:Q54"/>
-    <mergeCell ref="L56:Q56"/>
-    <mergeCell ref="AT50:AY50"/>
-    <mergeCell ref="BT68:BY68"/>
-    <mergeCell ref="Z60:AB60"/>
-    <mergeCell ref="AI60:AN60"/>
-    <mergeCell ref="AT60:BA60"/>
-    <mergeCell ref="BE60:BL60"/>
-    <mergeCell ref="BT60:BY60"/>
-    <mergeCell ref="Z73:AA73"/>
-    <mergeCell ref="AI73:AJ73"/>
-    <mergeCell ref="AL73:AM73"/>
-    <mergeCell ref="AT73:BA73"/>
-    <mergeCell ref="BE68:BL68"/>
-    <mergeCell ref="C68:J68"/>
-    <mergeCell ref="Z68:AB68"/>
-    <mergeCell ref="AI68:AN68"/>
-    <mergeCell ref="AT68:BA68"/>
-    <mergeCell ref="C70:J70"/>
-    <mergeCell ref="AI77:AJ77"/>
-    <mergeCell ref="AL77:AM77"/>
-    <mergeCell ref="AT77:BA77"/>
-    <mergeCell ref="C79:J79"/>
-    <mergeCell ref="A75:A76"/>
-    <mergeCell ref="J92:J94"/>
-    <mergeCell ref="L95:Q95"/>
-    <mergeCell ref="A100:I100"/>
-    <mergeCell ref="A102:A109"/>
-    <mergeCell ref="C77:J77"/>
-    <mergeCell ref="BE81:BL81"/>
-    <mergeCell ref="BT81:BY81"/>
-    <mergeCell ref="A83:A90"/>
-    <mergeCell ref="L91:Q91"/>
-    <mergeCell ref="AI91:AP91"/>
-    <mergeCell ref="AT91:BA91"/>
-    <mergeCell ref="BE91:BL91"/>
-    <mergeCell ref="BT91:BY91"/>
-    <mergeCell ref="C81:J81"/>
-    <mergeCell ref="AI81:AP81"/>
-    <mergeCell ref="AT81:BA81"/>
-    <mergeCell ref="A112:I112"/>
-    <mergeCell ref="C143:H143"/>
-    <mergeCell ref="C120:E120"/>
-    <mergeCell ref="G120:I120"/>
-    <mergeCell ref="K120:M120"/>
-    <mergeCell ref="A125:A130"/>
-    <mergeCell ref="C135:H135"/>
-    <mergeCell ref="A137:A142"/>
-    <mergeCell ref="A114:A119"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -38236,11 +38236,11 @@
     </row>
     <row r="26" spans="1:278">
       <c r="B26" s="10"/>
-      <c r="C26" s="76" t="s">
+      <c r="C26" s="70" t="s">
         <v>30</v>
       </c>
-      <c r="D26" s="76"/>
-      <c r="E26" s="76"/>
+      <c r="D26" s="70"/>
+      <c r="E26" s="70"/>
       <c r="F26" s="47"/>
       <c r="G26" s="47"/>
       <c r="CQ26" t="s">
@@ -38499,11 +38499,11 @@
       <c r="CJ35" s="31"/>
     </row>
     <row r="36" spans="1:302" ht="18">
-      <c r="C36" s="76" t="s">
+      <c r="C36" s="70" t="s">
         <v>31</v>
       </c>
-      <c r="D36" s="76"/>
-      <c r="E36" s="76"/>
+      <c r="D36" s="70"/>
+      <c r="E36" s="70"/>
       <c r="F36" s="47"/>
       <c r="G36" s="47"/>
       <c r="BL36" s="31"/>
@@ -38558,31 +38558,31 @@
       <c r="CJ37" s="51"/>
     </row>
     <row r="38" spans="1:302">
-      <c r="BL38" s="73"/>
-      <c r="BM38" s="73"/>
-      <c r="BN38" s="73"/>
-      <c r="BO38" s="73"/>
-      <c r="BP38" s="73"/>
-      <c r="BQ38" s="73"/>
-      <c r="BR38" s="73"/>
-      <c r="BS38" s="73"/>
-      <c r="BT38" s="73"/>
-      <c r="BU38" s="73"/>
-      <c r="BV38" s="73"/>
-      <c r="BW38" s="73"/>
-      <c r="BX38" s="73"/>
-      <c r="BY38" s="73"/>
-      <c r="BZ38" s="73"/>
-      <c r="CA38" s="73"/>
-      <c r="CB38" s="73"/>
-      <c r="CC38" s="73"/>
-      <c r="CD38" s="73"/>
-      <c r="CE38" s="73"/>
-      <c r="CF38" s="73"/>
-      <c r="CG38" s="73"/>
-      <c r="CH38" s="73"/>
-      <c r="CI38" s="73"/>
-      <c r="CJ38" s="73"/>
+      <c r="BL38" s="76"/>
+      <c r="BM38" s="76"/>
+      <c r="BN38" s="76"/>
+      <c r="BO38" s="76"/>
+      <c r="BP38" s="76"/>
+      <c r="BQ38" s="76"/>
+      <c r="BR38" s="76"/>
+      <c r="BS38" s="76"/>
+      <c r="BT38" s="76"/>
+      <c r="BU38" s="76"/>
+      <c r="BV38" s="76"/>
+      <c r="BW38" s="76"/>
+      <c r="BX38" s="76"/>
+      <c r="BY38" s="76"/>
+      <c r="BZ38" s="76"/>
+      <c r="CA38" s="76"/>
+      <c r="CB38" s="76"/>
+      <c r="CC38" s="76"/>
+      <c r="CD38" s="76"/>
+      <c r="CE38" s="76"/>
+      <c r="CF38" s="76"/>
+      <c r="CG38" s="76"/>
+      <c r="CH38" s="76"/>
+      <c r="CI38" s="76"/>
+      <c r="CJ38" s="76"/>
     </row>
     <row r="40" spans="1:302">
       <c r="C40" s="69" t="s">
@@ -38728,8 +38728,8 @@
       <c r="JC40" s="69"/>
       <c r="JD40" s="69"/>
       <c r="JE40" s="69"/>
-      <c r="JL40" s="73"/>
-      <c r="JM40" s="73"/>
+      <c r="JL40" s="76"/>
+      <c r="JM40" s="76"/>
       <c r="KI40" s="69" t="s">
         <v>3</v>
       </c>
@@ -42413,14 +42413,14 @@
       <c r="EB50" s="58"/>
       <c r="EC50" s="58"/>
       <c r="ED50" s="58"/>
-      <c r="EE50" s="80" t="s">
+      <c r="EE50" s="79" t="s">
         <v>193</v>
       </c>
-      <c r="EF50" s="80"/>
-      <c r="EG50" s="80"/>
-      <c r="EH50" s="80"/>
-      <c r="EI50" s="80"/>
-      <c r="EJ50" s="80"/>
+      <c r="EF50" s="79"/>
+      <c r="EG50" s="79"/>
+      <c r="EH50" s="79"/>
+      <c r="EI50" s="79"/>
+      <c r="EJ50" s="79"/>
       <c r="EK50" s="58"/>
       <c r="EL50" s="58"/>
       <c r="EM50" s="58"/>
@@ -42462,14 +42462,14 @@
       <c r="HD50" s="58"/>
       <c r="HE50" s="58"/>
       <c r="HF50" s="58"/>
-      <c r="HG50" s="80" t="s">
+      <c r="HG50" s="79" t="s">
         <v>192</v>
       </c>
-      <c r="HH50" s="80"/>
-      <c r="HI50" s="80"/>
-      <c r="HJ50" s="80"/>
-      <c r="HK50" s="80"/>
-      <c r="HL50" s="80"/>
+      <c r="HH50" s="79"/>
+      <c r="HI50" s="79"/>
+      <c r="HJ50" s="79"/>
+      <c r="HK50" s="79"/>
+      <c r="HL50" s="79"/>
       <c r="HM50" s="58"/>
       <c r="HN50" s="58"/>
       <c r="HO50" s="58"/>
@@ -42482,15 +42482,15 @@
       <c r="IS50" s="8"/>
       <c r="IT50" s="8"/>
       <c r="IV50" s="31"/>
-      <c r="IW50" s="73"/>
-      <c r="IX50" s="73"/>
+      <c r="IW50" s="76"/>
+      <c r="IX50" s="76"/>
       <c r="IY50" s="31"/>
-      <c r="IZ50" s="80"/>
-      <c r="JA50" s="80"/>
-      <c r="JB50" s="80"/>
-      <c r="JC50" s="80"/>
-      <c r="JD50" s="80"/>
-      <c r="JE50" s="80"/>
+      <c r="IZ50" s="79"/>
+      <c r="JA50" s="79"/>
+      <c r="JB50" s="79"/>
+      <c r="JC50" s="79"/>
+      <c r="JD50" s="79"/>
+      <c r="JE50" s="79"/>
       <c r="JF50" s="31"/>
       <c r="JG50" s="55"/>
       <c r="JH50" s="31"/>
@@ -42504,14 +42504,14 @@
       <c r="KF50" s="58"/>
       <c r="KG50" s="58"/>
       <c r="KH50" s="58"/>
-      <c r="KI50" s="80" t="s">
+      <c r="KI50" s="79" t="s">
         <v>133</v>
       </c>
-      <c r="KJ50" s="80"/>
-      <c r="KK50" s="80"/>
-      <c r="KL50" s="80"/>
-      <c r="KM50" s="80"/>
-      <c r="KN50" s="80"/>
+      <c r="KJ50" s="79"/>
+      <c r="KK50" s="79"/>
+      <c r="KL50" s="79"/>
+      <c r="KM50" s="79"/>
+      <c r="KN50" s="79"/>
       <c r="KO50" s="58"/>
       <c r="KP50" s="59" t="s">
         <v>12</v>
@@ -42826,14 +42826,14 @@
     </row>
     <row r="54" spans="1:319" ht="20">
       <c r="B54" s="1"/>
-      <c r="L54" s="74" t="s">
+      <c r="L54" s="73" t="s">
         <v>42</v>
       </c>
-      <c r="M54" s="74"/>
-      <c r="N54" s="74"/>
-      <c r="O54" s="74"/>
-      <c r="P54" s="74"/>
-      <c r="Q54" s="74"/>
+      <c r="M54" s="73"/>
+      <c r="N54" s="73"/>
+      <c r="O54" s="73"/>
+      <c r="P54" s="73"/>
+      <c r="Q54" s="73"/>
       <c r="R54" s="15"/>
       <c r="S54" s="15"/>
       <c r="T54" s="15"/>
@@ -42861,14 +42861,14 @@
       <c r="JJ54" s="31"/>
       <c r="JK54" s="31"/>
       <c r="JL54" s="31"/>
-      <c r="KI54" s="74" t="s">
+      <c r="KI54" s="73" t="s">
         <v>148</v>
       </c>
-      <c r="KJ54" s="74"/>
-      <c r="KK54" s="74"/>
-      <c r="KL54" s="74"/>
-      <c r="KM54" s="74"/>
-      <c r="KN54" s="74"/>
+      <c r="KJ54" s="73"/>
+      <c r="KK54" s="73"/>
+      <c r="KL54" s="73"/>
+      <c r="KM54" s="73"/>
+      <c r="KN54" s="73"/>
     </row>
     <row r="55" spans="1:319">
       <c r="B55" s="1"/>
@@ -42998,11 +42998,11 @@
     </row>
     <row r="59" spans="1:319">
       <c r="B59" s="1"/>
-      <c r="Z59" s="76" t="s">
+      <c r="Z59" s="70" t="s">
         <v>30</v>
       </c>
-      <c r="AA59" s="76"/>
-      <c r="AB59" s="76"/>
+      <c r="AA59" s="70"/>
+      <c r="AB59" s="70"/>
       <c r="AH59" s="69" t="s">
         <v>3</v>
       </c>
@@ -43061,14 +43061,14 @@
       <c r="EC59" s="45"/>
       <c r="ES59" s="31"/>
       <c r="ET59" s="31"/>
-      <c r="EU59" s="73"/>
-      <c r="EV59" s="73"/>
-      <c r="EW59" s="73"/>
-      <c r="EX59" s="73"/>
-      <c r="EY59" s="73"/>
-      <c r="EZ59" s="73"/>
-      <c r="FA59" s="73"/>
-      <c r="FB59" s="73"/>
+      <c r="EU59" s="76"/>
+      <c r="EV59" s="76"/>
+      <c r="EW59" s="76"/>
+      <c r="EX59" s="76"/>
+      <c r="EY59" s="76"/>
+      <c r="EZ59" s="76"/>
+      <c r="FA59" s="76"/>
+      <c r="FB59" s="76"/>
       <c r="FC59" s="31"/>
       <c r="GM59" s="69" t="s">
         <v>3</v>
@@ -43092,26 +43092,26 @@
       <c r="HE59" s="52"/>
       <c r="HU59" s="31"/>
       <c r="HV59" s="31"/>
-      <c r="HW59" s="73"/>
-      <c r="HX59" s="73"/>
-      <c r="HY59" s="73"/>
-      <c r="HZ59" s="73"/>
-      <c r="IA59" s="73"/>
-      <c r="IB59" s="73"/>
-      <c r="IC59" s="73"/>
-      <c r="ID59" s="73"/>
+      <c r="HW59" s="76"/>
+      <c r="HX59" s="76"/>
+      <c r="HY59" s="76"/>
+      <c r="HZ59" s="76"/>
+      <c r="IA59" s="76"/>
+      <c r="IB59" s="76"/>
+      <c r="IC59" s="76"/>
+      <c r="ID59" s="76"/>
       <c r="IE59" s="31"/>
       <c r="JJ59" s="31"/>
       <c r="JK59" s="31"/>
       <c r="JL59" s="31"/>
       <c r="JM59" s="31"/>
       <c r="JN59" s="31"/>
-      <c r="JO59" s="73"/>
-      <c r="JP59" s="73"/>
-      <c r="JQ59" s="73"/>
-      <c r="JR59" s="73"/>
-      <c r="JS59" s="73"/>
-      <c r="JT59" s="73"/>
+      <c r="JO59" s="76"/>
+      <c r="JP59" s="76"/>
+      <c r="JQ59" s="76"/>
+      <c r="JR59" s="76"/>
+      <c r="JS59" s="76"/>
+      <c r="JT59" s="76"/>
       <c r="JU59" s="31"/>
       <c r="JX59" s="69" t="s">
         <v>4</v>
@@ -43125,21 +43125,21 @@
       <c r="KE59" s="69"/>
       <c r="KF59" s="52"/>
       <c r="KG59" s="52"/>
-      <c r="KP59" s="76" t="s">
+      <c r="KP59" s="70" t="s">
         <v>30</v>
       </c>
-      <c r="KQ59" s="76"/>
-      <c r="KR59" s="76"/>
+      <c r="KQ59" s="70"/>
+      <c r="KR59" s="70"/>
       <c r="KW59" s="31"/>
       <c r="KX59" s="31"/>
-      <c r="KY59" s="73"/>
-      <c r="KZ59" s="73"/>
-      <c r="LA59" s="73"/>
-      <c r="LB59" s="73"/>
-      <c r="LC59" s="73"/>
-      <c r="LD59" s="73"/>
-      <c r="LE59" s="73"/>
-      <c r="LF59" s="73"/>
+      <c r="KY59" s="76"/>
+      <c r="KZ59" s="76"/>
+      <c r="LA59" s="76"/>
+      <c r="LB59" s="76"/>
+      <c r="LC59" s="76"/>
+      <c r="LD59" s="76"/>
+      <c r="LE59" s="76"/>
+      <c r="LF59" s="76"/>
       <c r="LG59" s="31"/>
     </row>
     <row r="60" spans="1:319" ht="51" customHeight="1">
@@ -44043,14 +44043,14 @@
       <c r="EC62" s="50"/>
       <c r="ES62" s="31"/>
       <c r="ET62" s="31"/>
-      <c r="EU62" s="74"/>
-      <c r="EV62" s="74"/>
-      <c r="EW62" s="74"/>
-      <c r="EX62" s="74"/>
-      <c r="EY62" s="74"/>
-      <c r="EZ62" s="74"/>
-      <c r="FA62" s="74"/>
-      <c r="FB62" s="74"/>
+      <c r="EU62" s="73"/>
+      <c r="EV62" s="73"/>
+      <c r="EW62" s="73"/>
+      <c r="EX62" s="73"/>
+      <c r="EY62" s="73"/>
+      <c r="EZ62" s="73"/>
+      <c r="FA62" s="73"/>
+      <c r="FB62" s="73"/>
       <c r="FC62" s="31"/>
       <c r="GH62" s="71"/>
       <c r="GI62" s="1" t="s">
@@ -44120,14 +44120,14 @@
       <c r="HE62" s="51"/>
       <c r="HU62" s="31"/>
       <c r="HV62" s="31"/>
-      <c r="HW62" s="74"/>
-      <c r="HX62" s="74"/>
-      <c r="HY62" s="74"/>
-      <c r="HZ62" s="74"/>
-      <c r="IA62" s="74"/>
-      <c r="IB62" s="74"/>
-      <c r="IC62" s="74"/>
-      <c r="ID62" s="74"/>
+      <c r="HW62" s="73"/>
+      <c r="HX62" s="73"/>
+      <c r="HY62" s="73"/>
+      <c r="HZ62" s="73"/>
+      <c r="IA62" s="73"/>
+      <c r="IB62" s="73"/>
+      <c r="IC62" s="73"/>
+      <c r="ID62" s="73"/>
       <c r="IE62" s="31"/>
       <c r="JJ62" s="78"/>
       <c r="JK62" s="63"/>
@@ -44197,14 +44197,14 @@
       </c>
       <c r="KW62" s="31"/>
       <c r="KX62" s="31"/>
-      <c r="KY62" s="74"/>
-      <c r="KZ62" s="74"/>
-      <c r="LA62" s="74"/>
-      <c r="LB62" s="74"/>
-      <c r="LC62" s="74"/>
-      <c r="LD62" s="74"/>
-      <c r="LE62" s="74"/>
-      <c r="LF62" s="74"/>
+      <c r="KY62" s="73"/>
+      <c r="KZ62" s="73"/>
+      <c r="LA62" s="73"/>
+      <c r="LB62" s="73"/>
+      <c r="LC62" s="73"/>
+      <c r="LD62" s="73"/>
+      <c r="LE62" s="73"/>
+      <c r="LF62" s="73"/>
       <c r="LG62" s="31"/>
     </row>
     <row r="63" spans="1:319">
@@ -45801,11 +45801,11 @@
       <c r="J67" s="69"/>
       <c r="X67" s="15"/>
       <c r="Y67" s="15"/>
-      <c r="Z67" s="74" t="s">
+      <c r="Z67" s="73" t="s">
         <v>96</v>
       </c>
-      <c r="AA67" s="74"/>
-      <c r="AB67" s="74"/>
+      <c r="AA67" s="73"/>
+      <c r="AB67" s="73"/>
       <c r="AD67" s="45" t="s">
         <v>34</v>
       </c>
@@ -46020,23 +46020,23 @@
       <c r="JL67" s="55"/>
       <c r="JM67" s="31"/>
       <c r="JN67" s="31"/>
-      <c r="JO67" s="73"/>
-      <c r="JP67" s="73"/>
-      <c r="JQ67" s="73"/>
-      <c r="JR67" s="73"/>
-      <c r="JS67" s="73"/>
-      <c r="JT67" s="73"/>
+      <c r="JO67" s="76"/>
+      <c r="JP67" s="76"/>
+      <c r="JQ67" s="76"/>
+      <c r="JR67" s="76"/>
+      <c r="JS67" s="76"/>
+      <c r="JT67" s="76"/>
       <c r="JU67" s="31"/>
-      <c r="JX67" s="79" t="s">
+      <c r="JX67" s="80" t="s">
         <v>134</v>
       </c>
-      <c r="JY67" s="79"/>
-      <c r="JZ67" s="79"/>
-      <c r="KA67" s="79"/>
-      <c r="KB67" s="79"/>
-      <c r="KC67" s="79"/>
-      <c r="KD67" s="79"/>
-      <c r="KE67" s="79"/>
+      <c r="JY67" s="80"/>
+      <c r="JZ67" s="80"/>
+      <c r="KA67" s="80"/>
+      <c r="KB67" s="80"/>
+      <c r="KC67" s="80"/>
+      <c r="KD67" s="80"/>
+      <c r="KE67" s="80"/>
       <c r="KF67" s="54"/>
       <c r="KG67" s="54"/>
       <c r="KH67" s="26"/>
@@ -46047,11 +46047,11 @@
       <c r="KM67" s="26"/>
       <c r="KN67" s="26"/>
       <c r="KO67" s="26"/>
-      <c r="KP67" s="74" t="s">
+      <c r="KP67" s="73" t="s">
         <v>142</v>
       </c>
-      <c r="KQ67" s="74"/>
-      <c r="KR67" s="74"/>
+      <c r="KQ67" s="73"/>
+      <c r="KR67" s="73"/>
       <c r="KS67" s="26"/>
       <c r="KT67" s="52" t="s">
         <v>145</v>
@@ -46169,18 +46169,18 @@
       <c r="W70" s="15"/>
       <c r="X70" s="15"/>
       <c r="Y70" s="15"/>
-      <c r="Z70" s="76" t="s">
+      <c r="Z70" s="70" t="s">
         <v>30</v>
       </c>
-      <c r="AA70" s="76"/>
-      <c r="AB70" s="76"/>
-      <c r="AH70" s="77" t="s">
+      <c r="AA70" s="70"/>
+      <c r="AB70" s="70"/>
+      <c r="AH70" s="74" t="s">
         <v>52</v>
       </c>
-      <c r="AI70" s="77"/>
+      <c r="AI70" s="74"/>
       <c r="AJ70" s="31"/>
-      <c r="AK70" s="77"/>
-      <c r="AL70" s="77"/>
+      <c r="AK70" s="74"/>
+      <c r="AL70" s="74"/>
       <c r="AM70" s="31"/>
       <c r="AN70" s="31"/>
       <c r="AO70" s="31"/>
@@ -46506,37 +46506,37 @@
       <c r="W74" s="15"/>
       <c r="X74" s="15"/>
       <c r="Y74" s="15"/>
-      <c r="Z74" s="73" t="s">
+      <c r="Z74" s="76" t="s">
         <v>95</v>
       </c>
-      <c r="AA74" s="73"/>
-      <c r="AB74" s="73"/>
+      <c r="AA74" s="76"/>
+      <c r="AB74" s="76"/>
       <c r="AD74" s="45" t="s">
         <v>53</v>
       </c>
-      <c r="AH74" s="73" t="s">
+      <c r="AH74" s="76" t="s">
         <v>64</v>
       </c>
-      <c r="AI74" s="73"/>
+      <c r="AI74" s="76"/>
       <c r="AJ74" s="29"/>
-      <c r="AK74" s="73"/>
-      <c r="AL74" s="73"/>
+      <c r="AK74" s="76"/>
+      <c r="AL74" s="76"/>
       <c r="AM74" s="29"/>
       <c r="AN74" s="31"/>
       <c r="AO74" s="31"/>
       <c r="AP74" s="31"/>
       <c r="AQ74" s="31"/>
       <c r="AR74" s="31"/>
-      <c r="AS74" s="73" t="s">
+      <c r="AS74" s="76" t="s">
         <v>65</v>
       </c>
-      <c r="AT74" s="73"/>
-      <c r="AU74" s="73"/>
-      <c r="AV74" s="73"/>
-      <c r="AW74" s="73"/>
-      <c r="AX74" s="73"/>
-      <c r="AY74" s="73"/>
-      <c r="AZ74" s="73"/>
+      <c r="AT74" s="76"/>
+      <c r="AU74" s="76"/>
+      <c r="AV74" s="76"/>
+      <c r="AW74" s="76"/>
+      <c r="AX74" s="76"/>
+      <c r="AY74" s="76"/>
+      <c r="AZ74" s="76"/>
       <c r="ES74" s="31"/>
       <c r="ET74" s="31"/>
       <c r="EU74" s="31"/>
@@ -48760,16 +48760,16 @@
       <c r="FA83" s="29"/>
       <c r="FB83" s="29"/>
       <c r="FC83" s="31"/>
-      <c r="FD83" s="70" t="s">
+      <c r="FD83" s="77" t="s">
         <v>119</v>
       </c>
-      <c r="FE83" s="70"/>
-      <c r="FF83" s="70"/>
-      <c r="FG83" s="70"/>
-      <c r="FH83" s="70"/>
-      <c r="FI83" s="70"/>
-      <c r="FJ83" s="70"/>
-      <c r="FK83" s="70"/>
+      <c r="FE83" s="77"/>
+      <c r="FF83" s="77"/>
+      <c r="FG83" s="77"/>
+      <c r="FH83" s="77"/>
+      <c r="FI83" s="77"/>
+      <c r="FJ83" s="77"/>
+      <c r="FK83" s="77"/>
       <c r="GH83" s="71"/>
       <c r="GI83" s="1" t="s">
         <v>27</v>
@@ -48881,16 +48881,16 @@
       <c r="IC83" s="29"/>
       <c r="ID83" s="29"/>
       <c r="IE83" s="31"/>
-      <c r="IF83" s="70" t="s">
+      <c r="IF83" s="77" t="s">
         <v>130</v>
       </c>
-      <c r="IG83" s="70"/>
-      <c r="IH83" s="70"/>
-      <c r="II83" s="70"/>
-      <c r="IJ83" s="70"/>
-      <c r="IK83" s="70"/>
-      <c r="IL83" s="70"/>
-      <c r="IM83" s="70"/>
+      <c r="IG83" s="77"/>
+      <c r="IH83" s="77"/>
+      <c r="II83" s="77"/>
+      <c r="IJ83" s="77"/>
+      <c r="IK83" s="77"/>
+      <c r="IL83" s="77"/>
+      <c r="IM83" s="77"/>
       <c r="JJ83" s="78"/>
       <c r="JK83" s="63"/>
       <c r="JL83" s="51"/>
@@ -48977,16 +48977,16 @@
       <c r="LE83" s="29"/>
       <c r="LF83" s="29"/>
       <c r="LG83" s="31"/>
-      <c r="LH83" s="70" t="s">
+      <c r="LH83" s="77" t="s">
         <v>139</v>
       </c>
-      <c r="LI83" s="70"/>
-      <c r="LJ83" s="70"/>
-      <c r="LK83" s="70"/>
-      <c r="LL83" s="70"/>
-      <c r="LM83" s="70"/>
-      <c r="LN83" s="70"/>
-      <c r="LO83" s="70"/>
+      <c r="LI83" s="77"/>
+      <c r="LJ83" s="77"/>
+      <c r="LK83" s="77"/>
+      <c r="LL83" s="77"/>
+      <c r="LM83" s="77"/>
+      <c r="LN83" s="77"/>
+      <c r="LO83" s="77"/>
     </row>
     <row r="84" spans="1:327">
       <c r="A84" s="71"/>
@@ -49955,16 +49955,16 @@
       <c r="LE85" s="31"/>
       <c r="LF85" s="31"/>
       <c r="LG85" s="31"/>
-      <c r="LH85" s="70" t="s">
+      <c r="LH85" s="77" t="s">
         <v>140</v>
       </c>
-      <c r="LI85" s="70"/>
-      <c r="LJ85" s="70"/>
-      <c r="LK85" s="70"/>
-      <c r="LL85" s="70"/>
-      <c r="LM85" s="70"/>
-      <c r="LN85" s="70"/>
-      <c r="LO85" s="70"/>
+      <c r="LI85" s="77"/>
+      <c r="LJ85" s="77"/>
+      <c r="LK85" s="77"/>
+      <c r="LL85" s="77"/>
+      <c r="LM85" s="77"/>
+      <c r="LN85" s="77"/>
+      <c r="LO85" s="77"/>
     </row>
     <row r="86" spans="1:327">
       <c r="A86" s="71"/>
@@ -51371,14 +51371,14 @@
       <c r="LG88" s="31"/>
     </row>
     <row r="89" spans="1:327" ht="20">
-      <c r="L89" s="70" t="s">
+      <c r="L89" s="77" t="s">
         <v>13</v>
       </c>
-      <c r="M89" s="70"/>
-      <c r="N89" s="70"/>
-      <c r="O89" s="70"/>
-      <c r="P89" s="70"/>
-      <c r="Q89" s="70"/>
+      <c r="M89" s="77"/>
+      <c r="N89" s="77"/>
+      <c r="O89" s="77"/>
+      <c r="P89" s="77"/>
+      <c r="Q89" s="77"/>
       <c r="Z89" s="45" t="s">
         <v>11</v>
       </c>
@@ -51484,30 +51484,30 @@
       <c r="EB89" s="8"/>
       <c r="EC89" s="8"/>
       <c r="ED89" s="8"/>
-      <c r="EE89" s="70" t="s">
+      <c r="EE89" s="77" t="s">
         <v>114</v>
       </c>
-      <c r="EF89" s="70"/>
-      <c r="EG89" s="70"/>
-      <c r="EH89" s="70"/>
-      <c r="EI89" s="70"/>
-      <c r="EJ89" s="70"/>
+      <c r="EF89" s="77"/>
+      <c r="EG89" s="77"/>
+      <c r="EH89" s="77"/>
+      <c r="EI89" s="77"/>
+      <c r="EJ89" s="77"/>
       <c r="EM89" s="45" t="s">
         <v>116</v>
       </c>
       <c r="EO89" s="48" t="s">
         <v>117</v>
       </c>
-      <c r="ER89" s="70" t="s">
+      <c r="ER89" s="77" t="s">
         <v>118</v>
       </c>
-      <c r="ES89" s="70"/>
-      <c r="ET89" s="70"/>
-      <c r="EU89" s="70"/>
-      <c r="EV89" s="70"/>
-      <c r="EW89" s="70"/>
-      <c r="EX89" s="70"/>
-      <c r="EY89" s="70"/>
+      <c r="ES89" s="77"/>
+      <c r="ET89" s="77"/>
+      <c r="EU89" s="77"/>
+      <c r="EV89" s="77"/>
+      <c r="EW89" s="77"/>
+      <c r="EX89" s="77"/>
+      <c r="EY89" s="77"/>
       <c r="FO89" s="57"/>
       <c r="FP89" s="8"/>
       <c r="FQ89" s="8"/>
@@ -51552,30 +51552,30 @@
       <c r="HD89" s="8"/>
       <c r="HE89" s="8"/>
       <c r="HF89" s="8"/>
-      <c r="HG89" s="70" t="s">
+      <c r="HG89" s="77" t="s">
         <v>125</v>
       </c>
-      <c r="HH89" s="70"/>
-      <c r="HI89" s="70"/>
-      <c r="HJ89" s="70"/>
-      <c r="HK89" s="70"/>
-      <c r="HL89" s="70"/>
+      <c r="HH89" s="77"/>
+      <c r="HI89" s="77"/>
+      <c r="HJ89" s="77"/>
+      <c r="HK89" s="77"/>
+      <c r="HL89" s="77"/>
       <c r="HO89" s="52" t="s">
         <v>127</v>
       </c>
       <c r="HQ89" s="53" t="s">
         <v>128</v>
       </c>
-      <c r="HT89" s="70" t="s">
+      <c r="HT89" s="77" t="s">
         <v>129</v>
       </c>
-      <c r="HU89" s="70"/>
-      <c r="HV89" s="70"/>
-      <c r="HW89" s="70"/>
-      <c r="HX89" s="70"/>
-      <c r="HY89" s="70"/>
-      <c r="HZ89" s="70"/>
-      <c r="IA89" s="70"/>
+      <c r="HU89" s="77"/>
+      <c r="HV89" s="77"/>
+      <c r="HW89" s="77"/>
+      <c r="HX89" s="77"/>
+      <c r="HY89" s="77"/>
+      <c r="HZ89" s="77"/>
+      <c r="IA89" s="77"/>
       <c r="IQ89" s="57"/>
       <c r="IR89" s="8"/>
       <c r="IS89" s="8"/>
@@ -51600,14 +51600,14 @@
       <c r="JL89" s="55"/>
       <c r="JM89" s="31"/>
       <c r="JN89" s="31"/>
-      <c r="JO89" s="73"/>
-      <c r="JP89" s="73"/>
-      <c r="JQ89" s="73"/>
-      <c r="JR89" s="73"/>
-      <c r="JS89" s="73"/>
-      <c r="JT89" s="73"/>
-      <c r="JU89" s="73"/>
-      <c r="JV89" s="73"/>
+      <c r="JO89" s="76"/>
+      <c r="JP89" s="76"/>
+      <c r="JQ89" s="76"/>
+      <c r="JR89" s="76"/>
+      <c r="JS89" s="76"/>
+      <c r="JT89" s="76"/>
+      <c r="JU89" s="76"/>
+      <c r="JV89" s="76"/>
       <c r="JW89" s="29"/>
       <c r="JX89" s="29"/>
       <c r="JY89" s="8"/>
@@ -51620,30 +51620,30 @@
       <c r="KF89" s="8"/>
       <c r="KG89" s="8"/>
       <c r="KH89" s="8"/>
-      <c r="KI89" s="70" t="s">
+      <c r="KI89" s="77" t="s">
         <v>97</v>
       </c>
-      <c r="KJ89" s="70"/>
-      <c r="KK89" s="70"/>
-      <c r="KL89" s="70"/>
-      <c r="KM89" s="70"/>
-      <c r="KN89" s="70"/>
+      <c r="KJ89" s="77"/>
+      <c r="KK89" s="77"/>
+      <c r="KL89" s="77"/>
+      <c r="KM89" s="77"/>
+      <c r="KN89" s="77"/>
       <c r="KQ89" s="52" t="s">
         <v>98</v>
       </c>
       <c r="KS89" s="53" t="s">
         <v>135</v>
       </c>
-      <c r="KV89" s="70" t="s">
+      <c r="KV89" s="77" t="s">
         <v>136</v>
       </c>
-      <c r="KW89" s="70"/>
-      <c r="KX89" s="70"/>
-      <c r="KY89" s="70"/>
-      <c r="KZ89" s="70"/>
-      <c r="LA89" s="70"/>
-      <c r="LB89" s="70"/>
-      <c r="LC89" s="70"/>
+      <c r="KW89" s="77"/>
+      <c r="KX89" s="77"/>
+      <c r="KY89" s="77"/>
+      <c r="KZ89" s="77"/>
+      <c r="LA89" s="77"/>
+      <c r="LB89" s="77"/>
+      <c r="LC89" s="77"/>
     </row>
     <row r="90" spans="1:327" ht="16" customHeight="1">
       <c r="J90" s="71" t="s">
@@ -52013,22 +52013,22 @@
       </c>
     </row>
     <row r="93" spans="1:327" ht="20">
-      <c r="L93" s="70" t="s">
+      <c r="L93" s="77" t="s">
         <v>35</v>
       </c>
-      <c r="M93" s="70"/>
-      <c r="N93" s="70"/>
-      <c r="O93" s="70"/>
-      <c r="P93" s="70"/>
-      <c r="Q93" s="70"/>
-      <c r="EE93" s="70" t="s">
+      <c r="M93" s="77"/>
+      <c r="N93" s="77"/>
+      <c r="O93" s="77"/>
+      <c r="P93" s="77"/>
+      <c r="Q93" s="77"/>
+      <c r="EE93" s="77" t="s">
         <v>115</v>
       </c>
-      <c r="EF93" s="70"/>
-      <c r="EG93" s="70"/>
-      <c r="EH93" s="70"/>
-      <c r="EI93" s="70"/>
-      <c r="EJ93" s="70"/>
+      <c r="EF93" s="77"/>
+      <c r="EG93" s="77"/>
+      <c r="EH93" s="77"/>
+      <c r="EI93" s="77"/>
+      <c r="EJ93" s="77"/>
       <c r="EM93" s="53" t="s">
         <v>137</v>
       </c>
@@ -52037,25 +52037,25 @@
       <c r="EP93" s="53"/>
       <c r="EQ93" s="53"/>
       <c r="ER93" s="53"/>
-      <c r="HG93" s="70" t="s">
+      <c r="HG93" s="77" t="s">
         <v>126</v>
       </c>
-      <c r="HH93" s="70"/>
-      <c r="HI93" s="70"/>
-      <c r="HJ93" s="70"/>
-      <c r="HK93" s="70"/>
-      <c r="HL93" s="70"/>
+      <c r="HH93" s="77"/>
+      <c r="HI93" s="77"/>
+      <c r="HJ93" s="77"/>
+      <c r="HK93" s="77"/>
+      <c r="HL93" s="77"/>
       <c r="HO93" s="53" t="s">
         <v>138</v>
       </c>
-      <c r="KI93" s="70" t="s">
+      <c r="KI93" s="77" t="s">
         <v>99</v>
       </c>
-      <c r="KJ93" s="70"/>
-      <c r="KK93" s="70"/>
-      <c r="KL93" s="70"/>
-      <c r="KM93" s="70"/>
-      <c r="KN93" s="70"/>
+      <c r="KJ93" s="77"/>
+      <c r="KK93" s="77"/>
+      <c r="KL93" s="77"/>
+      <c r="KM93" s="77"/>
+      <c r="KN93" s="77"/>
     </row>
     <row r="96" spans="1:327" ht="47">
       <c r="A96" s="27" t="s">
@@ -53271,17 +53271,17 @@
       </c>
       <c r="D118" s="69"/>
       <c r="E118" s="69"/>
-      <c r="G118" s="70" t="s">
+      <c r="G118" s="77" t="s">
         <v>39</v>
       </c>
-      <c r="H118" s="70"/>
-      <c r="I118" s="70"/>
+      <c r="H118" s="77"/>
+      <c r="I118" s="77"/>
       <c r="J118" s="17"/>
-      <c r="K118" s="70" t="s">
+      <c r="K118" s="77" t="s">
         <v>40</v>
       </c>
-      <c r="L118" s="70"/>
-      <c r="M118" s="70"/>
+      <c r="L118" s="77"/>
+      <c r="M118" s="77"/>
       <c r="N118" s="17"/>
       <c r="O118" s="17" t="s">
         <v>41</v>
@@ -53296,17 +53296,17 @@
       </c>
       <c r="JZ118" s="69"/>
       <c r="KA118" s="69"/>
-      <c r="KC118" s="70" t="s">
+      <c r="KC118" s="77" t="s">
         <v>144</v>
       </c>
-      <c r="KD118" s="70"/>
-      <c r="KE118" s="70"/>
+      <c r="KD118" s="77"/>
+      <c r="KE118" s="77"/>
       <c r="KF118" s="17"/>
-      <c r="KG118" s="70" t="s">
+      <c r="KG118" s="77" t="s">
         <v>149</v>
       </c>
-      <c r="KH118" s="70"/>
-      <c r="KI118" s="70"/>
+      <c r="KH118" s="77"/>
+      <c r="KI118" s="77"/>
       <c r="KJ118" s="17"/>
       <c r="KK118" s="17" t="s">
         <v>150</v>
@@ -53585,28 +53585,133 @@
     </row>
   </sheetData>
   <mergeCells count="173">
-    <mergeCell ref="GH81:GH88"/>
-    <mergeCell ref="HE81:HE88"/>
-    <mergeCell ref="A123:A128"/>
-    <mergeCell ref="A100:A107"/>
-    <mergeCell ref="A110:I110"/>
-    <mergeCell ref="A112:A117"/>
-    <mergeCell ref="C118:E118"/>
-    <mergeCell ref="G118:I118"/>
-    <mergeCell ref="K118:M118"/>
-    <mergeCell ref="ER89:EY89"/>
-    <mergeCell ref="J90:J92"/>
-    <mergeCell ref="EC90:EC92"/>
-    <mergeCell ref="L93:Q93"/>
-    <mergeCell ref="EE93:EJ93"/>
-    <mergeCell ref="A98:I98"/>
-    <mergeCell ref="L89:Q89"/>
-    <mergeCell ref="AH89:AO89"/>
-    <mergeCell ref="AS89:AZ89"/>
-    <mergeCell ref="BD89:BK89"/>
-    <mergeCell ref="DK89:DR89"/>
-    <mergeCell ref="EE89:EJ89"/>
-    <mergeCell ref="BS89:BX89"/>
+    <mergeCell ref="JW98:KE98"/>
+    <mergeCell ref="JW100:JW107"/>
+    <mergeCell ref="JW110:KE110"/>
+    <mergeCell ref="JW112:JW117"/>
+    <mergeCell ref="JY118:KA118"/>
+    <mergeCell ref="KC118:KE118"/>
+    <mergeCell ref="KG118:KI118"/>
+    <mergeCell ref="JW123:JW128"/>
+    <mergeCell ref="JJ81:JJ88"/>
+    <mergeCell ref="KG81:KG88"/>
+    <mergeCell ref="LF81:LF82"/>
+    <mergeCell ref="LH83:LO83"/>
+    <mergeCell ref="JO89:JV89"/>
+    <mergeCell ref="KI89:KN89"/>
+    <mergeCell ref="KV89:LC89"/>
+    <mergeCell ref="KG90:KG92"/>
+    <mergeCell ref="KI93:KN93"/>
+    <mergeCell ref="LH85:LO85"/>
+    <mergeCell ref="KY59:LF59"/>
+    <mergeCell ref="KP59:KR59"/>
+    <mergeCell ref="JJ61:JJ66"/>
+    <mergeCell ref="KY62:LF62"/>
+    <mergeCell ref="JO67:JT67"/>
+    <mergeCell ref="JX67:KE67"/>
+    <mergeCell ref="JO79:JV79"/>
+    <mergeCell ref="KI79:KN79"/>
+    <mergeCell ref="KV79:LC79"/>
+    <mergeCell ref="LH79:LO79"/>
+    <mergeCell ref="JV61:JV66"/>
+    <mergeCell ref="KP67:KR67"/>
+    <mergeCell ref="JL40:JM40"/>
+    <mergeCell ref="KI40:KN40"/>
+    <mergeCell ref="IU42:IU49"/>
+    <mergeCell ref="JJ42:JJ49"/>
+    <mergeCell ref="IW50:IX50"/>
+    <mergeCell ref="IZ50:JE50"/>
+    <mergeCell ref="KI50:KN50"/>
+    <mergeCell ref="JO59:JT59"/>
+    <mergeCell ref="JX59:KE59"/>
+    <mergeCell ref="KG42:KG49"/>
+    <mergeCell ref="KG51:KG53"/>
+    <mergeCell ref="KI54:KN54"/>
+    <mergeCell ref="KI56:KN56"/>
+    <mergeCell ref="ID81:ID82"/>
+    <mergeCell ref="IF83:IM83"/>
+    <mergeCell ref="GM89:GT89"/>
+    <mergeCell ref="HG89:HL89"/>
+    <mergeCell ref="HT89:IA89"/>
+    <mergeCell ref="HE90:HE92"/>
+    <mergeCell ref="HG93:HL93"/>
+    <mergeCell ref="IW40:IX40"/>
+    <mergeCell ref="IZ40:JE40"/>
+    <mergeCell ref="GJ40:GO40"/>
+    <mergeCell ref="GJ50:GO50"/>
+    <mergeCell ref="HW59:ID59"/>
+    <mergeCell ref="GM79:GT79"/>
+    <mergeCell ref="HG79:HL79"/>
+    <mergeCell ref="HT79:IA79"/>
+    <mergeCell ref="IF79:IM79"/>
+    <mergeCell ref="HW62:ID62"/>
+    <mergeCell ref="GM67:GR67"/>
+    <mergeCell ref="GV67:HC67"/>
+    <mergeCell ref="GM59:GR59"/>
+    <mergeCell ref="GV59:HC59"/>
+    <mergeCell ref="CV40:DA40"/>
+    <mergeCell ref="CV50:DA50"/>
+    <mergeCell ref="FU40:FV40"/>
+    <mergeCell ref="FX40:GC40"/>
+    <mergeCell ref="HG40:HL40"/>
+    <mergeCell ref="FS42:FS49"/>
+    <mergeCell ref="FU50:FV50"/>
+    <mergeCell ref="FX50:GC50"/>
+    <mergeCell ref="HG50:HL50"/>
+    <mergeCell ref="DH40:DM40"/>
+    <mergeCell ref="DH50:DM50"/>
+    <mergeCell ref="EE50:EJ50"/>
+    <mergeCell ref="CQ42:CQ49"/>
+    <mergeCell ref="DF42:DF49"/>
+    <mergeCell ref="A72:A73"/>
+    <mergeCell ref="C74:J74"/>
+    <mergeCell ref="Z74:AB74"/>
+    <mergeCell ref="AH74:AI74"/>
+    <mergeCell ref="AK74:AL74"/>
+    <mergeCell ref="AS74:AZ74"/>
+    <mergeCell ref="DT59:EA59"/>
+    <mergeCell ref="Z59:AB59"/>
+    <mergeCell ref="AH59:AM59"/>
+    <mergeCell ref="AS70:AZ70"/>
+    <mergeCell ref="L50:Q50"/>
+    <mergeCell ref="W50:X50"/>
+    <mergeCell ref="A42:A49"/>
+    <mergeCell ref="U42:U49"/>
+    <mergeCell ref="J51:J53"/>
+    <mergeCell ref="L54:Q54"/>
+    <mergeCell ref="Z70:AB70"/>
+    <mergeCell ref="AH70:AI70"/>
+    <mergeCell ref="AK70:AL70"/>
+    <mergeCell ref="A61:A66"/>
+    <mergeCell ref="L71:Q71"/>
+    <mergeCell ref="L56:Q56"/>
+    <mergeCell ref="GH61:GH66"/>
+    <mergeCell ref="AS59:AZ59"/>
+    <mergeCell ref="BD59:BK59"/>
+    <mergeCell ref="AH50:AO50"/>
+    <mergeCell ref="AS50:AX50"/>
+    <mergeCell ref="BD50:BI50"/>
+    <mergeCell ref="CS50:CT50"/>
+    <mergeCell ref="BS50:BX50"/>
+    <mergeCell ref="BZ50:CG50"/>
+    <mergeCell ref="EU59:FB59"/>
+    <mergeCell ref="DF61:DF66"/>
+    <mergeCell ref="EU62:FB62"/>
+    <mergeCell ref="DK59:DP59"/>
+    <mergeCell ref="BS59:BX59"/>
+    <mergeCell ref="C26:E26"/>
+    <mergeCell ref="A28:A35"/>
+    <mergeCell ref="C36:E36"/>
+    <mergeCell ref="BL38:CJ38"/>
+    <mergeCell ref="C40:J40"/>
+    <mergeCell ref="L40:Q40"/>
+    <mergeCell ref="W40:X40"/>
+    <mergeCell ref="AH40:AO40"/>
+    <mergeCell ref="AS40:AX40"/>
+    <mergeCell ref="BD40:BI40"/>
+    <mergeCell ref="BS40:BX40"/>
+    <mergeCell ref="BZ40:CG40"/>
+    <mergeCell ref="CI40:CJ40"/>
     <mergeCell ref="CS40:CT40"/>
     <mergeCell ref="EE40:EJ40"/>
     <mergeCell ref="C76:J76"/>
@@ -53631,133 +53736,28 @@
     <mergeCell ref="BS79:BX79"/>
     <mergeCell ref="DK67:DP67"/>
     <mergeCell ref="DT67:EA67"/>
-    <mergeCell ref="C26:E26"/>
-    <mergeCell ref="A28:A35"/>
-    <mergeCell ref="C36:E36"/>
-    <mergeCell ref="BL38:CJ38"/>
-    <mergeCell ref="C40:J40"/>
-    <mergeCell ref="L40:Q40"/>
-    <mergeCell ref="W40:X40"/>
-    <mergeCell ref="AH40:AO40"/>
-    <mergeCell ref="AS40:AX40"/>
-    <mergeCell ref="BD40:BI40"/>
-    <mergeCell ref="BS40:BX40"/>
-    <mergeCell ref="BZ40:CG40"/>
-    <mergeCell ref="CI40:CJ40"/>
-    <mergeCell ref="GH61:GH66"/>
-    <mergeCell ref="AS59:AZ59"/>
-    <mergeCell ref="BD59:BK59"/>
-    <mergeCell ref="AH50:AO50"/>
-    <mergeCell ref="AS50:AX50"/>
-    <mergeCell ref="BD50:BI50"/>
-    <mergeCell ref="CS50:CT50"/>
-    <mergeCell ref="BS50:BX50"/>
-    <mergeCell ref="BZ50:CG50"/>
-    <mergeCell ref="EU59:FB59"/>
-    <mergeCell ref="DF61:DF66"/>
-    <mergeCell ref="EU62:FB62"/>
-    <mergeCell ref="DK59:DP59"/>
-    <mergeCell ref="BS59:BX59"/>
-    <mergeCell ref="CQ42:CQ49"/>
-    <mergeCell ref="DF42:DF49"/>
-    <mergeCell ref="A72:A73"/>
-    <mergeCell ref="C74:J74"/>
-    <mergeCell ref="Z74:AB74"/>
-    <mergeCell ref="AH74:AI74"/>
-    <mergeCell ref="AK74:AL74"/>
-    <mergeCell ref="AS74:AZ74"/>
-    <mergeCell ref="DT59:EA59"/>
-    <mergeCell ref="Z59:AB59"/>
-    <mergeCell ref="AH59:AM59"/>
-    <mergeCell ref="AS70:AZ70"/>
-    <mergeCell ref="L50:Q50"/>
-    <mergeCell ref="W50:X50"/>
-    <mergeCell ref="A42:A49"/>
-    <mergeCell ref="U42:U49"/>
-    <mergeCell ref="J51:J53"/>
-    <mergeCell ref="L54:Q54"/>
-    <mergeCell ref="Z70:AB70"/>
-    <mergeCell ref="AH70:AI70"/>
-    <mergeCell ref="AK70:AL70"/>
-    <mergeCell ref="A61:A66"/>
-    <mergeCell ref="L71:Q71"/>
-    <mergeCell ref="L56:Q56"/>
-    <mergeCell ref="CV40:DA40"/>
-    <mergeCell ref="CV50:DA50"/>
-    <mergeCell ref="FU40:FV40"/>
-    <mergeCell ref="FX40:GC40"/>
-    <mergeCell ref="HG40:HL40"/>
-    <mergeCell ref="FS42:FS49"/>
-    <mergeCell ref="FU50:FV50"/>
-    <mergeCell ref="FX50:GC50"/>
-    <mergeCell ref="HG50:HL50"/>
-    <mergeCell ref="DH40:DM40"/>
-    <mergeCell ref="DH50:DM50"/>
-    <mergeCell ref="EE50:EJ50"/>
-    <mergeCell ref="ID81:ID82"/>
-    <mergeCell ref="IF83:IM83"/>
-    <mergeCell ref="GM89:GT89"/>
-    <mergeCell ref="HG89:HL89"/>
-    <mergeCell ref="HT89:IA89"/>
-    <mergeCell ref="HE90:HE92"/>
-    <mergeCell ref="HG93:HL93"/>
-    <mergeCell ref="IW40:IX40"/>
-    <mergeCell ref="IZ40:JE40"/>
-    <mergeCell ref="GJ40:GO40"/>
-    <mergeCell ref="GJ50:GO50"/>
-    <mergeCell ref="HW59:ID59"/>
-    <mergeCell ref="GM79:GT79"/>
-    <mergeCell ref="HG79:HL79"/>
-    <mergeCell ref="HT79:IA79"/>
-    <mergeCell ref="IF79:IM79"/>
-    <mergeCell ref="HW62:ID62"/>
-    <mergeCell ref="GM67:GR67"/>
-    <mergeCell ref="GV67:HC67"/>
-    <mergeCell ref="GM59:GR59"/>
-    <mergeCell ref="GV59:HC59"/>
-    <mergeCell ref="JL40:JM40"/>
-    <mergeCell ref="KI40:KN40"/>
-    <mergeCell ref="IU42:IU49"/>
-    <mergeCell ref="JJ42:JJ49"/>
-    <mergeCell ref="IW50:IX50"/>
-    <mergeCell ref="IZ50:JE50"/>
-    <mergeCell ref="KI50:KN50"/>
-    <mergeCell ref="JO59:JT59"/>
-    <mergeCell ref="JX59:KE59"/>
-    <mergeCell ref="KG42:KG49"/>
-    <mergeCell ref="KG51:KG53"/>
-    <mergeCell ref="KI54:KN54"/>
-    <mergeCell ref="KI56:KN56"/>
-    <mergeCell ref="JJ61:JJ66"/>
-    <mergeCell ref="KY62:LF62"/>
-    <mergeCell ref="JO67:JT67"/>
-    <mergeCell ref="JX67:KE67"/>
-    <mergeCell ref="JO79:JV79"/>
-    <mergeCell ref="KI79:KN79"/>
-    <mergeCell ref="KV79:LC79"/>
-    <mergeCell ref="LH79:LO79"/>
-    <mergeCell ref="JV61:JV66"/>
-    <mergeCell ref="KP67:KR67"/>
-    <mergeCell ref="LF81:LF82"/>
-    <mergeCell ref="LH83:LO83"/>
-    <mergeCell ref="JO89:JV89"/>
-    <mergeCell ref="KI89:KN89"/>
-    <mergeCell ref="KV89:LC89"/>
-    <mergeCell ref="KG90:KG92"/>
-    <mergeCell ref="KI93:KN93"/>
-    <mergeCell ref="LH85:LO85"/>
-    <mergeCell ref="KY59:LF59"/>
-    <mergeCell ref="KP59:KR59"/>
-    <mergeCell ref="JW98:KE98"/>
-    <mergeCell ref="JW100:JW107"/>
-    <mergeCell ref="JW110:KE110"/>
-    <mergeCell ref="JW112:JW117"/>
-    <mergeCell ref="JY118:KA118"/>
-    <mergeCell ref="KC118:KE118"/>
-    <mergeCell ref="KG118:KI118"/>
-    <mergeCell ref="JW123:JW128"/>
-    <mergeCell ref="JJ81:JJ88"/>
-    <mergeCell ref="KG81:KG88"/>
+    <mergeCell ref="GH81:GH88"/>
+    <mergeCell ref="HE81:HE88"/>
+    <mergeCell ref="A123:A128"/>
+    <mergeCell ref="A100:A107"/>
+    <mergeCell ref="A110:I110"/>
+    <mergeCell ref="A112:A117"/>
+    <mergeCell ref="C118:E118"/>
+    <mergeCell ref="G118:I118"/>
+    <mergeCell ref="K118:M118"/>
+    <mergeCell ref="ER89:EY89"/>
+    <mergeCell ref="J90:J92"/>
+    <mergeCell ref="EC90:EC92"/>
+    <mergeCell ref="L93:Q93"/>
+    <mergeCell ref="EE93:EJ93"/>
+    <mergeCell ref="A98:I98"/>
+    <mergeCell ref="L89:Q89"/>
+    <mergeCell ref="AH89:AO89"/>
+    <mergeCell ref="AS89:AZ89"/>
+    <mergeCell ref="BD89:BK89"/>
+    <mergeCell ref="DK89:DR89"/>
+    <mergeCell ref="EE89:EJ89"/>
+    <mergeCell ref="BS89:BX89"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -53770,7 +53770,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81DB1CE6-E3EC-7B4E-8832-2A8872C682BA}">
   <dimension ref="A1:J21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Eliminating .csv files. Reading from .xlsx files directly.
</commit_message>
<xml_diff>
--- a/inst/extdata/PerfectSubstitutionraw/UTEI_Sankey_Simple_ECC_Perfect_Sub.xlsx
+++ b/inst/extdata/PerfectSubstitutionraw/UTEI_Sankey_Simple_ECC_Perfect_Sub.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11109"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mkh2/github/Recca/inst/extdata/PerfectSubstitutionraw/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matt/github/Recca/inst/extdata/PerfectSubstitutionraw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A39AC02-0FAA-C344-A179-FC0EFD04C3AB}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61524CCD-45FA-FF45-A47A-92231EF698CF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20680" yWindow="440" windowWidth="26200" windowHeight="17560" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20680" yWindow="460" windowWidth="26200" windowHeight="17560" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Meta" sheetId="10" r:id="rId1"/>
@@ -19,6 +19,16 @@
     <sheet name="PerfectSubstitutionRaw" sheetId="11" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -5323,9 +5333,6 @@
     <t>Product</t>
   </si>
   <si>
-    <t>EX.ktoe</t>
-  </si>
-  <si>
     <t>Unit</t>
   </si>
   <si>
@@ -5333,9 +5340,6 @@
   </si>
   <si>
     <t>Total primary energy supply</t>
-  </si>
-  <si>
-    <t>E.ktoe</t>
   </si>
   <si>
     <t>Resources - Rens</t>
@@ -5354,9 +5358,6 @@
   </si>
   <si>
     <t>Consumption</t>
-  </si>
-  <si>
-    <t>services</t>
   </si>
   <si>
     <t>Commercial and public services</t>
@@ -5992,6 +5993,15 @@
       </rPr>
       <t>f_hat</t>
     </r>
+  </si>
+  <si>
+    <t>Services</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>E.dot</t>
   </si>
 </sst>
 </file>
@@ -6859,7 +6869,7 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -6868,28 +6878,28 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -30459,7 +30469,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{338BDA73-949D-6141-997A-6445BD9150B1}">
   <dimension ref="A1:CO144"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="AW56" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="AW56" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="BT50" sqref="BT50:BY50"/>
     </sheetView>
   </sheetViews>
@@ -30640,11 +30650,11 @@
     </row>
     <row r="26" spans="1:93">
       <c r="B26" s="10"/>
-      <c r="C26" s="70" t="s">
+      <c r="C26" s="76" t="s">
         <v>30</v>
       </c>
-      <c r="D26" s="70"/>
-      <c r="E26" s="70"/>
+      <c r="D26" s="76"/>
+      <c r="E26" s="76"/>
       <c r="F26" s="39"/>
       <c r="G26" s="39"/>
     </row>
@@ -30913,11 +30923,11 @@
       <c r="CO35" s="31"/>
     </row>
     <row r="36" spans="1:93" ht="18">
-      <c r="C36" s="70" t="s">
+      <c r="C36" s="76" t="s">
         <v>31</v>
       </c>
-      <c r="D36" s="70"/>
-      <c r="E36" s="70"/>
+      <c r="D36" s="76"/>
+      <c r="E36" s="76"/>
       <c r="F36" s="39"/>
       <c r="G36" s="39"/>
       <c r="BM36" s="31"/>
@@ -31135,7 +31145,7 @@
       </c>
       <c r="V41" s="28"/>
       <c r="W41" s="2" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="X41" s="2" t="s">
         <v>58</v>
@@ -31243,7 +31253,7 @@
         <v>18</v>
       </c>
       <c r="CJ41" s="2" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="CK41" s="2" t="s">
         <v>58</v>
@@ -33051,14 +33061,14 @@
       <c r="AA53" s="15"/>
     </row>
     <row r="54" spans="1:93" ht="20">
-      <c r="L54" s="73" t="s">
+      <c r="L54" s="74" t="s">
         <v>42</v>
       </c>
-      <c r="M54" s="73"/>
-      <c r="N54" s="73"/>
-      <c r="O54" s="73"/>
-      <c r="P54" s="73"/>
-      <c r="Q54" s="73"/>
+      <c r="M54" s="74"/>
+      <c r="N54" s="74"/>
+      <c r="O54" s="74"/>
+      <c r="P54" s="74"/>
+      <c r="Q54" s="74"/>
     </row>
     <row r="55" spans="1:93">
       <c r="L55" s="6">
@@ -33098,11 +33108,11 @@
     </row>
     <row r="60" spans="1:93">
       <c r="B60" s="1"/>
-      <c r="Z60" s="70" t="s">
+      <c r="Z60" s="76" t="s">
         <v>30</v>
       </c>
-      <c r="AA60" s="70"/>
-      <c r="AB60" s="70"/>
+      <c r="AA60" s="76"/>
+      <c r="AB60" s="76"/>
       <c r="AI60" s="69" t="s">
         <v>3</v>
       </c>
@@ -34238,11 +34248,11 @@
       <c r="J68" s="69"/>
       <c r="X68" s="15"/>
       <c r="Y68" s="15"/>
-      <c r="Z68" s="73" t="s">
+      <c r="Z68" s="74" t="s">
         <v>69</v>
       </c>
-      <c r="AA68" s="73"/>
-      <c r="AB68" s="73"/>
+      <c r="AA68" s="74"/>
+      <c r="AB68" s="74"/>
       <c r="AD68" s="34" t="s">
         <v>71</v>
       </c>
@@ -34448,17 +34458,17 @@
       <c r="W73" s="15"/>
       <c r="X73" s="15"/>
       <c r="Y73" s="15"/>
-      <c r="Z73" s="70" t="s">
+      <c r="Z73" s="76" t="s">
         <v>30</v>
       </c>
-      <c r="AA73" s="70"/>
-      <c r="AI73" s="74" t="s">
+      <c r="AA73" s="76"/>
+      <c r="AI73" s="77" t="s">
         <v>52</v>
       </c>
-      <c r="AJ73" s="74"/>
+      <c r="AJ73" s="77"/>
       <c r="AK73" s="31"/>
-      <c r="AL73" s="74"/>
-      <c r="AM73" s="74"/>
+      <c r="AL73" s="77"/>
+      <c r="AM73" s="77"/>
       <c r="AN73" s="31"/>
       <c r="AO73" s="31"/>
       <c r="AP73" s="31"/>
@@ -34782,29 +34792,29 @@
       <c r="AC77" s="41" t="s">
         <v>53</v>
       </c>
-      <c r="AI77" s="76" t="s">
+      <c r="AI77" s="73" t="s">
         <v>64</v>
       </c>
-      <c r="AJ77" s="76"/>
+      <c r="AJ77" s="73"/>
       <c r="AK77" s="29"/>
-      <c r="AL77" s="76"/>
-      <c r="AM77" s="76"/>
+      <c r="AL77" s="73"/>
+      <c r="AM77" s="73"/>
       <c r="AN77" s="29"/>
       <c r="AO77" s="31"/>
       <c r="AP77" s="31"/>
       <c r="AQ77" s="31"/>
       <c r="AR77" s="31"/>
       <c r="AS77" s="31"/>
-      <c r="AT77" s="76" t="s">
+      <c r="AT77" s="73" t="s">
         <v>65</v>
       </c>
-      <c r="AU77" s="76"/>
-      <c r="AV77" s="76"/>
-      <c r="AW77" s="76"/>
-      <c r="AX77" s="76"/>
-      <c r="AY77" s="76"/>
-      <c r="AZ77" s="76"/>
-      <c r="BA77" s="76"/>
+      <c r="AU77" s="73"/>
+      <c r="AV77" s="73"/>
+      <c r="AW77" s="73"/>
+      <c r="AX77" s="73"/>
+      <c r="AY77" s="73"/>
+      <c r="AZ77" s="73"/>
+      <c r="BA77" s="73"/>
     </row>
     <row r="78" spans="1:78">
       <c r="B78" s="1"/>
@@ -34904,16 +34914,16 @@
       </c>
     </row>
     <row r="81" spans="1:93" ht="16" customHeight="1">
-      <c r="C81" s="77" t="s">
+      <c r="C81" s="70" t="s">
         <v>85</v>
       </c>
-      <c r="D81" s="77"/>
-      <c r="E81" s="77"/>
-      <c r="F81" s="77"/>
-      <c r="G81" s="77"/>
-      <c r="H81" s="77"/>
-      <c r="I81" s="77"/>
-      <c r="J81" s="77"/>
+      <c r="D81" s="70"/>
+      <c r="E81" s="70"/>
+      <c r="F81" s="70"/>
+      <c r="G81" s="70"/>
+      <c r="H81" s="70"/>
+      <c r="I81" s="70"/>
+      <c r="J81" s="70"/>
       <c r="AI81" s="69" t="s">
         <v>4</v>
       </c>
@@ -36329,14 +36339,14 @@
       </c>
     </row>
     <row r="91" spans="1:93" ht="19">
-      <c r="L91" s="77" t="s">
+      <c r="L91" s="70" t="s">
         <v>13</v>
       </c>
-      <c r="M91" s="77"/>
-      <c r="N91" s="77"/>
-      <c r="O91" s="77"/>
-      <c r="P91" s="77"/>
-      <c r="Q91" s="77"/>
+      <c r="M91" s="70"/>
+      <c r="N91" s="70"/>
+      <c r="O91" s="70"/>
+      <c r="P91" s="70"/>
+      <c r="Q91" s="70"/>
       <c r="Z91" s="41" t="s">
         <v>11</v>
       </c>
@@ -36489,14 +36499,14 @@
       <c r="AA94" s="17"/>
     </row>
     <row r="95" spans="1:93" ht="20">
-      <c r="L95" s="77" t="s">
+      <c r="L95" s="70" t="s">
         <v>35</v>
       </c>
-      <c r="M95" s="77"/>
-      <c r="N95" s="77"/>
-      <c r="O95" s="77"/>
-      <c r="P95" s="77"/>
-      <c r="Q95" s="77"/>
+      <c r="M95" s="70"/>
+      <c r="N95" s="70"/>
+      <c r="O95" s="70"/>
+      <c r="P95" s="70"/>
+      <c r="Q95" s="70"/>
     </row>
     <row r="98" spans="1:40" ht="47">
       <c r="A98" s="27" t="s">
@@ -37117,16 +37127,16 @@
       </c>
       <c r="D120" s="69"/>
       <c r="E120" s="69"/>
-      <c r="G120" s="77" t="s">
+      <c r="G120" s="70" t="s">
         <v>39</v>
       </c>
-      <c r="H120" s="77"/>
-      <c r="I120" s="77"/>
-      <c r="K120" s="77" t="s">
+      <c r="H120" s="70"/>
+      <c r="I120" s="70"/>
+      <c r="K120" s="70" t="s">
         <v>40</v>
       </c>
-      <c r="L120" s="77"/>
-      <c r="M120" s="77"/>
+      <c r="L120" s="70"/>
+      <c r="M120" s="70"/>
       <c r="N120" s="17"/>
       <c r="O120" s="17" t="s">
         <v>41</v>
@@ -37550,65 +37560,6 @@
     </row>
   </sheetData>
   <mergeCells count="71">
-    <mergeCell ref="A112:I112"/>
-    <mergeCell ref="C143:H143"/>
-    <mergeCell ref="C120:E120"/>
-    <mergeCell ref="G120:I120"/>
-    <mergeCell ref="K120:M120"/>
-    <mergeCell ref="A125:A130"/>
-    <mergeCell ref="C135:H135"/>
-    <mergeCell ref="A137:A142"/>
-    <mergeCell ref="A114:A119"/>
-    <mergeCell ref="BE81:BL81"/>
-    <mergeCell ref="BT81:BY81"/>
-    <mergeCell ref="A83:A90"/>
-    <mergeCell ref="L91:Q91"/>
-    <mergeCell ref="AI91:AP91"/>
-    <mergeCell ref="AT91:BA91"/>
-    <mergeCell ref="BE91:BL91"/>
-    <mergeCell ref="BT91:BY91"/>
-    <mergeCell ref="C81:J81"/>
-    <mergeCell ref="AI81:AP81"/>
-    <mergeCell ref="AT81:BA81"/>
-    <mergeCell ref="J92:J94"/>
-    <mergeCell ref="L95:Q95"/>
-    <mergeCell ref="A100:I100"/>
-    <mergeCell ref="A102:A109"/>
-    <mergeCell ref="C77:J77"/>
-    <mergeCell ref="AI77:AJ77"/>
-    <mergeCell ref="AL77:AM77"/>
-    <mergeCell ref="AT77:BA77"/>
-    <mergeCell ref="C79:J79"/>
-    <mergeCell ref="A75:A76"/>
-    <mergeCell ref="C68:J68"/>
-    <mergeCell ref="Z68:AB68"/>
-    <mergeCell ref="AI68:AN68"/>
-    <mergeCell ref="AT68:BA68"/>
-    <mergeCell ref="C70:J70"/>
-    <mergeCell ref="Z73:AA73"/>
-    <mergeCell ref="AI73:AJ73"/>
-    <mergeCell ref="AL73:AM73"/>
-    <mergeCell ref="AT73:BA73"/>
-    <mergeCell ref="BE68:BL68"/>
-    <mergeCell ref="BT68:BY68"/>
-    <mergeCell ref="Z60:AB60"/>
-    <mergeCell ref="AI60:AN60"/>
-    <mergeCell ref="AT60:BA60"/>
-    <mergeCell ref="BE60:BL60"/>
-    <mergeCell ref="BT60:BY60"/>
-    <mergeCell ref="A62:A67"/>
-    <mergeCell ref="BE50:BJ50"/>
-    <mergeCell ref="BT50:BY50"/>
-    <mergeCell ref="CA50:CH50"/>
-    <mergeCell ref="J51:J53"/>
-    <mergeCell ref="L54:Q54"/>
-    <mergeCell ref="L56:Q56"/>
-    <mergeCell ref="AT50:AY50"/>
-    <mergeCell ref="A42:A49"/>
-    <mergeCell ref="U42:U49"/>
-    <mergeCell ref="L50:Q50"/>
-    <mergeCell ref="W50:X50"/>
-    <mergeCell ref="AI50:AP50"/>
     <mergeCell ref="CJ40:CK40"/>
     <mergeCell ref="C26:E26"/>
     <mergeCell ref="A28:A35"/>
@@ -37621,6 +37572,65 @@
     <mergeCell ref="BE40:BJ40"/>
     <mergeCell ref="BT40:BY40"/>
     <mergeCell ref="CA40:CH40"/>
+    <mergeCell ref="A42:A49"/>
+    <mergeCell ref="U42:U49"/>
+    <mergeCell ref="L50:Q50"/>
+    <mergeCell ref="W50:X50"/>
+    <mergeCell ref="AI50:AP50"/>
+    <mergeCell ref="A62:A67"/>
+    <mergeCell ref="BE50:BJ50"/>
+    <mergeCell ref="BT50:BY50"/>
+    <mergeCell ref="CA50:CH50"/>
+    <mergeCell ref="J51:J53"/>
+    <mergeCell ref="L54:Q54"/>
+    <mergeCell ref="L56:Q56"/>
+    <mergeCell ref="AT50:AY50"/>
+    <mergeCell ref="BT68:BY68"/>
+    <mergeCell ref="Z60:AB60"/>
+    <mergeCell ref="AI60:AN60"/>
+    <mergeCell ref="AT60:BA60"/>
+    <mergeCell ref="BE60:BL60"/>
+    <mergeCell ref="BT60:BY60"/>
+    <mergeCell ref="Z73:AA73"/>
+    <mergeCell ref="AI73:AJ73"/>
+    <mergeCell ref="AL73:AM73"/>
+    <mergeCell ref="AT73:BA73"/>
+    <mergeCell ref="BE68:BL68"/>
+    <mergeCell ref="C68:J68"/>
+    <mergeCell ref="Z68:AB68"/>
+    <mergeCell ref="AI68:AN68"/>
+    <mergeCell ref="AT68:BA68"/>
+    <mergeCell ref="C70:J70"/>
+    <mergeCell ref="AI77:AJ77"/>
+    <mergeCell ref="AL77:AM77"/>
+    <mergeCell ref="AT77:BA77"/>
+    <mergeCell ref="C79:J79"/>
+    <mergeCell ref="A75:A76"/>
+    <mergeCell ref="J92:J94"/>
+    <mergeCell ref="L95:Q95"/>
+    <mergeCell ref="A100:I100"/>
+    <mergeCell ref="A102:A109"/>
+    <mergeCell ref="C77:J77"/>
+    <mergeCell ref="BE81:BL81"/>
+    <mergeCell ref="BT81:BY81"/>
+    <mergeCell ref="A83:A90"/>
+    <mergeCell ref="L91:Q91"/>
+    <mergeCell ref="AI91:AP91"/>
+    <mergeCell ref="AT91:BA91"/>
+    <mergeCell ref="BE91:BL91"/>
+    <mergeCell ref="BT91:BY91"/>
+    <mergeCell ref="C81:J81"/>
+    <mergeCell ref="AI81:AP81"/>
+    <mergeCell ref="AT81:BA81"/>
+    <mergeCell ref="A112:I112"/>
+    <mergeCell ref="C143:H143"/>
+    <mergeCell ref="C120:E120"/>
+    <mergeCell ref="G120:I120"/>
+    <mergeCell ref="K120:M120"/>
+    <mergeCell ref="A125:A130"/>
+    <mergeCell ref="C135:H135"/>
+    <mergeCell ref="A137:A142"/>
+    <mergeCell ref="A114:A119"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -38236,11 +38246,11 @@
     </row>
     <row r="26" spans="1:278">
       <c r="B26" s="10"/>
-      <c r="C26" s="70" t="s">
+      <c r="C26" s="76" t="s">
         <v>30</v>
       </c>
-      <c r="D26" s="70"/>
-      <c r="E26" s="70"/>
+      <c r="D26" s="76"/>
+      <c r="E26" s="76"/>
       <c r="F26" s="47"/>
       <c r="G26" s="47"/>
       <c r="CQ26" t="s">
@@ -38499,11 +38509,11 @@
       <c r="CJ35" s="31"/>
     </row>
     <row r="36" spans="1:302" ht="18">
-      <c r="C36" s="70" t="s">
+      <c r="C36" s="76" t="s">
         <v>31</v>
       </c>
-      <c r="D36" s="70"/>
-      <c r="E36" s="70"/>
+      <c r="D36" s="76"/>
+      <c r="E36" s="76"/>
       <c r="F36" s="47"/>
       <c r="G36" s="47"/>
       <c r="BL36" s="31"/>
@@ -38558,31 +38568,31 @@
       <c r="CJ37" s="51"/>
     </row>
     <row r="38" spans="1:302">
-      <c r="BL38" s="76"/>
-      <c r="BM38" s="76"/>
-      <c r="BN38" s="76"/>
-      <c r="BO38" s="76"/>
-      <c r="BP38" s="76"/>
-      <c r="BQ38" s="76"/>
-      <c r="BR38" s="76"/>
-      <c r="BS38" s="76"/>
-      <c r="BT38" s="76"/>
-      <c r="BU38" s="76"/>
-      <c r="BV38" s="76"/>
-      <c r="BW38" s="76"/>
-      <c r="BX38" s="76"/>
-      <c r="BY38" s="76"/>
-      <c r="BZ38" s="76"/>
-      <c r="CA38" s="76"/>
-      <c r="CB38" s="76"/>
-      <c r="CC38" s="76"/>
-      <c r="CD38" s="76"/>
-      <c r="CE38" s="76"/>
-      <c r="CF38" s="76"/>
-      <c r="CG38" s="76"/>
-      <c r="CH38" s="76"/>
-      <c r="CI38" s="76"/>
-      <c r="CJ38" s="76"/>
+      <c r="BL38" s="73"/>
+      <c r="BM38" s="73"/>
+      <c r="BN38" s="73"/>
+      <c r="BO38" s="73"/>
+      <c r="BP38" s="73"/>
+      <c r="BQ38" s="73"/>
+      <c r="BR38" s="73"/>
+      <c r="BS38" s="73"/>
+      <c r="BT38" s="73"/>
+      <c r="BU38" s="73"/>
+      <c r="BV38" s="73"/>
+      <c r="BW38" s="73"/>
+      <c r="BX38" s="73"/>
+      <c r="BY38" s="73"/>
+      <c r="BZ38" s="73"/>
+      <c r="CA38" s="73"/>
+      <c r="CB38" s="73"/>
+      <c r="CC38" s="73"/>
+      <c r="CD38" s="73"/>
+      <c r="CE38" s="73"/>
+      <c r="CF38" s="73"/>
+      <c r="CG38" s="73"/>
+      <c r="CH38" s="73"/>
+      <c r="CI38" s="73"/>
+      <c r="CJ38" s="73"/>
     </row>
     <row r="40" spans="1:302">
       <c r="C40" s="69" t="s">
@@ -38728,8 +38738,8 @@
       <c r="JC40" s="69"/>
       <c r="JD40" s="69"/>
       <c r="JE40" s="69"/>
-      <c r="JL40" s="76"/>
-      <c r="JM40" s="76"/>
+      <c r="JL40" s="73"/>
+      <c r="JM40" s="73"/>
       <c r="KI40" s="69" t="s">
         <v>3</v>
       </c>
@@ -38784,7 +38794,7 @@
       </c>
       <c r="V41" s="28"/>
       <c r="W41" s="2" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="X41" s="2" t="s">
         <v>58</v>
@@ -38892,7 +38902,7 @@
         <v>18</v>
       </c>
       <c r="CI41" s="2" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="CJ41" s="2" t="s">
         <v>58</v>
@@ -38901,7 +38911,7 @@
       <c r="CL41" s="2"/>
       <c r="CR41" s="28"/>
       <c r="CS41" s="2" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="CT41" s="2" t="s">
         <v>58</v>
@@ -38962,7 +38972,7 @@
       </c>
       <c r="FT41" s="28"/>
       <c r="FU41" s="2" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="FV41" s="2" t="s">
         <v>58</v>
@@ -42357,7 +42367,7 @@
       <c r="BH50" s="69"/>
       <c r="BI50" s="69"/>
       <c r="BS50" s="72" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="BT50" s="72"/>
       <c r="BU50" s="72"/>
@@ -42389,7 +42399,7 @@
       </c>
       <c r="CT50" s="69"/>
       <c r="CV50" s="72" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="CW50" s="72"/>
       <c r="CX50" s="72"/>
@@ -42397,11 +42407,11 @@
       <c r="CZ50" s="72"/>
       <c r="DA50" s="72"/>
       <c r="DC50" s="52" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="DF50" s="31"/>
       <c r="DH50" s="69" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="DI50" s="69"/>
       <c r="DJ50" s="69"/>
@@ -42413,14 +42423,14 @@
       <c r="EB50" s="58"/>
       <c r="EC50" s="58"/>
       <c r="ED50" s="58"/>
-      <c r="EE50" s="79" t="s">
-        <v>193</v>
-      </c>
-      <c r="EF50" s="79"/>
-      <c r="EG50" s="79"/>
-      <c r="EH50" s="79"/>
-      <c r="EI50" s="79"/>
-      <c r="EJ50" s="79"/>
+      <c r="EE50" s="80" t="s">
+        <v>190</v>
+      </c>
+      <c r="EF50" s="80"/>
+      <c r="EG50" s="80"/>
+      <c r="EH50" s="80"/>
+      <c r="EI50" s="80"/>
+      <c r="EJ50" s="80"/>
       <c r="EK50" s="58"/>
       <c r="EL50" s="58"/>
       <c r="EM50" s="58"/>
@@ -42437,7 +42447,7 @@
       </c>
       <c r="FV50" s="69"/>
       <c r="FX50" s="72" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="FY50" s="72"/>
       <c r="FZ50" s="72"/>
@@ -42445,12 +42455,12 @@
       <c r="GB50" s="72"/>
       <c r="GC50" s="72"/>
       <c r="GE50" s="52" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="GH50" s="29"/>
       <c r="GI50" s="29"/>
       <c r="GJ50" s="69" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="GK50" s="69"/>
       <c r="GL50" s="69"/>
@@ -42462,14 +42472,14 @@
       <c r="HD50" s="58"/>
       <c r="HE50" s="58"/>
       <c r="HF50" s="58"/>
-      <c r="HG50" s="79" t="s">
-        <v>192</v>
-      </c>
-      <c r="HH50" s="79"/>
-      <c r="HI50" s="79"/>
-      <c r="HJ50" s="79"/>
-      <c r="HK50" s="79"/>
-      <c r="HL50" s="79"/>
+      <c r="HG50" s="80" t="s">
+        <v>189</v>
+      </c>
+      <c r="HH50" s="80"/>
+      <c r="HI50" s="80"/>
+      <c r="HJ50" s="80"/>
+      <c r="HK50" s="80"/>
+      <c r="HL50" s="80"/>
       <c r="HM50" s="58"/>
       <c r="HN50" s="58"/>
       <c r="HO50" s="58"/>
@@ -42482,15 +42492,15 @@
       <c r="IS50" s="8"/>
       <c r="IT50" s="8"/>
       <c r="IV50" s="31"/>
-      <c r="IW50" s="76"/>
-      <c r="IX50" s="76"/>
+      <c r="IW50" s="73"/>
+      <c r="IX50" s="73"/>
       <c r="IY50" s="31"/>
-      <c r="IZ50" s="79"/>
-      <c r="JA50" s="79"/>
-      <c r="JB50" s="79"/>
-      <c r="JC50" s="79"/>
-      <c r="JD50" s="79"/>
-      <c r="JE50" s="79"/>
+      <c r="IZ50" s="80"/>
+      <c r="JA50" s="80"/>
+      <c r="JB50" s="80"/>
+      <c r="JC50" s="80"/>
+      <c r="JD50" s="80"/>
+      <c r="JE50" s="80"/>
       <c r="JF50" s="31"/>
       <c r="JG50" s="55"/>
       <c r="JH50" s="31"/>
@@ -42504,14 +42514,14 @@
       <c r="KF50" s="58"/>
       <c r="KG50" s="58"/>
       <c r="KH50" s="58"/>
-      <c r="KI50" s="79" t="s">
+      <c r="KI50" s="80" t="s">
         <v>133</v>
       </c>
-      <c r="KJ50" s="79"/>
-      <c r="KK50" s="79"/>
-      <c r="KL50" s="79"/>
-      <c r="KM50" s="79"/>
-      <c r="KN50" s="79"/>
+      <c r="KJ50" s="80"/>
+      <c r="KK50" s="80"/>
+      <c r="KL50" s="80"/>
+      <c r="KM50" s="80"/>
+      <c r="KN50" s="80"/>
       <c r="KO50" s="58"/>
       <c r="KP50" s="59" t="s">
         <v>12</v>
@@ -42826,14 +42836,14 @@
     </row>
     <row r="54" spans="1:319" ht="20">
       <c r="B54" s="1"/>
-      <c r="L54" s="73" t="s">
+      <c r="L54" s="74" t="s">
         <v>42</v>
       </c>
-      <c r="M54" s="73"/>
-      <c r="N54" s="73"/>
-      <c r="O54" s="73"/>
-      <c r="P54" s="73"/>
-      <c r="Q54" s="73"/>
+      <c r="M54" s="74"/>
+      <c r="N54" s="74"/>
+      <c r="O54" s="74"/>
+      <c r="P54" s="74"/>
+      <c r="Q54" s="74"/>
       <c r="R54" s="15"/>
       <c r="S54" s="15"/>
       <c r="T54" s="15"/>
@@ -42861,14 +42871,14 @@
       <c r="JJ54" s="31"/>
       <c r="JK54" s="31"/>
       <c r="JL54" s="31"/>
-      <c r="KI54" s="73" t="s">
+      <c r="KI54" s="74" t="s">
         <v>148</v>
       </c>
-      <c r="KJ54" s="73"/>
-      <c r="KK54" s="73"/>
-      <c r="KL54" s="73"/>
-      <c r="KM54" s="73"/>
-      <c r="KN54" s="73"/>
+      <c r="KJ54" s="74"/>
+      <c r="KK54" s="74"/>
+      <c r="KL54" s="74"/>
+      <c r="KM54" s="74"/>
+      <c r="KN54" s="74"/>
     </row>
     <row r="55" spans="1:319">
       <c r="B55" s="1"/>
@@ -42998,11 +43008,11 @@
     </row>
     <row r="59" spans="1:319">
       <c r="B59" s="1"/>
-      <c r="Z59" s="70" t="s">
+      <c r="Z59" s="76" t="s">
         <v>30</v>
       </c>
-      <c r="AA59" s="70"/>
-      <c r="AB59" s="70"/>
+      <c r="AA59" s="76"/>
+      <c r="AB59" s="76"/>
       <c r="AH59" s="69" t="s">
         <v>3</v>
       </c>
@@ -43061,14 +43071,14 @@
       <c r="EC59" s="45"/>
       <c r="ES59" s="31"/>
       <c r="ET59" s="31"/>
-      <c r="EU59" s="76"/>
-      <c r="EV59" s="76"/>
-      <c r="EW59" s="76"/>
-      <c r="EX59" s="76"/>
-      <c r="EY59" s="76"/>
-      <c r="EZ59" s="76"/>
-      <c r="FA59" s="76"/>
-      <c r="FB59" s="76"/>
+      <c r="EU59" s="73"/>
+      <c r="EV59" s="73"/>
+      <c r="EW59" s="73"/>
+      <c r="EX59" s="73"/>
+      <c r="EY59" s="73"/>
+      <c r="EZ59" s="73"/>
+      <c r="FA59" s="73"/>
+      <c r="FB59" s="73"/>
       <c r="FC59" s="31"/>
       <c r="GM59" s="69" t="s">
         <v>3</v>
@@ -43092,26 +43102,26 @@
       <c r="HE59" s="52"/>
       <c r="HU59" s="31"/>
       <c r="HV59" s="31"/>
-      <c r="HW59" s="76"/>
-      <c r="HX59" s="76"/>
-      <c r="HY59" s="76"/>
-      <c r="HZ59" s="76"/>
-      <c r="IA59" s="76"/>
-      <c r="IB59" s="76"/>
-      <c r="IC59" s="76"/>
-      <c r="ID59" s="76"/>
+      <c r="HW59" s="73"/>
+      <c r="HX59" s="73"/>
+      <c r="HY59" s="73"/>
+      <c r="HZ59" s="73"/>
+      <c r="IA59" s="73"/>
+      <c r="IB59" s="73"/>
+      <c r="IC59" s="73"/>
+      <c r="ID59" s="73"/>
       <c r="IE59" s="31"/>
       <c r="JJ59" s="31"/>
       <c r="JK59" s="31"/>
       <c r="JL59" s="31"/>
       <c r="JM59" s="31"/>
       <c r="JN59" s="31"/>
-      <c r="JO59" s="76"/>
-      <c r="JP59" s="76"/>
-      <c r="JQ59" s="76"/>
-      <c r="JR59" s="76"/>
-      <c r="JS59" s="76"/>
-      <c r="JT59" s="76"/>
+      <c r="JO59" s="73"/>
+      <c r="JP59" s="73"/>
+      <c r="JQ59" s="73"/>
+      <c r="JR59" s="73"/>
+      <c r="JS59" s="73"/>
+      <c r="JT59" s="73"/>
       <c r="JU59" s="31"/>
       <c r="JX59" s="69" t="s">
         <v>4</v>
@@ -43125,21 +43135,21 @@
       <c r="KE59" s="69"/>
       <c r="KF59" s="52"/>
       <c r="KG59" s="52"/>
-      <c r="KP59" s="70" t="s">
+      <c r="KP59" s="76" t="s">
         <v>30</v>
       </c>
-      <c r="KQ59" s="70"/>
-      <c r="KR59" s="70"/>
+      <c r="KQ59" s="76"/>
+      <c r="KR59" s="76"/>
       <c r="KW59" s="31"/>
       <c r="KX59" s="31"/>
-      <c r="KY59" s="76"/>
-      <c r="KZ59" s="76"/>
-      <c r="LA59" s="76"/>
-      <c r="LB59" s="76"/>
-      <c r="LC59" s="76"/>
-      <c r="LD59" s="76"/>
-      <c r="LE59" s="76"/>
-      <c r="LF59" s="76"/>
+      <c r="KY59" s="73"/>
+      <c r="KZ59" s="73"/>
+      <c r="LA59" s="73"/>
+      <c r="LB59" s="73"/>
+      <c r="LC59" s="73"/>
+      <c r="LD59" s="73"/>
+      <c r="LE59" s="73"/>
+      <c r="LF59" s="73"/>
       <c r="LG59" s="31"/>
     </row>
     <row r="60" spans="1:319" ht="51" customHeight="1">
@@ -44043,14 +44053,14 @@
       <c r="EC62" s="50"/>
       <c r="ES62" s="31"/>
       <c r="ET62" s="31"/>
-      <c r="EU62" s="73"/>
-      <c r="EV62" s="73"/>
-      <c r="EW62" s="73"/>
-      <c r="EX62" s="73"/>
-      <c r="EY62" s="73"/>
-      <c r="EZ62" s="73"/>
-      <c r="FA62" s="73"/>
-      <c r="FB62" s="73"/>
+      <c r="EU62" s="74"/>
+      <c r="EV62" s="74"/>
+      <c r="EW62" s="74"/>
+      <c r="EX62" s="74"/>
+      <c r="EY62" s="74"/>
+      <c r="EZ62" s="74"/>
+      <c r="FA62" s="74"/>
+      <c r="FB62" s="74"/>
       <c r="FC62" s="31"/>
       <c r="GH62" s="71"/>
       <c r="GI62" s="1" t="s">
@@ -44120,14 +44130,14 @@
       <c r="HE62" s="51"/>
       <c r="HU62" s="31"/>
       <c r="HV62" s="31"/>
-      <c r="HW62" s="73"/>
-      <c r="HX62" s="73"/>
-      <c r="HY62" s="73"/>
-      <c r="HZ62" s="73"/>
-      <c r="IA62" s="73"/>
-      <c r="IB62" s="73"/>
-      <c r="IC62" s="73"/>
-      <c r="ID62" s="73"/>
+      <c r="HW62" s="74"/>
+      <c r="HX62" s="74"/>
+      <c r="HY62" s="74"/>
+      <c r="HZ62" s="74"/>
+      <c r="IA62" s="74"/>
+      <c r="IB62" s="74"/>
+      <c r="IC62" s="74"/>
+      <c r="ID62" s="74"/>
       <c r="IE62" s="31"/>
       <c r="JJ62" s="78"/>
       <c r="JK62" s="63"/>
@@ -44197,14 +44207,14 @@
       </c>
       <c r="KW62" s="31"/>
       <c r="KX62" s="31"/>
-      <c r="KY62" s="73"/>
-      <c r="KZ62" s="73"/>
-      <c r="LA62" s="73"/>
-      <c r="LB62" s="73"/>
-      <c r="LC62" s="73"/>
-      <c r="LD62" s="73"/>
-      <c r="LE62" s="73"/>
-      <c r="LF62" s="73"/>
+      <c r="KY62" s="74"/>
+      <c r="KZ62" s="74"/>
+      <c r="LA62" s="74"/>
+      <c r="LB62" s="74"/>
+      <c r="LC62" s="74"/>
+      <c r="LD62" s="74"/>
+      <c r="LE62" s="74"/>
+      <c r="LF62" s="74"/>
       <c r="LG62" s="31"/>
     </row>
     <row r="63" spans="1:319">
@@ -45801,11 +45811,11 @@
       <c r="J67" s="69"/>
       <c r="X67" s="15"/>
       <c r="Y67" s="15"/>
-      <c r="Z67" s="73" t="s">
+      <c r="Z67" s="74" t="s">
         <v>96</v>
       </c>
-      <c r="AA67" s="73"/>
-      <c r="AB67" s="73"/>
+      <c r="AA67" s="74"/>
+      <c r="AB67" s="74"/>
       <c r="AD67" s="45" t="s">
         <v>34</v>
       </c>
@@ -46020,23 +46030,23 @@
       <c r="JL67" s="55"/>
       <c r="JM67" s="31"/>
       <c r="JN67" s="31"/>
-      <c r="JO67" s="76"/>
-      <c r="JP67" s="76"/>
-      <c r="JQ67" s="76"/>
-      <c r="JR67" s="76"/>
-      <c r="JS67" s="76"/>
-      <c r="JT67" s="76"/>
+      <c r="JO67" s="73"/>
+      <c r="JP67" s="73"/>
+      <c r="JQ67" s="73"/>
+      <c r="JR67" s="73"/>
+      <c r="JS67" s="73"/>
+      <c r="JT67" s="73"/>
       <c r="JU67" s="31"/>
-      <c r="JX67" s="80" t="s">
+      <c r="JX67" s="79" t="s">
         <v>134</v>
       </c>
-      <c r="JY67" s="80"/>
-      <c r="JZ67" s="80"/>
-      <c r="KA67" s="80"/>
-      <c r="KB67" s="80"/>
-      <c r="KC67" s="80"/>
-      <c r="KD67" s="80"/>
-      <c r="KE67" s="80"/>
+      <c r="JY67" s="79"/>
+      <c r="JZ67" s="79"/>
+      <c r="KA67" s="79"/>
+      <c r="KB67" s="79"/>
+      <c r="KC67" s="79"/>
+      <c r="KD67" s="79"/>
+      <c r="KE67" s="79"/>
       <c r="KF67" s="54"/>
       <c r="KG67" s="54"/>
       <c r="KH67" s="26"/>
@@ -46047,11 +46057,11 @@
       <c r="KM67" s="26"/>
       <c r="KN67" s="26"/>
       <c r="KO67" s="26"/>
-      <c r="KP67" s="73" t="s">
+      <c r="KP67" s="74" t="s">
         <v>142</v>
       </c>
-      <c r="KQ67" s="73"/>
-      <c r="KR67" s="73"/>
+      <c r="KQ67" s="74"/>
+      <c r="KR67" s="74"/>
       <c r="KS67" s="26"/>
       <c r="KT67" s="52" t="s">
         <v>145</v>
@@ -46169,18 +46179,18 @@
       <c r="W70" s="15"/>
       <c r="X70" s="15"/>
       <c r="Y70" s="15"/>
-      <c r="Z70" s="70" t="s">
+      <c r="Z70" s="76" t="s">
         <v>30</v>
       </c>
-      <c r="AA70" s="70"/>
-      <c r="AB70" s="70"/>
-      <c r="AH70" s="74" t="s">
+      <c r="AA70" s="76"/>
+      <c r="AB70" s="76"/>
+      <c r="AH70" s="77" t="s">
         <v>52</v>
       </c>
-      <c r="AI70" s="74"/>
+      <c r="AI70" s="77"/>
       <c r="AJ70" s="31"/>
-      <c r="AK70" s="74"/>
-      <c r="AL70" s="74"/>
+      <c r="AK70" s="77"/>
+      <c r="AL70" s="77"/>
       <c r="AM70" s="31"/>
       <c r="AN70" s="31"/>
       <c r="AO70" s="31"/>
@@ -46268,7 +46278,7 @@
         <v>52</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C72" s="4">
         <f>F5</f>
@@ -46506,37 +46516,37 @@
       <c r="W74" s="15"/>
       <c r="X74" s="15"/>
       <c r="Y74" s="15"/>
-      <c r="Z74" s="76" t="s">
+      <c r="Z74" s="73" t="s">
         <v>95</v>
       </c>
-      <c r="AA74" s="76"/>
-      <c r="AB74" s="76"/>
+      <c r="AA74" s="73"/>
+      <c r="AB74" s="73"/>
       <c r="AD74" s="45" t="s">
         <v>53</v>
       </c>
-      <c r="AH74" s="76" t="s">
+      <c r="AH74" s="73" t="s">
         <v>64</v>
       </c>
-      <c r="AI74" s="76"/>
+      <c r="AI74" s="73"/>
       <c r="AJ74" s="29"/>
-      <c r="AK74" s="76"/>
-      <c r="AL74" s="76"/>
+      <c r="AK74" s="73"/>
+      <c r="AL74" s="73"/>
       <c r="AM74" s="29"/>
       <c r="AN74" s="31"/>
       <c r="AO74" s="31"/>
       <c r="AP74" s="31"/>
       <c r="AQ74" s="31"/>
       <c r="AR74" s="31"/>
-      <c r="AS74" s="76" t="s">
+      <c r="AS74" s="73" t="s">
         <v>65</v>
       </c>
-      <c r="AT74" s="76"/>
-      <c r="AU74" s="76"/>
-      <c r="AV74" s="76"/>
-      <c r="AW74" s="76"/>
-      <c r="AX74" s="76"/>
-      <c r="AY74" s="76"/>
-      <c r="AZ74" s="76"/>
+      <c r="AT74" s="73"/>
+      <c r="AU74" s="73"/>
+      <c r="AV74" s="73"/>
+      <c r="AW74" s="73"/>
+      <c r="AX74" s="73"/>
+      <c r="AY74" s="73"/>
+      <c r="AZ74" s="73"/>
       <c r="ES74" s="31"/>
       <c r="ET74" s="31"/>
       <c r="EU74" s="31"/>
@@ -48760,16 +48770,16 @@
       <c r="FA83" s="29"/>
       <c r="FB83" s="29"/>
       <c r="FC83" s="31"/>
-      <c r="FD83" s="77" t="s">
+      <c r="FD83" s="70" t="s">
         <v>119</v>
       </c>
-      <c r="FE83" s="77"/>
-      <c r="FF83" s="77"/>
-      <c r="FG83" s="77"/>
-      <c r="FH83" s="77"/>
-      <c r="FI83" s="77"/>
-      <c r="FJ83" s="77"/>
-      <c r="FK83" s="77"/>
+      <c r="FE83" s="70"/>
+      <c r="FF83" s="70"/>
+      <c r="FG83" s="70"/>
+      <c r="FH83" s="70"/>
+      <c r="FI83" s="70"/>
+      <c r="FJ83" s="70"/>
+      <c r="FK83" s="70"/>
       <c r="GH83" s="71"/>
       <c r="GI83" s="1" t="s">
         <v>27</v>
@@ -48881,16 +48891,16 @@
       <c r="IC83" s="29"/>
       <c r="ID83" s="29"/>
       <c r="IE83" s="31"/>
-      <c r="IF83" s="77" t="s">
+      <c r="IF83" s="70" t="s">
         <v>130</v>
       </c>
-      <c r="IG83" s="77"/>
-      <c r="IH83" s="77"/>
-      <c r="II83" s="77"/>
-      <c r="IJ83" s="77"/>
-      <c r="IK83" s="77"/>
-      <c r="IL83" s="77"/>
-      <c r="IM83" s="77"/>
+      <c r="IG83" s="70"/>
+      <c r="IH83" s="70"/>
+      <c r="II83" s="70"/>
+      <c r="IJ83" s="70"/>
+      <c r="IK83" s="70"/>
+      <c r="IL83" s="70"/>
+      <c r="IM83" s="70"/>
       <c r="JJ83" s="78"/>
       <c r="JK83" s="63"/>
       <c r="JL83" s="51"/>
@@ -48977,16 +48987,16 @@
       <c r="LE83" s="29"/>
       <c r="LF83" s="29"/>
       <c r="LG83" s="31"/>
-      <c r="LH83" s="77" t="s">
+      <c r="LH83" s="70" t="s">
         <v>139</v>
       </c>
-      <c r="LI83" s="77"/>
-      <c r="LJ83" s="77"/>
-      <c r="LK83" s="77"/>
-      <c r="LL83" s="77"/>
-      <c r="LM83" s="77"/>
-      <c r="LN83" s="77"/>
-      <c r="LO83" s="77"/>
+      <c r="LI83" s="70"/>
+      <c r="LJ83" s="70"/>
+      <c r="LK83" s="70"/>
+      <c r="LL83" s="70"/>
+      <c r="LM83" s="70"/>
+      <c r="LN83" s="70"/>
+      <c r="LO83" s="70"/>
     </row>
     <row r="84" spans="1:327">
       <c r="A84" s="71"/>
@@ -49955,16 +49965,16 @@
       <c r="LE85" s="31"/>
       <c r="LF85" s="31"/>
       <c r="LG85" s="31"/>
-      <c r="LH85" s="77" t="s">
+      <c r="LH85" s="70" t="s">
         <v>140</v>
       </c>
-      <c r="LI85" s="77"/>
-      <c r="LJ85" s="77"/>
-      <c r="LK85" s="77"/>
-      <c r="LL85" s="77"/>
-      <c r="LM85" s="77"/>
-      <c r="LN85" s="77"/>
-      <c r="LO85" s="77"/>
+      <c r="LI85" s="70"/>
+      <c r="LJ85" s="70"/>
+      <c r="LK85" s="70"/>
+      <c r="LL85" s="70"/>
+      <c r="LM85" s="70"/>
+      <c r="LN85" s="70"/>
+      <c r="LO85" s="70"/>
     </row>
     <row r="86" spans="1:327">
       <c r="A86" s="71"/>
@@ -51371,14 +51381,14 @@
       <c r="LG88" s="31"/>
     </row>
     <row r="89" spans="1:327" ht="20">
-      <c r="L89" s="77" t="s">
+      <c r="L89" s="70" t="s">
         <v>13</v>
       </c>
-      <c r="M89" s="77"/>
-      <c r="N89" s="77"/>
-      <c r="O89" s="77"/>
-      <c r="P89" s="77"/>
-      <c r="Q89" s="77"/>
+      <c r="M89" s="70"/>
+      <c r="N89" s="70"/>
+      <c r="O89" s="70"/>
+      <c r="P89" s="70"/>
+      <c r="Q89" s="70"/>
       <c r="Z89" s="45" t="s">
         <v>11</v>
       </c>
@@ -51484,30 +51494,30 @@
       <c r="EB89" s="8"/>
       <c r="EC89" s="8"/>
       <c r="ED89" s="8"/>
-      <c r="EE89" s="77" t="s">
+      <c r="EE89" s="70" t="s">
         <v>114</v>
       </c>
-      <c r="EF89" s="77"/>
-      <c r="EG89" s="77"/>
-      <c r="EH89" s="77"/>
-      <c r="EI89" s="77"/>
-      <c r="EJ89" s="77"/>
+      <c r="EF89" s="70"/>
+      <c r="EG89" s="70"/>
+      <c r="EH89" s="70"/>
+      <c r="EI89" s="70"/>
+      <c r="EJ89" s="70"/>
       <c r="EM89" s="45" t="s">
         <v>116</v>
       </c>
       <c r="EO89" s="48" t="s">
         <v>117</v>
       </c>
-      <c r="ER89" s="77" t="s">
+      <c r="ER89" s="70" t="s">
         <v>118</v>
       </c>
-      <c r="ES89" s="77"/>
-      <c r="ET89" s="77"/>
-      <c r="EU89" s="77"/>
-      <c r="EV89" s="77"/>
-      <c r="EW89" s="77"/>
-      <c r="EX89" s="77"/>
-      <c r="EY89" s="77"/>
+      <c r="ES89" s="70"/>
+      <c r="ET89" s="70"/>
+      <c r="EU89" s="70"/>
+      <c r="EV89" s="70"/>
+      <c r="EW89" s="70"/>
+      <c r="EX89" s="70"/>
+      <c r="EY89" s="70"/>
       <c r="FO89" s="57"/>
       <c r="FP89" s="8"/>
       <c r="FQ89" s="8"/>
@@ -51552,30 +51562,30 @@
       <c r="HD89" s="8"/>
       <c r="HE89" s="8"/>
       <c r="HF89" s="8"/>
-      <c r="HG89" s="77" t="s">
+      <c r="HG89" s="70" t="s">
         <v>125</v>
       </c>
-      <c r="HH89" s="77"/>
-      <c r="HI89" s="77"/>
-      <c r="HJ89" s="77"/>
-      <c r="HK89" s="77"/>
-      <c r="HL89" s="77"/>
+      <c r="HH89" s="70"/>
+      <c r="HI89" s="70"/>
+      <c r="HJ89" s="70"/>
+      <c r="HK89" s="70"/>
+      <c r="HL89" s="70"/>
       <c r="HO89" s="52" t="s">
         <v>127</v>
       </c>
       <c r="HQ89" s="53" t="s">
         <v>128</v>
       </c>
-      <c r="HT89" s="77" t="s">
+      <c r="HT89" s="70" t="s">
         <v>129</v>
       </c>
-      <c r="HU89" s="77"/>
-      <c r="HV89" s="77"/>
-      <c r="HW89" s="77"/>
-      <c r="HX89" s="77"/>
-      <c r="HY89" s="77"/>
-      <c r="HZ89" s="77"/>
-      <c r="IA89" s="77"/>
+      <c r="HU89" s="70"/>
+      <c r="HV89" s="70"/>
+      <c r="HW89" s="70"/>
+      <c r="HX89" s="70"/>
+      <c r="HY89" s="70"/>
+      <c r="HZ89" s="70"/>
+      <c r="IA89" s="70"/>
       <c r="IQ89" s="57"/>
       <c r="IR89" s="8"/>
       <c r="IS89" s="8"/>
@@ -51600,14 +51610,14 @@
       <c r="JL89" s="55"/>
       <c r="JM89" s="31"/>
       <c r="JN89" s="31"/>
-      <c r="JO89" s="76"/>
-      <c r="JP89" s="76"/>
-      <c r="JQ89" s="76"/>
-      <c r="JR89" s="76"/>
-      <c r="JS89" s="76"/>
-      <c r="JT89" s="76"/>
-      <c r="JU89" s="76"/>
-      <c r="JV89" s="76"/>
+      <c r="JO89" s="73"/>
+      <c r="JP89" s="73"/>
+      <c r="JQ89" s="73"/>
+      <c r="JR89" s="73"/>
+      <c r="JS89" s="73"/>
+      <c r="JT89" s="73"/>
+      <c r="JU89" s="73"/>
+      <c r="JV89" s="73"/>
       <c r="JW89" s="29"/>
       <c r="JX89" s="29"/>
       <c r="JY89" s="8"/>
@@ -51620,30 +51630,30 @@
       <c r="KF89" s="8"/>
       <c r="KG89" s="8"/>
       <c r="KH89" s="8"/>
-      <c r="KI89" s="77" t="s">
+      <c r="KI89" s="70" t="s">
         <v>97</v>
       </c>
-      <c r="KJ89" s="77"/>
-      <c r="KK89" s="77"/>
-      <c r="KL89" s="77"/>
-      <c r="KM89" s="77"/>
-      <c r="KN89" s="77"/>
+      <c r="KJ89" s="70"/>
+      <c r="KK89" s="70"/>
+      <c r="KL89" s="70"/>
+      <c r="KM89" s="70"/>
+      <c r="KN89" s="70"/>
       <c r="KQ89" s="52" t="s">
         <v>98</v>
       </c>
       <c r="KS89" s="53" t="s">
         <v>135</v>
       </c>
-      <c r="KV89" s="77" t="s">
+      <c r="KV89" s="70" t="s">
         <v>136</v>
       </c>
-      <c r="KW89" s="77"/>
-      <c r="KX89" s="77"/>
-      <c r="KY89" s="77"/>
-      <c r="KZ89" s="77"/>
-      <c r="LA89" s="77"/>
-      <c r="LB89" s="77"/>
-      <c r="LC89" s="77"/>
+      <c r="KW89" s="70"/>
+      <c r="KX89" s="70"/>
+      <c r="KY89" s="70"/>
+      <c r="KZ89" s="70"/>
+      <c r="LA89" s="70"/>
+      <c r="LB89" s="70"/>
+      <c r="LC89" s="70"/>
     </row>
     <row r="90" spans="1:327" ht="16" customHeight="1">
       <c r="J90" s="71" t="s">
@@ -52013,22 +52023,22 @@
       </c>
     </row>
     <row r="93" spans="1:327" ht="20">
-      <c r="L93" s="77" t="s">
+      <c r="L93" s="70" t="s">
         <v>35</v>
       </c>
-      <c r="M93" s="77"/>
-      <c r="N93" s="77"/>
-      <c r="O93" s="77"/>
-      <c r="P93" s="77"/>
-      <c r="Q93" s="77"/>
-      <c r="EE93" s="77" t="s">
+      <c r="M93" s="70"/>
+      <c r="N93" s="70"/>
+      <c r="O93" s="70"/>
+      <c r="P93" s="70"/>
+      <c r="Q93" s="70"/>
+      <c r="EE93" s="70" t="s">
         <v>115</v>
       </c>
-      <c r="EF93" s="77"/>
-      <c r="EG93" s="77"/>
-      <c r="EH93" s="77"/>
-      <c r="EI93" s="77"/>
-      <c r="EJ93" s="77"/>
+      <c r="EF93" s="70"/>
+      <c r="EG93" s="70"/>
+      <c r="EH93" s="70"/>
+      <c r="EI93" s="70"/>
+      <c r="EJ93" s="70"/>
       <c r="EM93" s="53" t="s">
         <v>137</v>
       </c>
@@ -52037,25 +52047,25 @@
       <c r="EP93" s="53"/>
       <c r="EQ93" s="53"/>
       <c r="ER93" s="53"/>
-      <c r="HG93" s="77" t="s">
+      <c r="HG93" s="70" t="s">
         <v>126</v>
       </c>
-      <c r="HH93" s="77"/>
-      <c r="HI93" s="77"/>
-      <c r="HJ93" s="77"/>
-      <c r="HK93" s="77"/>
-      <c r="HL93" s="77"/>
+      <c r="HH93" s="70"/>
+      <c r="HI93" s="70"/>
+      <c r="HJ93" s="70"/>
+      <c r="HK93" s="70"/>
+      <c r="HL93" s="70"/>
       <c r="HO93" s="53" t="s">
         <v>138</v>
       </c>
-      <c r="KI93" s="77" t="s">
+      <c r="KI93" s="70" t="s">
         <v>99</v>
       </c>
-      <c r="KJ93" s="77"/>
-      <c r="KK93" s="77"/>
-      <c r="KL93" s="77"/>
-      <c r="KM93" s="77"/>
-      <c r="KN93" s="77"/>
+      <c r="KJ93" s="70"/>
+      <c r="KK93" s="70"/>
+      <c r="KL93" s="70"/>
+      <c r="KM93" s="70"/>
+      <c r="KN93" s="70"/>
     </row>
     <row r="96" spans="1:327" ht="47">
       <c r="A96" s="27" t="s">
@@ -53271,17 +53281,17 @@
       </c>
       <c r="D118" s="69"/>
       <c r="E118" s="69"/>
-      <c r="G118" s="77" t="s">
+      <c r="G118" s="70" t="s">
         <v>39</v>
       </c>
-      <c r="H118" s="77"/>
-      <c r="I118" s="77"/>
+      <c r="H118" s="70"/>
+      <c r="I118" s="70"/>
       <c r="J118" s="17"/>
-      <c r="K118" s="77" t="s">
+      <c r="K118" s="70" t="s">
         <v>40</v>
       </c>
-      <c r="L118" s="77"/>
-      <c r="M118" s="77"/>
+      <c r="L118" s="70"/>
+      <c r="M118" s="70"/>
       <c r="N118" s="17"/>
       <c r="O118" s="17" t="s">
         <v>41</v>
@@ -53296,17 +53306,17 @@
       </c>
       <c r="JZ118" s="69"/>
       <c r="KA118" s="69"/>
-      <c r="KC118" s="77" t="s">
+      <c r="KC118" s="70" t="s">
         <v>144</v>
       </c>
-      <c r="KD118" s="77"/>
-      <c r="KE118" s="77"/>
+      <c r="KD118" s="70"/>
+      <c r="KE118" s="70"/>
       <c r="KF118" s="17"/>
-      <c r="KG118" s="77" t="s">
+      <c r="KG118" s="70" t="s">
         <v>149</v>
       </c>
-      <c r="KH118" s="77"/>
-      <c r="KI118" s="77"/>
+      <c r="KH118" s="70"/>
+      <c r="KI118" s="70"/>
       <c r="KJ118" s="17"/>
       <c r="KK118" s="17" t="s">
         <v>150</v>
@@ -53585,82 +53595,79 @@
     </row>
   </sheetData>
   <mergeCells count="173">
-    <mergeCell ref="JW98:KE98"/>
-    <mergeCell ref="JW100:JW107"/>
-    <mergeCell ref="JW110:KE110"/>
-    <mergeCell ref="JW112:JW117"/>
-    <mergeCell ref="JY118:KA118"/>
-    <mergeCell ref="KC118:KE118"/>
-    <mergeCell ref="KG118:KI118"/>
-    <mergeCell ref="JW123:JW128"/>
-    <mergeCell ref="JJ81:JJ88"/>
-    <mergeCell ref="KG81:KG88"/>
-    <mergeCell ref="LF81:LF82"/>
-    <mergeCell ref="LH83:LO83"/>
-    <mergeCell ref="JO89:JV89"/>
-    <mergeCell ref="KI89:KN89"/>
-    <mergeCell ref="KV89:LC89"/>
-    <mergeCell ref="KG90:KG92"/>
-    <mergeCell ref="KI93:KN93"/>
-    <mergeCell ref="LH85:LO85"/>
-    <mergeCell ref="KY59:LF59"/>
-    <mergeCell ref="KP59:KR59"/>
-    <mergeCell ref="JJ61:JJ66"/>
-    <mergeCell ref="KY62:LF62"/>
-    <mergeCell ref="JO67:JT67"/>
-    <mergeCell ref="JX67:KE67"/>
-    <mergeCell ref="JO79:JV79"/>
-    <mergeCell ref="KI79:KN79"/>
-    <mergeCell ref="KV79:LC79"/>
-    <mergeCell ref="LH79:LO79"/>
-    <mergeCell ref="JV61:JV66"/>
-    <mergeCell ref="KP67:KR67"/>
-    <mergeCell ref="JL40:JM40"/>
-    <mergeCell ref="KI40:KN40"/>
-    <mergeCell ref="IU42:IU49"/>
-    <mergeCell ref="JJ42:JJ49"/>
-    <mergeCell ref="IW50:IX50"/>
-    <mergeCell ref="IZ50:JE50"/>
-    <mergeCell ref="KI50:KN50"/>
-    <mergeCell ref="JO59:JT59"/>
-    <mergeCell ref="JX59:KE59"/>
-    <mergeCell ref="KG42:KG49"/>
-    <mergeCell ref="KG51:KG53"/>
-    <mergeCell ref="KI54:KN54"/>
-    <mergeCell ref="KI56:KN56"/>
-    <mergeCell ref="ID81:ID82"/>
-    <mergeCell ref="IF83:IM83"/>
-    <mergeCell ref="GM89:GT89"/>
-    <mergeCell ref="HG89:HL89"/>
-    <mergeCell ref="HT89:IA89"/>
-    <mergeCell ref="HE90:HE92"/>
-    <mergeCell ref="HG93:HL93"/>
-    <mergeCell ref="IW40:IX40"/>
-    <mergeCell ref="IZ40:JE40"/>
-    <mergeCell ref="GJ40:GO40"/>
-    <mergeCell ref="GJ50:GO50"/>
-    <mergeCell ref="HW59:ID59"/>
-    <mergeCell ref="GM79:GT79"/>
-    <mergeCell ref="HG79:HL79"/>
-    <mergeCell ref="HT79:IA79"/>
-    <mergeCell ref="IF79:IM79"/>
-    <mergeCell ref="HW62:ID62"/>
-    <mergeCell ref="GM67:GR67"/>
-    <mergeCell ref="GV67:HC67"/>
-    <mergeCell ref="GM59:GR59"/>
-    <mergeCell ref="GV59:HC59"/>
-    <mergeCell ref="CV40:DA40"/>
-    <mergeCell ref="CV50:DA50"/>
-    <mergeCell ref="FU40:FV40"/>
-    <mergeCell ref="FX40:GC40"/>
-    <mergeCell ref="HG40:HL40"/>
-    <mergeCell ref="FS42:FS49"/>
-    <mergeCell ref="FU50:FV50"/>
-    <mergeCell ref="FX50:GC50"/>
-    <mergeCell ref="HG50:HL50"/>
-    <mergeCell ref="DH40:DM40"/>
-    <mergeCell ref="DH50:DM50"/>
-    <mergeCell ref="EE50:EJ50"/>
+    <mergeCell ref="GH81:GH88"/>
+    <mergeCell ref="HE81:HE88"/>
+    <mergeCell ref="A123:A128"/>
+    <mergeCell ref="A100:A107"/>
+    <mergeCell ref="A110:I110"/>
+    <mergeCell ref="A112:A117"/>
+    <mergeCell ref="C118:E118"/>
+    <mergeCell ref="G118:I118"/>
+    <mergeCell ref="K118:M118"/>
+    <mergeCell ref="ER89:EY89"/>
+    <mergeCell ref="J90:J92"/>
+    <mergeCell ref="EC90:EC92"/>
+    <mergeCell ref="L93:Q93"/>
+    <mergeCell ref="EE93:EJ93"/>
+    <mergeCell ref="A98:I98"/>
+    <mergeCell ref="L89:Q89"/>
+    <mergeCell ref="AH89:AO89"/>
+    <mergeCell ref="AS89:AZ89"/>
+    <mergeCell ref="BD89:BK89"/>
+    <mergeCell ref="DK89:DR89"/>
+    <mergeCell ref="EE89:EJ89"/>
+    <mergeCell ref="BS89:BX89"/>
+    <mergeCell ref="CS40:CT40"/>
+    <mergeCell ref="EE40:EJ40"/>
+    <mergeCell ref="C76:J76"/>
+    <mergeCell ref="BS67:BX67"/>
+    <mergeCell ref="EE79:EJ79"/>
+    <mergeCell ref="ER79:EY79"/>
+    <mergeCell ref="FD79:FK79"/>
+    <mergeCell ref="A81:A88"/>
+    <mergeCell ref="DF81:DF88"/>
+    <mergeCell ref="EC81:EC88"/>
+    <mergeCell ref="FB81:FB82"/>
+    <mergeCell ref="FD83:FK83"/>
+    <mergeCell ref="AH79:AO79"/>
+    <mergeCell ref="AS79:AZ79"/>
+    <mergeCell ref="BD79:BK79"/>
+    <mergeCell ref="DK79:DR79"/>
+    <mergeCell ref="C67:J67"/>
+    <mergeCell ref="Z67:AB67"/>
+    <mergeCell ref="AH67:AM67"/>
+    <mergeCell ref="AS67:AZ67"/>
+    <mergeCell ref="BD67:BK67"/>
+    <mergeCell ref="BS79:BX79"/>
+    <mergeCell ref="DK67:DP67"/>
+    <mergeCell ref="DT67:EA67"/>
+    <mergeCell ref="C26:E26"/>
+    <mergeCell ref="A28:A35"/>
+    <mergeCell ref="C36:E36"/>
+    <mergeCell ref="BL38:CJ38"/>
+    <mergeCell ref="C40:J40"/>
+    <mergeCell ref="L40:Q40"/>
+    <mergeCell ref="W40:X40"/>
+    <mergeCell ref="AH40:AO40"/>
+    <mergeCell ref="AS40:AX40"/>
+    <mergeCell ref="BD40:BI40"/>
+    <mergeCell ref="BS40:BX40"/>
+    <mergeCell ref="BZ40:CG40"/>
+    <mergeCell ref="CI40:CJ40"/>
+    <mergeCell ref="GH61:GH66"/>
+    <mergeCell ref="AS59:AZ59"/>
+    <mergeCell ref="BD59:BK59"/>
+    <mergeCell ref="AH50:AO50"/>
+    <mergeCell ref="AS50:AX50"/>
+    <mergeCell ref="BD50:BI50"/>
+    <mergeCell ref="CS50:CT50"/>
+    <mergeCell ref="BS50:BX50"/>
+    <mergeCell ref="BZ50:CG50"/>
+    <mergeCell ref="EU59:FB59"/>
+    <mergeCell ref="DF61:DF66"/>
+    <mergeCell ref="EU62:FB62"/>
+    <mergeCell ref="DK59:DP59"/>
+    <mergeCell ref="BS59:BX59"/>
     <mergeCell ref="CQ42:CQ49"/>
     <mergeCell ref="DF42:DF49"/>
     <mergeCell ref="A72:A73"/>
@@ -53685,79 +53692,82 @@
     <mergeCell ref="A61:A66"/>
     <mergeCell ref="L71:Q71"/>
     <mergeCell ref="L56:Q56"/>
-    <mergeCell ref="GH61:GH66"/>
-    <mergeCell ref="AS59:AZ59"/>
-    <mergeCell ref="BD59:BK59"/>
-    <mergeCell ref="AH50:AO50"/>
-    <mergeCell ref="AS50:AX50"/>
-    <mergeCell ref="BD50:BI50"/>
-    <mergeCell ref="CS50:CT50"/>
-    <mergeCell ref="BS50:BX50"/>
-    <mergeCell ref="BZ50:CG50"/>
-    <mergeCell ref="EU59:FB59"/>
-    <mergeCell ref="DF61:DF66"/>
-    <mergeCell ref="EU62:FB62"/>
-    <mergeCell ref="DK59:DP59"/>
-    <mergeCell ref="BS59:BX59"/>
-    <mergeCell ref="C26:E26"/>
-    <mergeCell ref="A28:A35"/>
-    <mergeCell ref="C36:E36"/>
-    <mergeCell ref="BL38:CJ38"/>
-    <mergeCell ref="C40:J40"/>
-    <mergeCell ref="L40:Q40"/>
-    <mergeCell ref="W40:X40"/>
-    <mergeCell ref="AH40:AO40"/>
-    <mergeCell ref="AS40:AX40"/>
-    <mergeCell ref="BD40:BI40"/>
-    <mergeCell ref="BS40:BX40"/>
-    <mergeCell ref="BZ40:CG40"/>
-    <mergeCell ref="CI40:CJ40"/>
-    <mergeCell ref="CS40:CT40"/>
-    <mergeCell ref="EE40:EJ40"/>
-    <mergeCell ref="C76:J76"/>
-    <mergeCell ref="BS67:BX67"/>
-    <mergeCell ref="EE79:EJ79"/>
-    <mergeCell ref="ER79:EY79"/>
-    <mergeCell ref="FD79:FK79"/>
-    <mergeCell ref="A81:A88"/>
-    <mergeCell ref="DF81:DF88"/>
-    <mergeCell ref="EC81:EC88"/>
-    <mergeCell ref="FB81:FB82"/>
-    <mergeCell ref="FD83:FK83"/>
-    <mergeCell ref="AH79:AO79"/>
-    <mergeCell ref="AS79:AZ79"/>
-    <mergeCell ref="BD79:BK79"/>
-    <mergeCell ref="DK79:DR79"/>
-    <mergeCell ref="C67:J67"/>
-    <mergeCell ref="Z67:AB67"/>
-    <mergeCell ref="AH67:AM67"/>
-    <mergeCell ref="AS67:AZ67"/>
-    <mergeCell ref="BD67:BK67"/>
-    <mergeCell ref="BS79:BX79"/>
-    <mergeCell ref="DK67:DP67"/>
-    <mergeCell ref="DT67:EA67"/>
-    <mergeCell ref="GH81:GH88"/>
-    <mergeCell ref="HE81:HE88"/>
-    <mergeCell ref="A123:A128"/>
-    <mergeCell ref="A100:A107"/>
-    <mergeCell ref="A110:I110"/>
-    <mergeCell ref="A112:A117"/>
-    <mergeCell ref="C118:E118"/>
-    <mergeCell ref="G118:I118"/>
-    <mergeCell ref="K118:M118"/>
-    <mergeCell ref="ER89:EY89"/>
-    <mergeCell ref="J90:J92"/>
-    <mergeCell ref="EC90:EC92"/>
-    <mergeCell ref="L93:Q93"/>
-    <mergeCell ref="EE93:EJ93"/>
-    <mergeCell ref="A98:I98"/>
-    <mergeCell ref="L89:Q89"/>
-    <mergeCell ref="AH89:AO89"/>
-    <mergeCell ref="AS89:AZ89"/>
-    <mergeCell ref="BD89:BK89"/>
-    <mergeCell ref="DK89:DR89"/>
-    <mergeCell ref="EE89:EJ89"/>
-    <mergeCell ref="BS89:BX89"/>
+    <mergeCell ref="CV40:DA40"/>
+    <mergeCell ref="CV50:DA50"/>
+    <mergeCell ref="FU40:FV40"/>
+    <mergeCell ref="FX40:GC40"/>
+    <mergeCell ref="HG40:HL40"/>
+    <mergeCell ref="FS42:FS49"/>
+    <mergeCell ref="FU50:FV50"/>
+    <mergeCell ref="FX50:GC50"/>
+    <mergeCell ref="HG50:HL50"/>
+    <mergeCell ref="DH40:DM40"/>
+    <mergeCell ref="DH50:DM50"/>
+    <mergeCell ref="EE50:EJ50"/>
+    <mergeCell ref="ID81:ID82"/>
+    <mergeCell ref="IF83:IM83"/>
+    <mergeCell ref="GM89:GT89"/>
+    <mergeCell ref="HG89:HL89"/>
+    <mergeCell ref="HT89:IA89"/>
+    <mergeCell ref="HE90:HE92"/>
+    <mergeCell ref="HG93:HL93"/>
+    <mergeCell ref="IW40:IX40"/>
+    <mergeCell ref="IZ40:JE40"/>
+    <mergeCell ref="GJ40:GO40"/>
+    <mergeCell ref="GJ50:GO50"/>
+    <mergeCell ref="HW59:ID59"/>
+    <mergeCell ref="GM79:GT79"/>
+    <mergeCell ref="HG79:HL79"/>
+    <mergeCell ref="HT79:IA79"/>
+    <mergeCell ref="IF79:IM79"/>
+    <mergeCell ref="HW62:ID62"/>
+    <mergeCell ref="GM67:GR67"/>
+    <mergeCell ref="GV67:HC67"/>
+    <mergeCell ref="GM59:GR59"/>
+    <mergeCell ref="GV59:HC59"/>
+    <mergeCell ref="JL40:JM40"/>
+    <mergeCell ref="KI40:KN40"/>
+    <mergeCell ref="IU42:IU49"/>
+    <mergeCell ref="JJ42:JJ49"/>
+    <mergeCell ref="IW50:IX50"/>
+    <mergeCell ref="IZ50:JE50"/>
+    <mergeCell ref="KI50:KN50"/>
+    <mergeCell ref="JO59:JT59"/>
+    <mergeCell ref="JX59:KE59"/>
+    <mergeCell ref="KG42:KG49"/>
+    <mergeCell ref="KG51:KG53"/>
+    <mergeCell ref="KI54:KN54"/>
+    <mergeCell ref="KI56:KN56"/>
+    <mergeCell ref="JJ61:JJ66"/>
+    <mergeCell ref="KY62:LF62"/>
+    <mergeCell ref="JO67:JT67"/>
+    <mergeCell ref="JX67:KE67"/>
+    <mergeCell ref="JO79:JV79"/>
+    <mergeCell ref="KI79:KN79"/>
+    <mergeCell ref="KV79:LC79"/>
+    <mergeCell ref="LH79:LO79"/>
+    <mergeCell ref="JV61:JV66"/>
+    <mergeCell ref="KP67:KR67"/>
+    <mergeCell ref="LF81:LF82"/>
+    <mergeCell ref="LH83:LO83"/>
+    <mergeCell ref="JO89:JV89"/>
+    <mergeCell ref="KI89:KN89"/>
+    <mergeCell ref="KV89:LC89"/>
+    <mergeCell ref="KG90:KG92"/>
+    <mergeCell ref="KI93:KN93"/>
+    <mergeCell ref="LH85:LO85"/>
+    <mergeCell ref="KY59:LF59"/>
+    <mergeCell ref="KP59:KR59"/>
+    <mergeCell ref="JW98:KE98"/>
+    <mergeCell ref="JW100:JW107"/>
+    <mergeCell ref="JW110:KE110"/>
+    <mergeCell ref="JW112:JW117"/>
+    <mergeCell ref="JY118:KA118"/>
+    <mergeCell ref="KC118:KE118"/>
+    <mergeCell ref="KG118:KI118"/>
+    <mergeCell ref="JW123:JW128"/>
+    <mergeCell ref="JJ81:JJ88"/>
+    <mergeCell ref="KG81:KG88"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -53770,8 +53780,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81DB1CE6-E3EC-7B4E-8832-2A8872C682BA}">
   <dimension ref="A1:J21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -53805,33 +53815,33 @@
         <v>169</v>
       </c>
       <c r="I1" t="s">
+        <v>193</v>
+      </c>
+      <c r="J1" t="s">
         <v>170</v>
-      </c>
-      <c r="J1" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="2" spans="1:10">
       <c r="A2" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="B2">
         <v>2000</v>
       </c>
       <c r="C2" t="s">
+        <v>171</v>
+      </c>
+      <c r="D2" t="s">
         <v>172</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
+        <v>192</v>
+      </c>
+      <c r="F2" t="s">
+        <v>191</v>
+      </c>
+      <c r="G2" t="s">
         <v>173</v>
-      </c>
-      <c r="E2" t="s">
-        <v>174</v>
-      </c>
-      <c r="F2" t="s">
-        <v>181</v>
-      </c>
-      <c r="G2" t="s">
-        <v>175</v>
       </c>
       <c r="H2" t="s">
         <v>23</v>
@@ -53841,27 +53851,27 @@
         <v>97</v>
       </c>
       <c r="J2" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="B3">
         <v>2000</v>
       </c>
       <c r="C3" t="s">
+        <v>171</v>
+      </c>
+      <c r="D3" t="s">
         <v>172</v>
       </c>
-      <c r="D3" t="s">
-        <v>173</v>
-      </c>
       <c r="E3" t="s">
-        <v>174</v>
+        <v>192</v>
       </c>
       <c r="F3" t="s">
-        <v>181</v>
+        <v>191</v>
       </c>
       <c r="G3" t="s">
         <v>21</v>
@@ -53874,27 +53884,27 @@
         <v>87</v>
       </c>
       <c r="J3" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="B4">
         <v>2000</v>
       </c>
       <c r="C4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D4" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="E4" t="s">
-        <v>174</v>
+        <v>192</v>
       </c>
       <c r="F4" t="s">
-        <v>181</v>
+        <v>191</v>
       </c>
       <c r="G4" t="s">
         <v>22</v>
@@ -53907,27 +53917,27 @@
         <v>-97</v>
       </c>
       <c r="J4" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="B5">
         <v>2000</v>
       </c>
       <c r="C5" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D5" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="E5" t="s">
-        <v>174</v>
+        <v>192</v>
       </c>
       <c r="F5" t="s">
-        <v>181</v>
+        <v>191</v>
       </c>
       <c r="G5" t="s">
         <v>22</v>
@@ -53940,27 +53950,27 @@
         <v>-3</v>
       </c>
       <c r="J5" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="B6">
         <v>2000</v>
       </c>
       <c r="C6" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D6" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="E6" t="s">
-        <v>174</v>
+        <v>192</v>
       </c>
       <c r="F6" t="s">
-        <v>181</v>
+        <v>191</v>
       </c>
       <c r="G6" t="s">
         <v>22</v>
@@ -53973,27 +53983,27 @@
         <v>22.4</v>
       </c>
       <c r="J6" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="B7">
         <v>2000</v>
       </c>
       <c r="C7" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D7" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="E7" t="s">
-        <v>174</v>
+        <v>192</v>
       </c>
       <c r="F7" t="s">
-        <v>181</v>
+        <v>191</v>
       </c>
       <c r="G7" t="s">
         <v>24</v>
@@ -54006,27 +54016,27 @@
         <v>-87</v>
       </c>
       <c r="J7" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="B8">
         <v>2000</v>
       </c>
       <c r="C8" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D8" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="E8" t="s">
-        <v>174</v>
+        <v>192</v>
       </c>
       <c r="F8" t="s">
-        <v>181</v>
+        <v>191</v>
       </c>
       <c r="G8" t="s">
         <v>24</v>
@@ -54039,27 +54049,27 @@
         <v>78.2</v>
       </c>
       <c r="J8" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="9" spans="1:10">
       <c r="A9" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="B9">
         <v>2000</v>
       </c>
       <c r="C9" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D9" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="E9" t="s">
-        <v>174</v>
+        <v>192</v>
       </c>
       <c r="F9" t="s">
-        <v>181</v>
+        <v>191</v>
       </c>
       <c r="G9" t="s">
         <v>25</v>
@@ -54072,27 +54082,27 @@
         <v>-17.8</v>
       </c>
       <c r="J9" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="10" spans="1:10">
       <c r="A10" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="B10">
         <v>2000</v>
       </c>
       <c r="C10" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D10" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="E10" t="s">
-        <v>174</v>
+        <v>192</v>
       </c>
       <c r="F10" t="s">
-        <v>181</v>
+        <v>191</v>
       </c>
       <c r="G10" t="s">
         <v>25</v>
@@ -54105,27 +54115,27 @@
         <v>12.6</v>
       </c>
       <c r="J10" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="B11">
         <v>2000</v>
       </c>
       <c r="C11" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D11" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="E11" t="s">
-        <v>174</v>
+        <v>192</v>
       </c>
       <c r="F11" t="s">
-        <v>181</v>
+        <v>191</v>
       </c>
       <c r="G11" t="s">
         <v>16</v>
@@ -54138,27 +54148,27 @@
         <v>-28.1</v>
       </c>
       <c r="J11" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="12" spans="1:10">
       <c r="A12" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="B12">
         <v>2000</v>
       </c>
       <c r="C12" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D12" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="E12" t="s">
-        <v>174</v>
+        <v>192</v>
       </c>
       <c r="F12" t="s">
-        <v>181</v>
+        <v>191</v>
       </c>
       <c r="G12" t="s">
         <v>16</v>
@@ -54176,22 +54186,22 @@
     </row>
     <row r="13" spans="1:10">
       <c r="A13" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="B13">
         <v>2000</v>
       </c>
       <c r="C13" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D13" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="E13" t="s">
-        <v>174</v>
+        <v>192</v>
       </c>
       <c r="F13" t="s">
-        <v>181</v>
+        <v>191</v>
       </c>
       <c r="G13" t="s">
         <v>15</v>
@@ -54204,27 +54214,27 @@
         <v>-19.399999999999999</v>
       </c>
       <c r="J13" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="14" spans="1:10">
       <c r="A14" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="B14">
         <v>2000</v>
       </c>
       <c r="C14" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D14" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="E14" t="s">
-        <v>174</v>
+        <v>192</v>
       </c>
       <c r="F14" t="s">
-        <v>181</v>
+        <v>191</v>
       </c>
       <c r="G14" t="s">
         <v>15</v>
@@ -54237,27 +54247,27 @@
         <v>-0.5</v>
       </c>
       <c r="J14" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="15" spans="1:10">
       <c r="A15" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="B15">
         <v>2000</v>
       </c>
       <c r="C15" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D15" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="E15" t="s">
-        <v>174</v>
+        <v>192</v>
       </c>
       <c r="F15" t="s">
-        <v>181</v>
+        <v>191</v>
       </c>
       <c r="G15" t="s">
         <v>15</v>
@@ -54275,22 +54285,22 @@
     </row>
     <row r="16" spans="1:10">
       <c r="A16" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="B16">
         <v>2000</v>
       </c>
       <c r="C16" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D16" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="E16" t="s">
-        <v>174</v>
+        <v>192</v>
       </c>
       <c r="F16" t="s">
-        <v>181</v>
+        <v>191</v>
       </c>
       <c r="G16" t="s">
         <v>0</v>
@@ -54303,27 +54313,27 @@
         <v>-12.1</v>
       </c>
       <c r="J16" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="17" spans="1:10">
       <c r="A17" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="B17">
         <v>2000</v>
       </c>
       <c r="C17" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D17" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="E17" t="s">
-        <v>174</v>
+        <v>192</v>
       </c>
       <c r="F17" t="s">
-        <v>181</v>
+        <v>191</v>
       </c>
       <c r="G17" t="s">
         <v>0</v>
@@ -54336,27 +54346,27 @@
         <v>-32.299999999999997</v>
       </c>
       <c r="J17" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="18" spans="1:10">
       <c r="A18" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="B18">
         <v>2000</v>
       </c>
       <c r="C18" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D18" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="E18" t="s">
-        <v>174</v>
+        <v>192</v>
       </c>
       <c r="F18" t="s">
-        <v>181</v>
+        <v>191</v>
       </c>
       <c r="G18" t="s">
         <v>0</v>
@@ -54369,30 +54379,30 @@
         <v>25.2</v>
       </c>
       <c r="J18" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="19" spans="1:10">
       <c r="A19" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="B19">
         <v>2000</v>
       </c>
       <c r="C19" t="s">
+        <v>178</v>
+      </c>
+      <c r="D19" t="s">
         <v>180</v>
       </c>
-      <c r="D19" t="s">
-        <v>183</v>
-      </c>
       <c r="E19" t="s">
-        <v>174</v>
+        <v>192</v>
       </c>
       <c r="F19" t="s">
-        <v>181</v>
+        <v>191</v>
       </c>
       <c r="G19" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="H19" t="s">
         <v>18</v>
@@ -54407,25 +54417,25 @@
     </row>
     <row r="20" spans="1:10">
       <c r="A20" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="B20">
         <v>2000</v>
       </c>
       <c r="C20" t="s">
+        <v>178</v>
+      </c>
+      <c r="D20" t="s">
         <v>180</v>
       </c>
-      <c r="D20" t="s">
-        <v>183</v>
-      </c>
       <c r="E20" t="s">
-        <v>174</v>
+        <v>192</v>
       </c>
       <c r="F20" t="s">
-        <v>181</v>
+        <v>191</v>
       </c>
       <c r="G20" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="H20" t="s">
         <v>17</v>
@@ -54440,25 +54450,25 @@
     </row>
     <row r="21" spans="1:10">
       <c r="A21" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="B21">
         <v>2000</v>
       </c>
       <c r="C21" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D21" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="E21" t="s">
-        <v>174</v>
+        <v>192</v>
       </c>
       <c r="F21" t="s">
-        <v>181</v>
+        <v>191</v>
       </c>
       <c r="G21" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="H21" t="s">
         <v>19</v>
@@ -54468,7 +54478,7 @@
         <v>25.2</v>
       </c>
       <c r="J21" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated perfect sub .xlsx file.
</commit_message>
<xml_diff>
--- a/inst/extdata/PerfectSubstitutionraw/UTEI_Sankey_Simple_ECC_Perfect_Sub.xlsx
+++ b/inst/extdata/PerfectSubstitutionraw/UTEI_Sankey_Simple_ECC_Perfect_Sub.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matt/github/Recca/inst/extdata/PerfectSubstitutionraw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61524CCD-45FA-FF45-A47A-92231EF698CF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F0DA20C-DB24-914E-988F-511420BD33C2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20680" yWindow="460" windowWidth="26200" windowHeight="17560" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -53781,7 +53781,7 @@
   <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>

</xml_diff>